<commit_message>
auto commit @19.12.2020: 19:59:00,49
</commit_message>
<xml_diff>
--- a/Bachelorarbeit/Weckermann_ICS_and_Test Documentation.xlsx
+++ b/Bachelorarbeit/Weckermann_ICS_and_Test Documentation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Benutzer\Henry\Downloads\Abschlussarbeit_H-BRS\Bachelorarbeit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFBECBC7-D8D2-4D38-9562-250664CFFB3B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9587686D-3D9C-4262-BF11-FED81276D286}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1451" uniqueCount="655">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1451" uniqueCount="658">
   <si>
     <t>Im Rahmen von [BSI TR-03148 -P] muss ein Implementation Conformance Statement ausgefüllt werden. Im folgenden finden Sie eine Vorlage für das ICS. Das Originaldokument ist auf Englisch, weswegen hier die englischen Formulierungen übernommen wurden, da keine offizielle Übersetzung des Dokuments existiert. Die Eintragungen können aber auf deutsch oder englisch gemacht werden. Die hier eingetragenen Beispieldaten sind durch Echtdaten zu ersetzen. Alternativ oder ergänzend zu dem ICS in dieser Tabelle kann auch das ICS aus [BSI TR-03148-P] als Vorlage genutzt werden.</t>
   </si>
@@ -1450,11 +1450,6 @@
   </si>
   <si>
     <t>TR.E.5</t>
-  </si>
-  <si>
-    <t>https://openwrt.org/docs/guide-user/security/release_signatures
-https://openwrt.org/docs/guide-user/security/signatures
-Signatures are used, but they can easily be ignored or silenced.</t>
   </si>
   <si>
     <t>TP_E_5_1_signature_and_metadata_of_images.PNG</t>
@@ -4557,6 +4552,26 @@
   </si>
   <si>
     <t>Only one WAN Interface is available</t>
+  </si>
+  <si>
+    <t>Even if the router does not support configuration over the WAN interface it would be possible to change the port. The best way to support configuration over the WAN interface would be to use a VPN. In this case it is possible to change the port.</t>
+  </si>
+  <si>
+    <t>https://openwrt.org/docs/guide-user/security/release_signatures
+https://openwrt.org/docs/guide-user/security/signatures
+Signatures are used sometimes, but they can easily be ignored or silenced.
+The tester could not find firmware images that are signed with a valid signature</t>
+  </si>
+  <si>
+    <t>https://openwrt.org/docs/guide-user/security/release_signatures
+https://openwrt.org/docs/guide-user/security/signatures
+Signatures are used sometimes, but they can easily be ignored or silenced.
+The tester could not find firmware images that are signed with a valid signature.
+Instead the developers of OpenWrt chose to use signed sha2 hashes. The signed hashes aswell as the signature is available in each download directory on the download server. 
+After downloading the sha256sums and sha256sum.asc file the signature can be validated via "gpg --with-fingerprint --verify sha256sum.asc sha256sum". After that the firmware image's hash is validated via "sha256sum -c --ignore-missing sha256sums"</t>
+  </si>
+  <si>
+    <t>When the firmware metadata, which is used by the device to verify a firmware image, is tempered with the devices displays a message to warn the user. This also applies when the user tries to install a wrong firmware. Other than this no warning message is shown because there are no other mechanisms to validate the image.</t>
   </si>
 </sst>
 </file>
@@ -5471,7 +5486,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="260">
+  <cellXfs count="259">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -5995,12 +6010,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="7" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -6104,6 +6113,9 @@
     </xf>
     <xf numFmtId="0" fontId="22" fillId="7" borderId="11" xfId="3" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -6642,31 +6654,31 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="218" t="s">
+      <c r="A2" s="217" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="218"/>
-      <c r="C2" s="218"/>
-      <c r="D2" s="218"/>
-      <c r="E2" s="218"/>
-      <c r="F2" s="218"/>
-      <c r="G2" s="218"/>
-      <c r="H2" s="218"/>
-      <c r="I2" s="218"/>
-      <c r="J2" s="218"/>
-      <c r="K2" s="218"/>
+      <c r="B2" s="217"/>
+      <c r="C2" s="217"/>
+      <c r="D2" s="217"/>
+      <c r="E2" s="217"/>
+      <c r="F2" s="217"/>
+      <c r="G2" s="217"/>
+      <c r="H2" s="217"/>
+      <c r="I2" s="217"/>
+      <c r="J2" s="217"/>
+      <c r="K2" s="217"/>
     </row>
     <row r="4" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="215" t="s">
+      <c r="A5" s="213" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="219" t="s">
+      <c r="A6" s="218" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="219"/>
+      <c r="B6" s="218"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
@@ -6681,244 +6693,244 @@
       <c r="A7" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="220" t="s">
+      <c r="B7" s="219" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="220"/>
+      <c r="C7" s="219"/>
       <c r="D7" s="7"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="221" t="s">
+      <c r="B8" s="220" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="221"/>
+      <c r="C8" s="220"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="221" t="s">
+      <c r="B9" s="220" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="221"/>
+      <c r="C9" s="220"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="222" t="s">
+      <c r="B10" s="221" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="222"/>
+      <c r="C10" s="221"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
     </row>
     <row r="13" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A13" s="216" t="s">
+      <c r="A13" s="214" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="64.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="223" t="s">
+      <c r="A14" s="222" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="224"/>
+      <c r="B14" s="223"/>
     </row>
     <row r="15" spans="1:11" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="227" t="s">
+      <c r="B15" s="226" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="228"/>
-      <c r="D15" s="228"/>
-      <c r="E15" s="228"/>
-      <c r="F15" s="228"/>
-      <c r="G15" s="228"/>
-      <c r="H15" s="229"/>
+      <c r="C15" s="227"/>
+      <c r="D15" s="227"/>
+      <c r="E15" s="227"/>
+      <c r="F15" s="227"/>
+      <c r="G15" s="227"/>
+      <c r="H15" s="228"/>
     </row>
     <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="225" t="s">
+      <c r="B16" s="224" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="230"/>
-      <c r="D16" s="230"/>
-      <c r="E16" s="230"/>
-      <c r="F16" s="230"/>
-      <c r="G16" s="230"/>
-      <c r="H16" s="231"/>
+      <c r="C16" s="229"/>
+      <c r="D16" s="229"/>
+      <c r="E16" s="229"/>
+      <c r="F16" s="229"/>
+      <c r="G16" s="229"/>
+      <c r="H16" s="230"/>
     </row>
     <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="225" t="s">
+      <c r="B17" s="224" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="225"/>
-      <c r="D17" s="225"/>
-      <c r="E17" s="225"/>
-      <c r="F17" s="225"/>
-      <c r="G17" s="225"/>
-      <c r="H17" s="226"/>
+      <c r="C17" s="224"/>
+      <c r="D17" s="224"/>
+      <c r="E17" s="224"/>
+      <c r="F17" s="224"/>
+      <c r="G17" s="224"/>
+      <c r="H17" s="225"/>
     </row>
     <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="225" t="s">
+      <c r="B18" s="224" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="225"/>
-      <c r="D18" s="225"/>
-      <c r="E18" s="225"/>
-      <c r="F18" s="225"/>
-      <c r="G18" s="225"/>
-      <c r="H18" s="226"/>
+      <c r="C18" s="224"/>
+      <c r="D18" s="224"/>
+      <c r="E18" s="224"/>
+      <c r="F18" s="224"/>
+      <c r="G18" s="224"/>
+      <c r="H18" s="225"/>
     </row>
     <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="225" t="s">
+      <c r="B19" s="224" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="230"/>
-      <c r="D19" s="230"/>
-      <c r="E19" s="230"/>
-      <c r="F19" s="230"/>
-      <c r="G19" s="230"/>
-      <c r="H19" s="231"/>
+      <c r="C19" s="229"/>
+      <c r="D19" s="229"/>
+      <c r="E19" s="229"/>
+      <c r="F19" s="229"/>
+      <c r="G19" s="229"/>
+      <c r="H19" s="230"/>
     </row>
     <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="233" t="s">
+      <c r="B20" s="232" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="234"/>
-      <c r="D20" s="234"/>
-      <c r="E20" s="234"/>
-      <c r="F20" s="234"/>
-      <c r="G20" s="234"/>
-      <c r="H20" s="235"/>
+      <c r="C20" s="233"/>
+      <c r="D20" s="233"/>
+      <c r="E20" s="233"/>
+      <c r="F20" s="233"/>
+      <c r="G20" s="233"/>
+      <c r="H20" s="234"/>
     </row>
     <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="225"/>
-      <c r="C21" s="230"/>
-      <c r="D21" s="230"/>
-      <c r="E21" s="230"/>
-      <c r="F21" s="230"/>
-      <c r="G21" s="230"/>
-      <c r="H21" s="231"/>
+      <c r="B21" s="224"/>
+      <c r="C21" s="229"/>
+      <c r="D21" s="229"/>
+      <c r="E21" s="229"/>
+      <c r="F21" s="229"/>
+      <c r="G21" s="229"/>
+      <c r="H21" s="230"/>
     </row>
     <row r="24" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A24" s="215" t="s">
+      <c r="A24" s="213" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="232" t="s">
+      <c r="A25" s="231" t="s">
         <v>26</v>
       </c>
-      <c r="B25" s="232"/>
+      <c r="B25" s="231"/>
     </row>
     <row r="26" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B26" s="236" t="s">
+      <c r="B26" s="235" t="s">
         <v>14</v>
       </c>
-      <c r="C26" s="236"/>
-      <c r="D26" s="236"/>
+      <c r="C26" s="235"/>
+      <c r="D26" s="235"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="226" t="s">
+      <c r="B27" s="225" t="s">
         <v>28</v>
       </c>
-      <c r="C27" s="226"/>
-      <c r="D27" s="226"/>
+      <c r="C27" s="225"/>
+      <c r="D27" s="225"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="B28" s="226" t="s">
+      <c r="B28" s="225" t="s">
         <v>30</v>
       </c>
-      <c r="C28" s="226"/>
-      <c r="D28" s="226"/>
+      <c r="C28" s="225"/>
+      <c r="D28" s="225"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B29" s="226" t="s">
+      <c r="B29" s="225" t="s">
         <v>32</v>
       </c>
-      <c r="C29" s="226"/>
-      <c r="D29" s="226"/>
+      <c r="C29" s="225"/>
+      <c r="D29" s="225"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="B30" s="226" t="s">
+      <c r="B30" s="225" t="s">
         <v>34</v>
       </c>
-      <c r="C30" s="226"/>
-      <c r="D30" s="226"/>
+      <c r="C30" s="225"/>
+      <c r="D30" s="225"/>
     </row>
     <row r="31" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B31" s="226" t="s">
+      <c r="B31" s="225" t="s">
         <v>36</v>
       </c>
-      <c r="C31" s="226"/>
-      <c r="D31" s="226"/>
+      <c r="C31" s="225"/>
+      <c r="D31" s="225"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="15"/>
-      <c r="B32" s="201"/>
-      <c r="C32" s="201"/>
-      <c r="D32" s="201"/>
+      <c r="B32" s="199"/>
+      <c r="C32" s="199"/>
+      <c r="D32" s="199"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="15"/>
       <c r="B33" s="15"/>
     </row>
     <row r="34" spans="1:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="A34" s="215" t="s">
+      <c r="A34" s="213" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="218" t="s">
+      <c r="A35" s="217" t="s">
         <v>37</v>
       </c>
-      <c r="B35" s="218"/>
-      <c r="C35" s="218"/>
-      <c r="D35" s="218"/>
-      <c r="E35" s="218"/>
+      <c r="B35" s="217"/>
+      <c r="C35" s="217"/>
+      <c r="D35" s="217"/>
+      <c r="E35" s="217"/>
     </row>
     <row r="37" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="38" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6937,14 +6949,14 @@
       <c r="E38" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="F38" s="252" t="s">
-        <v>624</v>
-      </c>
-      <c r="G38" s="253"/>
-      <c r="H38" s="253"/>
-      <c r="I38" s="253"/>
-      <c r="J38" s="253"/>
-      <c r="K38" s="254"/>
+      <c r="F38" s="251" t="s">
+        <v>623</v>
+      </c>
+      <c r="G38" s="252"/>
+      <c r="H38" s="252"/>
+      <c r="I38" s="252"/>
+      <c r="J38" s="252"/>
+      <c r="K38" s="253"/>
     </row>
     <row r="39" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="14" t="s">
@@ -6962,14 +6974,14 @@
       <c r="E39" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="F39" s="225" t="s">
+      <c r="F39" s="224" t="s">
         <v>48</v>
       </c>
-      <c r="G39" s="230"/>
-      <c r="H39" s="230"/>
-      <c r="I39" s="230"/>
-      <c r="J39" s="230"/>
-      <c r="K39" s="231"/>
+      <c r="G39" s="229"/>
+      <c r="H39" s="229"/>
+      <c r="I39" s="229"/>
+      <c r="J39" s="229"/>
+      <c r="K39" s="230"/>
     </row>
     <row r="40" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="14" t="s">
@@ -6987,14 +6999,14 @@
       <c r="E40" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="F40" s="225" t="s">
+      <c r="F40" s="224" t="s">
         <v>50</v>
       </c>
-      <c r="G40" s="230"/>
-      <c r="H40" s="230"/>
-      <c r="I40" s="230"/>
-      <c r="J40" s="230"/>
-      <c r="K40" s="231"/>
+      <c r="G40" s="229"/>
+      <c r="H40" s="229"/>
+      <c r="I40" s="229"/>
+      <c r="J40" s="229"/>
+      <c r="K40" s="230"/>
     </row>
     <row r="41" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="14" t="s">
@@ -7012,12 +7024,12 @@
       <c r="E41" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="F41" s="225"/>
-      <c r="G41" s="230"/>
-      <c r="H41" s="230"/>
-      <c r="I41" s="230"/>
-      <c r="J41" s="230"/>
-      <c r="K41" s="231"/>
+      <c r="F41" s="224"/>
+      <c r="G41" s="229"/>
+      <c r="H41" s="229"/>
+      <c r="I41" s="229"/>
+      <c r="J41" s="229"/>
+      <c r="K41" s="230"/>
     </row>
     <row r="42" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="14" t="s">
@@ -7035,12 +7047,12 @@
       <c r="E42" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="F42" s="233"/>
-      <c r="G42" s="234"/>
-      <c r="H42" s="234"/>
-      <c r="I42" s="234"/>
-      <c r="J42" s="234"/>
-      <c r="K42" s="235"/>
+      <c r="F42" s="232"/>
+      <c r="G42" s="233"/>
+      <c r="H42" s="233"/>
+      <c r="I42" s="233"/>
+      <c r="J42" s="233"/>
+      <c r="K42" s="234"/>
     </row>
     <row r="43" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="14" t="s">
@@ -7058,12 +7070,12 @@
       <c r="E43" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="F43" s="225"/>
-      <c r="G43" s="230"/>
-      <c r="H43" s="230"/>
-      <c r="I43" s="230"/>
-      <c r="J43" s="230"/>
-      <c r="K43" s="231"/>
+      <c r="F43" s="224"/>
+      <c r="G43" s="229"/>
+      <c r="H43" s="229"/>
+      <c r="I43" s="229"/>
+      <c r="J43" s="229"/>
+      <c r="K43" s="230"/>
     </row>
     <row r="44" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="14" t="s">
@@ -7081,12 +7093,12 @@
       <c r="E44" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="F44" s="225"/>
-      <c r="G44" s="230"/>
-      <c r="H44" s="230"/>
-      <c r="I44" s="230"/>
-      <c r="J44" s="230"/>
-      <c r="K44" s="231"/>
+      <c r="F44" s="224"/>
+      <c r="G44" s="229"/>
+      <c r="H44" s="229"/>
+      <c r="I44" s="229"/>
+      <c r="J44" s="229"/>
+      <c r="K44" s="230"/>
     </row>
     <row r="45" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="14" t="s">
@@ -7104,14 +7116,14 @@
       <c r="E45" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="F45" s="225" t="s">
+      <c r="F45" s="224" t="s">
         <v>56</v>
       </c>
-      <c r="G45" s="230"/>
-      <c r="H45" s="230"/>
-      <c r="I45" s="230"/>
-      <c r="J45" s="230"/>
-      <c r="K45" s="231"/>
+      <c r="G45" s="229"/>
+      <c r="H45" s="229"/>
+      <c r="I45" s="229"/>
+      <c r="J45" s="229"/>
+      <c r="K45" s="230"/>
     </row>
     <row r="46" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="14" t="s">
@@ -7129,12 +7141,12 @@
       <c r="E46" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="F46" s="225"/>
-      <c r="G46" s="230"/>
-      <c r="H46" s="230"/>
-      <c r="I46" s="230"/>
-      <c r="J46" s="230"/>
-      <c r="K46" s="231"/>
+      <c r="F46" s="224"/>
+      <c r="G46" s="229"/>
+      <c r="H46" s="229"/>
+      <c r="I46" s="229"/>
+      <c r="J46" s="229"/>
+      <c r="K46" s="230"/>
     </row>
     <row r="47" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="14" t="s">
@@ -7152,12 +7164,12 @@
       <c r="E47" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="F47" s="225"/>
-      <c r="G47" s="230"/>
-      <c r="H47" s="230"/>
-      <c r="I47" s="230"/>
-      <c r="J47" s="230"/>
-      <c r="K47" s="231"/>
+      <c r="F47" s="224"/>
+      <c r="G47" s="229"/>
+      <c r="H47" s="229"/>
+      <c r="I47" s="229"/>
+      <c r="J47" s="229"/>
+      <c r="K47" s="230"/>
     </row>
     <row r="48" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="14" t="s">
@@ -7175,12 +7187,12 @@
       <c r="E48" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="F48" s="233"/>
-      <c r="G48" s="234"/>
-      <c r="H48" s="234"/>
-      <c r="I48" s="234"/>
-      <c r="J48" s="234"/>
-      <c r="K48" s="235"/>
+      <c r="F48" s="232"/>
+      <c r="G48" s="233"/>
+      <c r="H48" s="233"/>
+      <c r="I48" s="233"/>
+      <c r="J48" s="233"/>
+      <c r="K48" s="234"/>
     </row>
     <row r="49" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="14" t="s">
@@ -7198,12 +7210,12 @@
       <c r="E49" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="F49" s="225"/>
-      <c r="G49" s="230"/>
-      <c r="H49" s="230"/>
-      <c r="I49" s="230"/>
-      <c r="J49" s="230"/>
-      <c r="K49" s="231"/>
+      <c r="F49" s="224"/>
+      <c r="G49" s="229"/>
+      <c r="H49" s="229"/>
+      <c r="I49" s="229"/>
+      <c r="J49" s="229"/>
+      <c r="K49" s="230"/>
     </row>
     <row r="50" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="14" t="s">
@@ -7221,12 +7233,12 @@
       <c r="E50" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="F50" s="225"/>
-      <c r="G50" s="230"/>
-      <c r="H50" s="230"/>
-      <c r="I50" s="230"/>
-      <c r="J50" s="230"/>
-      <c r="K50" s="231"/>
+      <c r="F50" s="224"/>
+      <c r="G50" s="229"/>
+      <c r="H50" s="229"/>
+      <c r="I50" s="229"/>
+      <c r="J50" s="229"/>
+      <c r="K50" s="230"/>
     </row>
     <row r="51" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="14" t="s">
@@ -7244,14 +7256,14 @@
       <c r="E51" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="F51" s="225" t="s">
+      <c r="F51" s="224" t="s">
         <v>60</v>
       </c>
-      <c r="G51" s="230"/>
-      <c r="H51" s="230"/>
-      <c r="I51" s="230"/>
-      <c r="J51" s="230"/>
-      <c r="K51" s="231"/>
+      <c r="G51" s="229"/>
+      <c r="H51" s="229"/>
+      <c r="I51" s="229"/>
+      <c r="J51" s="229"/>
+      <c r="K51" s="230"/>
     </row>
     <row r="52" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="14" t="s">
@@ -7269,12 +7281,12 @@
       <c r="E52" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="F52" s="225"/>
-      <c r="G52" s="230"/>
-      <c r="H52" s="230"/>
-      <c r="I52" s="230"/>
-      <c r="J52" s="230"/>
-      <c r="K52" s="231"/>
+      <c r="F52" s="224"/>
+      <c r="G52" s="229"/>
+      <c r="H52" s="229"/>
+      <c r="I52" s="229"/>
+      <c r="J52" s="229"/>
+      <c r="K52" s="230"/>
     </row>
     <row r="53" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="14" t="s">
@@ -7292,12 +7304,12 @@
       <c r="E53" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="F53" s="225"/>
-      <c r="G53" s="230"/>
-      <c r="H53" s="230"/>
-      <c r="I53" s="230"/>
-      <c r="J53" s="230"/>
-      <c r="K53" s="231"/>
+      <c r="F53" s="224"/>
+      <c r="G53" s="229"/>
+      <c r="H53" s="229"/>
+      <c r="I53" s="229"/>
+      <c r="J53" s="229"/>
+      <c r="K53" s="230"/>
     </row>
     <row r="54" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="14" t="s">
@@ -7315,12 +7327,12 @@
       <c r="E54" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="F54" s="225"/>
-      <c r="G54" s="230"/>
-      <c r="H54" s="230"/>
-      <c r="I54" s="230"/>
-      <c r="J54" s="230"/>
-      <c r="K54" s="231"/>
+      <c r="F54" s="224"/>
+      <c r="G54" s="229"/>
+      <c r="H54" s="229"/>
+      <c r="I54" s="229"/>
+      <c r="J54" s="229"/>
+      <c r="K54" s="230"/>
     </row>
     <row r="55" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="14" t="s">
@@ -7338,12 +7350,12 @@
       <c r="E55" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="F55" s="225"/>
-      <c r="G55" s="230"/>
-      <c r="H55" s="230"/>
-      <c r="I55" s="230"/>
-      <c r="J55" s="230"/>
-      <c r="K55" s="231"/>
+      <c r="F55" s="224"/>
+      <c r="G55" s="229"/>
+      <c r="H55" s="229"/>
+      <c r="I55" s="229"/>
+      <c r="J55" s="229"/>
+      <c r="K55" s="230"/>
     </row>
     <row r="56" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="14" t="s">
@@ -7361,21 +7373,21 @@
       <c r="E56" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="F56" s="225"/>
-      <c r="G56" s="230"/>
-      <c r="H56" s="230"/>
-      <c r="I56" s="230"/>
-      <c r="J56" s="230"/>
-      <c r="K56" s="231"/>
+      <c r="F56" s="224"/>
+      <c r="G56" s="229"/>
+      <c r="H56" s="229"/>
+      <c r="I56" s="229"/>
+      <c r="J56" s="229"/>
+      <c r="K56" s="230"/>
     </row>
     <row r="59" spans="1:11" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="218" t="s">
+      <c r="A59" s="217" t="s">
         <v>61</v>
       </c>
-      <c r="B59" s="218"/>
-      <c r="C59" s="218"/>
-      <c r="D59" s="218"/>
-      <c r="E59" s="218"/>
+      <c r="B59" s="217"/>
+      <c r="C59" s="217"/>
+      <c r="D59" s="217"/>
+      <c r="E59" s="217"/>
     </row>
     <row r="60" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="61" spans="1:11" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -7486,13 +7498,13 @@
       </c>
     </row>
     <row r="70" spans="1:5" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="218" t="s">
+      <c r="A70" s="217" t="s">
         <v>67</v>
       </c>
-      <c r="B70" s="218"/>
-      <c r="C70" s="218"/>
-      <c r="D70" s="218"/>
-      <c r="E70" s="218"/>
+      <c r="B70" s="217"/>
+      <c r="C70" s="217"/>
+      <c r="D70" s="217"/>
+      <c r="E70" s="217"/>
     </row>
     <row r="71" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="25"/>
@@ -7501,29 +7513,29 @@
       <c r="A72" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="B72" s="202" t="s">
+      <c r="B72" s="200" t="s">
         <v>69</v>
       </c>
-      <c r="C72" s="196" t="s">
+      <c r="C72" s="194" t="s">
         <v>70</v>
       </c>
-      <c r="D72" s="197"/>
+      <c r="D72" s="195"/>
     </row>
     <row r="73" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="203"/>
-      <c r="B73" s="204"/>
-      <c r="C73" s="199" t="s">
+      <c r="A73" s="201"/>
+      <c r="B73" s="202"/>
+      <c r="C73" s="197" t="s">
         <v>71</v>
       </c>
-      <c r="D73" s="200"/>
+      <c r="D73" s="198"/>
     </row>
     <row r="75" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="218" t="s">
+      <c r="A75" s="217" t="s">
         <v>72</v>
       </c>
-      <c r="B75" s="218"/>
-      <c r="C75" s="218"/>
-      <c r="D75" s="218"/>
+      <c r="B75" s="217"/>
+      <c r="C75" s="217"/>
+      <c r="D75" s="217"/>
       <c r="E75" s="26"/>
     </row>
     <row r="76" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -7531,17 +7543,17 @@
       <c r="A77" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="B77" s="181" t="s">
+      <c r="B77" s="179" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="218" t="s">
+      <c r="A80" s="217" t="s">
         <v>74</v>
       </c>
-      <c r="B80" s="218"/>
-      <c r="C80" s="218"/>
-      <c r="D80" s="218"/>
+      <c r="B80" s="217"/>
+      <c r="C80" s="217"/>
+      <c r="D80" s="217"/>
     </row>
     <row r="82" spans="1:5" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="27" t="s">
@@ -7561,8 +7573,8 @@
       <c r="B83" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="C83" s="206" t="s">
-        <v>625</v>
+      <c r="C83" s="204" t="s">
+        <v>624</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7572,62 +7584,62 @@
       <c r="B84" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="C84" s="206" t="s">
-        <v>625</v>
+      <c r="C84" s="204" t="s">
+        <v>624</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A85" s="208" t="s">
+      <c r="A85" s="206" t="s">
         <v>66</v>
       </c>
-      <c r="B85" s="208" t="s">
+      <c r="B85" s="206" t="s">
         <v>81</v>
       </c>
-      <c r="C85" s="208" t="s">
+      <c r="C85" s="206" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A86" s="208" t="s">
+      <c r="A86" s="206" t="s">
         <v>66</v>
       </c>
-      <c r="B86" s="208" t="s">
+      <c r="B86" s="206" t="s">
         <v>81</v>
       </c>
-      <c r="C86" s="208" t="s">
+      <c r="C86" s="206" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A87" s="208" t="s">
+      <c r="A87" s="206" t="s">
         <v>66</v>
       </c>
-      <c r="B87" s="208" t="s">
+      <c r="B87" s="206" t="s">
         <v>81</v>
       </c>
-      <c r="C87" s="208" t="s">
+      <c r="C87" s="206" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A88" s="208" t="s">
+      <c r="A88" s="206" t="s">
         <v>66</v>
       </c>
-      <c r="B88" s="208" t="s">
+      <c r="B88" s="206" t="s">
         <v>81</v>
       </c>
-      <c r="C88" s="208" t="s">
+      <c r="C88" s="206" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="237" t="s">
-        <v>539</v>
-      </c>
-      <c r="B91" s="237"/>
-      <c r="C91" s="237"/>
-      <c r="D91" s="237"/>
-      <c r="E91" s="237"/>
+      <c r="A91" s="236" t="s">
+        <v>538</v>
+      </c>
+      <c r="B91" s="236"/>
+      <c r="C91" s="236"/>
+      <c r="D91" s="236"/>
+      <c r="E91" s="236"/>
     </row>
     <row r="93" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="19" t="s">
@@ -7668,92 +7680,92 @@
         <v>86</v>
       </c>
       <c r="D95" s="29" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A96" s="208" t="s">
+      <c r="A96" s="206" t="s">
         <v>66</v>
       </c>
-      <c r="B96" s="208" t="s">
+      <c r="B96" s="206" t="s">
         <v>66</v>
       </c>
-      <c r="C96" s="208" t="s">
+      <c r="C96" s="206" t="s">
         <v>66</v>
       </c>
-      <c r="D96" s="208" t="s">
+      <c r="D96" s="206" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="208" t="s">
+      <c r="A97" s="206" t="s">
         <v>66</v>
       </c>
-      <c r="B97" s="208" t="s">
+      <c r="B97" s="206" t="s">
         <v>66</v>
       </c>
-      <c r="C97" s="208" t="s">
+      <c r="C97" s="206" t="s">
         <v>66</v>
       </c>
-      <c r="D97" s="208" t="s">
+      <c r="D97" s="206" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="208" t="s">
+      <c r="A98" s="206" t="s">
         <v>66</v>
       </c>
-      <c r="B98" s="208" t="s">
+      <c r="B98" s="206" t="s">
         <v>66</v>
       </c>
-      <c r="C98" s="208" t="s">
+      <c r="C98" s="206" t="s">
         <v>66</v>
       </c>
-      <c r="D98" s="208" t="s">
+      <c r="D98" s="206" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="208" t="s">
+      <c r="A99" s="206" t="s">
         <v>66</v>
       </c>
-      <c r="B99" s="208" t="s">
+      <c r="B99" s="206" t="s">
         <v>66</v>
       </c>
-      <c r="C99" s="208" t="s">
+      <c r="C99" s="206" t="s">
         <v>66</v>
       </c>
-      <c r="D99" s="208" t="s">
+      <c r="D99" s="206" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="102" spans="1:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="238" t="s">
+      <c r="A102" s="237" t="s">
         <v>89</v>
       </c>
-      <c r="B102" s="238"/>
+      <c r="B102" s="237"/>
     </row>
     <row r="103" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="104" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="B104" s="207" t="s">
+      <c r="B104" s="205" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="107" spans="1:4" ht="21" x14ac:dyDescent="0.35">
-      <c r="A107" s="215" t="s">
+      <c r="A107" s="213" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="108" spans="1:4" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="237" t="s">
-        <v>540</v>
-      </c>
-      <c r="B108" s="237"/>
-      <c r="C108" s="237"/>
-      <c r="D108" s="237"/>
+      <c r="A108" s="236" t="s">
+        <v>539</v>
+      </c>
+      <c r="B108" s="236"/>
+      <c r="C108" s="236"/>
+      <c r="D108" s="236"/>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
@@ -7798,7 +7810,7 @@
       <c r="C112" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="D112" s="209" t="s">
+      <c r="D112" s="207" t="s">
         <v>66</v>
       </c>
     </row>
@@ -7812,7 +7824,7 @@
       <c r="C113" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="D113" s="209" t="s">
+      <c r="D113" s="207" t="s">
         <v>66</v>
       </c>
     </row>
@@ -7826,7 +7838,7 @@
       <c r="C114" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="D114" s="209" t="s">
+      <c r="D114" s="207" t="s">
         <v>66</v>
       </c>
     </row>
@@ -7840,7 +7852,7 @@
       <c r="C115" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="D115" s="209" t="s">
+      <c r="D115" s="207" t="s">
         <v>66</v>
       </c>
     </row>
@@ -7854,7 +7866,7 @@
       <c r="C116" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="D116" s="209" t="s">
+      <c r="D116" s="207" t="s">
         <v>66</v>
       </c>
     </row>
@@ -7863,12 +7875,12 @@
       <c r="B117" s="31"/>
     </row>
     <row r="120" spans="1:4" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="239" t="s">
+      <c r="A120" s="238" t="s">
         <v>97</v>
       </c>
-      <c r="B120" s="239"/>
-      <c r="C120" s="239"/>
-      <c r="D120" s="239"/>
+      <c r="B120" s="238"/>
+      <c r="C120" s="238"/>
+      <c r="D120" s="238"/>
     </row>
     <row r="121" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A121" s="9" t="s">
@@ -7894,7 +7906,7 @@
       <c r="C122" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="D122" s="209" t="s">
+      <c r="D122" s="207" t="s">
         <v>66</v>
       </c>
     </row>
@@ -7969,9 +7981,9 @@
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A128" s="240"/>
-      <c r="B128" s="240"/>
-      <c r="C128" s="240"/>
+      <c r="A128" s="239"/>
+      <c r="B128" s="239"/>
+      <c r="C128" s="239"/>
     </row>
     <row r="130" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A130" s="32" t="s">
@@ -7979,12 +7991,12 @@
       </c>
     </row>
     <row r="131" spans="1:4" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="241" t="s">
+      <c r="A131" s="240" t="s">
         <v>99</v>
       </c>
-      <c r="B131" s="241"/>
-      <c r="C131" s="241"/>
-      <c r="D131" s="241"/>
+      <c r="B131" s="240"/>
+      <c r="C131" s="240"/>
+      <c r="D131" s="240"/>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="9" t="s">
@@ -8002,7 +8014,7 @@
         <v>103</v>
       </c>
       <c r="B133" s="20" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="C133" s="21" t="s">
         <v>104</v>
@@ -8024,7 +8036,7 @@
         <v>108</v>
       </c>
       <c r="B135" s="20" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="C135" s="21" t="s">
         <v>109</v>
@@ -8035,7 +8047,7 @@
         <v>110</v>
       </c>
       <c r="B136" s="20" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="C136" s="21" t="s">
         <v>111</v>
@@ -8046,10 +8058,10 @@
         <v>112</v>
       </c>
       <c r="B137" s="20" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="C137" s="21" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="138" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8057,21 +8069,21 @@
         <v>113</v>
       </c>
       <c r="B138" s="20" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="C138" s="21" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="139" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A139" s="30" t="s">
+        <v>645</v>
+      </c>
+      <c r="B139" s="20" t="s">
+        <v>626</v>
+      </c>
+      <c r="C139" s="30" t="s">
         <v>646</v>
-      </c>
-      <c r="B139" s="20" t="s">
-        <v>627</v>
-      </c>
-      <c r="C139" s="30" t="s">
-        <v>647</v>
       </c>
     </row>
     <row r="141" spans="1:4" ht="21" x14ac:dyDescent="0.25">
@@ -8080,12 +8092,12 @@
       </c>
     </row>
     <row r="142" spans="1:4" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A142" s="241" t="s">
+      <c r="A142" s="240" t="s">
         <v>114</v>
       </c>
-      <c r="B142" s="241"/>
-      <c r="C142" s="241"/>
-      <c r="D142" s="241"/>
+      <c r="B142" s="240"/>
+      <c r="C142" s="240"/>
+      <c r="D142" s="240"/>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" s="9" t="s">
@@ -8121,18 +8133,18 @@
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A146" s="242" t="s">
+      <c r="A146" s="241" t="s">
         <v>122</v>
       </c>
-      <c r="B146" s="242"/>
+      <c r="B146" s="241"/>
     </row>
     <row r="148" spans="1:4" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="241" t="s">
+      <c r="A148" s="240" t="s">
         <v>123</v>
       </c>
-      <c r="B148" s="241"/>
-      <c r="C148" s="241"/>
-      <c r="D148" s="241"/>
+      <c r="B148" s="240"/>
+      <c r="C148" s="240"/>
+      <c r="D148" s="240"/>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" s="9" t="s">
@@ -8163,12 +8175,12 @@
       <c r="B153" s="24"/>
     </row>
     <row r="155" spans="1:4" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A155" s="239" t="s">
+      <c r="A155" s="238" t="s">
         <v>125</v>
       </c>
-      <c r="B155" s="239"/>
-      <c r="C155" s="239"/>
-      <c r="D155" s="239"/>
+      <c r="B155" s="238"/>
+      <c r="C155" s="238"/>
+      <c r="D155" s="238"/>
     </row>
     <row r="156" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A156" s="9" t="s">
@@ -8250,10 +8262,10 @@
       <c r="A162" s="35"/>
     </row>
     <row r="163" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A163" s="243" t="s">
+      <c r="A163" s="242" t="s">
         <v>129</v>
       </c>
-      <c r="B163" s="243"/>
+      <c r="B163" s="242"/>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164" s="9" t="s">
@@ -8268,7 +8280,7 @@
         <v>131</v>
       </c>
       <c r="B165" s="21" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="166" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8276,40 +8288,40 @@
         <v>132</v>
       </c>
       <c r="B166" s="21" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A167" s="242" t="s">
+      <c r="A167" s="241" t="s">
         <v>133</v>
       </c>
-      <c r="B167" s="242"/>
+      <c r="B167" s="241"/>
     </row>
     <row r="169" spans="1:7" ht="53.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A169" s="241" t="s">
+      <c r="A169" s="240" t="s">
         <v>134</v>
       </c>
-      <c r="B169" s="241"/>
-      <c r="C169" s="241"/>
-      <c r="D169" s="241"/>
+      <c r="B169" s="240"/>
+      <c r="C169" s="240"/>
+      <c r="D169" s="240"/>
     </row>
     <row r="170" spans="1:7" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A170" s="210" t="s">
+      <c r="A170" s="208" t="s">
         <v>135</v>
       </c>
-      <c r="B170" s="244" t="s">
+      <c r="B170" s="243" t="s">
         <v>136</v>
       </c>
-      <c r="C170" s="244"/>
-      <c r="D170" s="244"/>
+      <c r="C170" s="243"/>
+      <c r="D170" s="243"/>
     </row>
     <row r="172" spans="1:7" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A172" s="247" t="s">
+      <c r="A172" s="246" t="s">
         <v>137</v>
       </c>
-      <c r="B172" s="247"/>
-      <c r="C172" s="247"/>
-      <c r="D172" s="247"/>
+      <c r="B172" s="246"/>
+      <c r="C172" s="246"/>
+      <c r="D172" s="246"/>
     </row>
     <row r="174" spans="1:7" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A174" s="36" t="s">
@@ -8347,20 +8359,20 @@
       <c r="G176" s="15"/>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A177" s="242"/>
-      <c r="B177" s="242"/>
+      <c r="A177" s="241"/>
+      <c r="B177" s="241"/>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" s="38"/>
       <c r="B178" s="38"/>
     </row>
     <row r="179" spans="1:4" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A179" s="239" t="s">
-        <v>541</v>
-      </c>
-      <c r="B179" s="239"/>
-      <c r="C179" s="239"/>
-      <c r="D179" s="239"/>
+      <c r="A179" s="238" t="s">
+        <v>540</v>
+      </c>
+      <c r="B179" s="238"/>
+      <c r="C179" s="238"/>
+      <c r="D179" s="238"/>
     </row>
     <row r="180" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" s="9" t="s">
@@ -8401,20 +8413,20 @@
       <c r="D183" s="21"/>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A184" s="248"/>
-      <c r="B184" s="248"/>
+      <c r="A184" s="247"/>
+      <c r="B184" s="247"/>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" s="39"/>
       <c r="B185" s="39"/>
     </row>
     <row r="186" spans="1:4" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A186" s="241" t="s">
+      <c r="A186" s="240" t="s">
         <v>150</v>
       </c>
-      <c r="B186" s="241"/>
-      <c r="C186" s="241"/>
-      <c r="D186" s="241"/>
+      <c r="B186" s="240"/>
+      <c r="C186" s="240"/>
+      <c r="D186" s="240"/>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" s="9" t="s">
@@ -8426,48 +8438,48 @@
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" s="20" t="s">
+        <v>627</v>
+      </c>
+      <c r="B189" s="21" t="s">
         <v>628</v>
-      </c>
-      <c r="B189" s="21" t="s">
-        <v>629</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" s="20" t="s">
+        <v>629</v>
+      </c>
+      <c r="B190" s="21" t="s">
         <v>630</v>
-      </c>
-      <c r="B190" s="21" t="s">
-        <v>631</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" s="20" t="s">
+        <v>631</v>
+      </c>
+      <c r="B191" s="21" t="s">
         <v>632</v>
-      </c>
-      <c r="B191" s="21" t="s">
-        <v>633</v>
       </c>
     </row>
     <row r="192" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A192" s="20" t="s">
+        <v>633</v>
+      </c>
+      <c r="B192" s="21" t="s">
         <v>634</v>
-      </c>
-      <c r="B192" s="21" t="s">
-        <v>635</v>
       </c>
     </row>
     <row r="194" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A194" s="40" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="195" spans="1:4" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A195" s="251" t="s">
+      <c r="A195" s="250" t="s">
         <v>152</v>
       </c>
-      <c r="B195" s="251"/>
-      <c r="C195" s="251"/>
-      <c r="D195" s="251"/>
+      <c r="B195" s="250"/>
+      <c r="C195" s="250"/>
+      <c r="D195" s="250"/>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" s="41" t="s">
@@ -8498,20 +8510,20 @@
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A200" s="242"/>
-      <c r="B200" s="242"/>
+      <c r="A200" s="241"/>
+      <c r="B200" s="241"/>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" s="38"/>
       <c r="B201" s="38"/>
     </row>
     <row r="202" spans="1:4" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A202" s="245" t="s">
+      <c r="A202" s="244" t="s">
         <v>158</v>
       </c>
-      <c r="B202" s="245"/>
-      <c r="C202" s="245"/>
-      <c r="D202" s="245"/>
+      <c r="B202" s="244"/>
+      <c r="C202" s="244"/>
+      <c r="D202" s="244"/>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" s="9" t="s">
@@ -8526,7 +8538,7 @@
         <v>160</v>
       </c>
       <c r="B205" s="21" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="206" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -8534,15 +8546,15 @@
         <v>161</v>
       </c>
       <c r="B206" s="21" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="207" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A207" s="20" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="B207" s="21" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="208" spans="1:4" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -8554,12 +8566,12 @@
       <c r="A210" s="43"/>
     </row>
     <row r="211" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A211" s="246" t="s">
-        <v>543</v>
-      </c>
-      <c r="B211" s="246"/>
-      <c r="C211" s="246"/>
-      <c r="D211" s="246"/>
+      <c r="A211" s="245" t="s">
+        <v>542</v>
+      </c>
+      <c r="B211" s="245"/>
+      <c r="C211" s="245"/>
+      <c r="D211" s="245"/>
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A212" s="9" t="s">
@@ -8577,7 +8589,7 @@
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A213" s="20" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B213" s="20"/>
       <c r="C213" s="20"/>
@@ -8585,7 +8597,7 @@
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A214" s="20" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B214" s="20"/>
       <c r="C214" s="20"/>
@@ -8593,7 +8605,7 @@
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A215" s="20" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B215" s="20"/>
       <c r="C215" s="20"/>
@@ -8608,40 +8620,40 @@
       <c r="B217" s="38"/>
     </row>
     <row r="218" spans="1:6" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A218" s="241" t="s">
+      <c r="A218" s="240" t="s">
         <v>162</v>
       </c>
-      <c r="B218" s="241"/>
-      <c r="C218" s="241"/>
-      <c r="D218" s="241"/>
+      <c r="B218" s="240"/>
+      <c r="C218" s="240"/>
+      <c r="D218" s="240"/>
     </row>
     <row r="219" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A219" s="211" t="s">
+      <c r="A219" s="209" t="s">
         <v>163</v>
       </c>
-      <c r="B219" s="207" t="s">
+      <c r="B219" s="205" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="221" spans="1:6" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A221" s="245" t="s">
+      <c r="A221" s="244" t="s">
         <v>165</v>
       </c>
-      <c r="B221" s="245"/>
-      <c r="C221" s="245"/>
-      <c r="D221" s="245"/>
+      <c r="B221" s="244"/>
+      <c r="C221" s="244"/>
+      <c r="D221" s="244"/>
     </row>
     <row r="222" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A222" s="211" t="s">
+      <c r="A222" s="209" t="s">
         <v>163</v>
       </c>
-      <c r="B222" s="212" t="s">
+      <c r="B222" s="210" t="s">
         <v>166</v>
       </c>
-      <c r="C222" s="212"/>
-      <c r="D222" s="212"/>
-      <c r="E222" s="212"/>
-      <c r="F222" s="181"/>
+      <c r="C222" s="210"/>
+      <c r="D222" s="210"/>
+      <c r="E222" s="210"/>
+      <c r="F222" s="179"/>
     </row>
     <row r="224" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A224" s="40" t="s">
@@ -8649,54 +8661,54 @@
       </c>
     </row>
     <row r="225" spans="1:11" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A225" s="245" t="s">
+      <c r="A225" s="244" t="s">
         <v>168</v>
       </c>
-      <c r="B225" s="245"/>
-      <c r="C225" s="245"/>
-      <c r="D225" s="245"/>
+      <c r="B225" s="244"/>
+      <c r="C225" s="244"/>
+      <c r="D225" s="244"/>
     </row>
     <row r="226" spans="1:11" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A226" s="211" t="s">
+      <c r="A226" s="209" t="s">
         <v>163</v>
       </c>
-      <c r="B226" s="207" t="s">
+      <c r="B226" s="205" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="228" spans="1:11" ht="21" x14ac:dyDescent="0.25">
       <c r="A228" s="40" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="229" spans="1:11" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A229" s="245" t="s">
+      <c r="A229" s="244" t="s">
         <v>170</v>
       </c>
-      <c r="B229" s="245"/>
-      <c r="C229" s="245"/>
-      <c r="D229" s="245"/>
+      <c r="B229" s="244"/>
+      <c r="C229" s="244"/>
+      <c r="D229" s="244"/>
     </row>
     <row r="230" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A230" s="213" t="s">
+      <c r="A230" s="211" t="s">
         <v>163</v>
       </c>
-      <c r="B230" s="196" t="s">
+      <c r="B230" s="194" t="s">
         <v>171</v>
       </c>
-      <c r="C230" s="196"/>
-      <c r="D230" s="196"/>
-      <c r="E230" s="196"/>
-      <c r="F230" s="196"/>
-      <c r="G230" s="196"/>
-      <c r="H230" s="196"/>
-      <c r="I230" s="196"/>
-      <c r="J230" s="196"/>
-      <c r="K230" s="197"/>
+      <c r="C230" s="194"/>
+      <c r="D230" s="194"/>
+      <c r="E230" s="194"/>
+      <c r="F230" s="194"/>
+      <c r="G230" s="194"/>
+      <c r="H230" s="194"/>
+      <c r="I230" s="194"/>
+      <c r="J230" s="194"/>
+      <c r="K230" s="195"/>
     </row>
     <row r="231" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A231" s="214"/>
-      <c r="B231" s="205" t="s">
+      <c r="A231" s="212"/>
+      <c r="B231" s="203" t="s">
         <v>172</v>
       </c>
       <c r="C231" s="15" t="s">
@@ -8711,63 +8723,63 @@
       <c r="H231" s="15"/>
       <c r="I231" s="15"/>
       <c r="J231" s="15"/>
-      <c r="K231" s="198"/>
+      <c r="K231" s="196"/>
     </row>
     <row r="232" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A232" s="203"/>
-      <c r="B232" s="199"/>
-      <c r="C232" s="199" t="s">
+      <c r="A232" s="201"/>
+      <c r="B232" s="197"/>
+      <c r="C232" s="197" t="s">
         <v>60</v>
       </c>
-      <c r="D232" s="199"/>
-      <c r="E232" s="199"/>
-      <c r="F232" s="199"/>
-      <c r="G232" s="199"/>
-      <c r="H232" s="199"/>
-      <c r="I232" s="199"/>
-      <c r="J232" s="199"/>
-      <c r="K232" s="200"/>
+      <c r="D232" s="197"/>
+      <c r="E232" s="197"/>
+      <c r="F232" s="197"/>
+      <c r="G232" s="197"/>
+      <c r="H232" s="197"/>
+      <c r="I232" s="197"/>
+      <c r="J232" s="197"/>
+      <c r="K232" s="198"/>
     </row>
     <row r="234" spans="1:11" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A234" s="245" t="s">
+      <c r="A234" s="244" t="s">
         <v>175</v>
       </c>
-      <c r="B234" s="245"/>
-      <c r="C234" s="245"/>
-      <c r="D234" s="245"/>
+      <c r="B234" s="244"/>
+      <c r="C234" s="244"/>
+      <c r="D234" s="244"/>
     </row>
     <row r="235" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A235" s="213" t="s">
+      <c r="A235" s="211" t="s">
         <v>163</v>
       </c>
-      <c r="B235" s="196" t="s">
+      <c r="B235" s="194" t="s">
         <v>176</v>
       </c>
-      <c r="C235" s="196"/>
-      <c r="D235" s="196" t="s">
+      <c r="C235" s="194"/>
+      <c r="D235" s="194" t="s">
         <v>177</v>
       </c>
-      <c r="E235" s="196"/>
-      <c r="F235" s="196"/>
-      <c r="G235" s="196"/>
-      <c r="H235" s="196"/>
-      <c r="I235" s="197"/>
+      <c r="E235" s="194"/>
+      <c r="F235" s="194"/>
+      <c r="G235" s="194"/>
+      <c r="H235" s="194"/>
+      <c r="I235" s="195"/>
     </row>
     <row r="236" spans="1:11" ht="144.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A236" s="214"/>
+      <c r="A236" s="212"/>
       <c r="B236" s="15"/>
       <c r="C236" s="15"/>
-      <c r="D236" s="250" t="s">
+      <c r="D236" s="249" t="s">
         <v>178</v>
       </c>
-      <c r="E236" s="250"/>
+      <c r="E236" s="249"/>
       <c r="F236" s="15"/>
       <c r="G236" s="15"/>
       <c r="H236" s="15"/>
-      <c r="I236" s="198"/>
+      <c r="I236" s="196"/>
     </row>
     <row r="237" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A237" s="214"/>
+      <c r="A237" s="212"/>
       <c r="B237" s="15"/>
       <c r="C237" s="15"/>
       <c r="D237" s="15" t="s">
@@ -8779,51 +8791,51 @@
       <c r="F237" s="15"/>
       <c r="G237" s="15"/>
       <c r="H237" s="15"/>
-      <c r="I237" s="198"/>
+      <c r="I237" s="196"/>
     </row>
     <row r="238" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A238" s="203"/>
-      <c r="B238" s="199"/>
-      <c r="C238" s="199"/>
-      <c r="D238" s="199"/>
-      <c r="E238" s="199" t="s">
+      <c r="A238" s="201"/>
+      <c r="B238" s="197"/>
+      <c r="C238" s="197"/>
+      <c r="D238" s="197"/>
+      <c r="E238" s="197" t="s">
         <v>181</v>
       </c>
-      <c r="F238" s="199"/>
-      <c r="G238" s="199"/>
-      <c r="H238" s="199"/>
-      <c r="I238" s="200"/>
+      <c r="F238" s="197"/>
+      <c r="G238" s="197"/>
+      <c r="H238" s="197"/>
+      <c r="I238" s="198"/>
     </row>
     <row r="240" spans="1:11" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A240" s="245" t="s">
+      <c r="A240" s="244" t="s">
         <v>182</v>
       </c>
-      <c r="B240" s="245"/>
-      <c r="C240" s="245"/>
-      <c r="D240" s="245"/>
+      <c r="B240" s="244"/>
+      <c r="C240" s="244"/>
+      <c r="D240" s="244"/>
     </row>
     <row r="241" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A241" s="211" t="s">
+      <c r="A241" s="209" t="s">
         <v>163</v>
       </c>
-      <c r="B241" s="207" t="s">
+      <c r="B241" s="205" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="243" spans="1:7" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A243" s="241" t="s">
+      <c r="A243" s="240" t="s">
         <v>184</v>
       </c>
-      <c r="B243" s="241"/>
-      <c r="C243" s="241"/>
-      <c r="D243" s="241"/>
+      <c r="B243" s="240"/>
+      <c r="C243" s="240"/>
+      <c r="D243" s="240"/>
     </row>
     <row r="244" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A244" s="211" t="s">
+      <c r="A244" s="209" t="s">
         <v>163</v>
       </c>
-      <c r="B244" s="181" t="s">
-        <v>640</v>
+      <c r="B244" s="179" t="s">
+        <v>639</v>
       </c>
     </row>
     <row r="246" spans="1:7" ht="21" x14ac:dyDescent="0.25">
@@ -8832,44 +8844,44 @@
       </c>
     </row>
     <row r="247" spans="1:7" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A247" s="245" t="s">
+      <c r="A247" s="244" t="s">
         <v>186</v>
       </c>
-      <c r="B247" s="245"/>
-      <c r="C247" s="245"/>
-      <c r="D247" s="245"/>
+      <c r="B247" s="244"/>
+      <c r="C247" s="244"/>
+      <c r="D247" s="244"/>
     </row>
     <row r="248" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A248" s="213" t="s">
+      <c r="A248" s="211" t="s">
         <v>163</v>
       </c>
-      <c r="B248" s="196" t="s">
+      <c r="B248" s="194" t="s">
         <v>171</v>
       </c>
-      <c r="C248" s="196" t="s">
+      <c r="C248" s="194" t="s">
         <v>60</v>
       </c>
-      <c r="D248" s="196"/>
-      <c r="E248" s="196" t="s">
+      <c r="D248" s="194"/>
+      <c r="E248" s="194" t="s">
         <v>172</v>
       </c>
-      <c r="F248" s="196"/>
-      <c r="G248" s="197"/>
+      <c r="F248" s="194"/>
+      <c r="G248" s="195"/>
     </row>
     <row r="249" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A249" s="203"/>
-      <c r="B249" s="199" t="s">
+      <c r="A249" s="201"/>
+      <c r="B249" s="197" t="s">
         <v>187</v>
       </c>
-      <c r="C249" s="199" t="s">
+      <c r="C249" s="197" t="s">
         <v>188</v>
       </c>
-      <c r="D249" s="199"/>
-      <c r="E249" s="199" t="s">
+      <c r="D249" s="197"/>
+      <c r="E249" s="197" t="s">
         <v>189</v>
       </c>
-      <c r="F249" s="199"/>
-      <c r="G249" s="200"/>
+      <c r="F249" s="197"/>
+      <c r="G249" s="198"/>
     </row>
     <row r="251" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A251" s="40" t="s">
@@ -8877,12 +8889,12 @@
       </c>
     </row>
     <row r="252" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A252" s="245" t="s">
+      <c r="A252" s="244" t="s">
         <v>191</v>
       </c>
-      <c r="B252" s="245"/>
-      <c r="C252" s="245"/>
-      <c r="D252" s="245"/>
+      <c r="B252" s="244"/>
+      <c r="C252" s="244"/>
+      <c r="D252" s="244"/>
     </row>
     <row r="254" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A254" s="9" t="s">
@@ -8906,7 +8918,7 @@
         <v>195</v>
       </c>
       <c r="B256" s="21" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
     </row>
     <row r="257" spans="1:5" ht="231.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -8914,7 +8926,7 @@
         <v>196</v>
       </c>
       <c r="B257" s="21" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="258" spans="1:5" ht="148.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8922,11 +8934,11 @@
         <v>197</v>
       </c>
       <c r="B258" s="21" t="s">
-        <v>642</v>
-      </c>
-      <c r="C258" s="249"/>
-      <c r="D258" s="249"/>
-      <c r="E258" s="249"/>
+        <v>641</v>
+      </c>
+      <c r="C258" s="248"/>
+      <c r="D258" s="248"/>
+      <c r="E258" s="248"/>
     </row>
     <row r="259" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A259" s="38"/>
@@ -8938,10 +8950,10 @@
       </c>
     </row>
     <row r="261" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A261" s="245" t="s">
+      <c r="A261" s="244" t="s">
         <v>199</v>
       </c>
-      <c r="B261" s="245"/>
+      <c r="B261" s="244"/>
     </row>
     <row r="262" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A262" s="44"/>
@@ -8952,65 +8964,65 @@
       </c>
     </row>
     <row r="264" spans="1:5" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A264" s="245" t="s">
+      <c r="A264" s="244" t="s">
         <v>201</v>
       </c>
-      <c r="B264" s="245"/>
-      <c r="C264" s="245"/>
-      <c r="D264" s="245"/>
+      <c r="B264" s="244"/>
+      <c r="C264" s="244"/>
+      <c r="D264" s="244"/>
     </row>
     <row r="265" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A265" s="211" t="s">
+      <c r="A265" s="209" t="s">
         <v>90</v>
       </c>
-      <c r="B265" s="181" t="s">
+      <c r="B265" s="179" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="267" spans="1:5" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A267" s="245" t="s">
+      <c r="A267" s="244" t="s">
         <v>203</v>
       </c>
-      <c r="B267" s="245"/>
-      <c r="C267" s="245"/>
-      <c r="D267" s="245"/>
+      <c r="B267" s="244"/>
+      <c r="C267" s="244"/>
+      <c r="D267" s="244"/>
     </row>
     <row r="268" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A268" s="211" t="s">
+      <c r="A268" s="209" t="s">
         <v>90</v>
       </c>
-      <c r="B268" s="181" t="s">
+      <c r="B268" s="179" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="269" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="270" spans="1:5" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A270" s="245" t="s">
+      <c r="A270" s="244" t="s">
         <v>204</v>
       </c>
-      <c r="B270" s="245"/>
+      <c r="B270" s="244"/>
     </row>
     <row r="271" spans="1:5" ht="59.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A271" s="245" t="s">
+      <c r="A271" s="244" t="s">
         <v>205</v>
       </c>
-      <c r="B271" s="245"/>
+      <c r="B271" s="244"/>
     </row>
     <row r="272" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A272" s="211" t="s">
+      <c r="A272" s="209" t="s">
         <v>90</v>
       </c>
-      <c r="B272" s="181" t="s">
+      <c r="B272" s="179" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="274" spans="1:7" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A274" s="243" t="s">
-        <v>546</v>
-      </c>
-      <c r="B274" s="243"/>
-      <c r="C274" s="243"/>
-      <c r="D274" s="243"/>
+      <c r="A274" s="242" t="s">
+        <v>545</v>
+      </c>
+      <c r="B274" s="242"/>
+      <c r="C274" s="242"/>
+      <c r="D274" s="242"/>
     </row>
     <row r="275" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A275" s="9" t="s">
@@ -9028,7 +9040,7 @@
     </row>
     <row r="276" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A276" s="22" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B276" s="45"/>
       <c r="C276" s="22"/>
@@ -9036,15 +9048,15 @@
     </row>
     <row r="277" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A277" s="22" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B277" s="22"/>
       <c r="C277" s="22"/>
       <c r="D277" s="23"/>
     </row>
     <row r="278" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A278" s="242"/>
-      <c r="B278" s="242"/>
+      <c r="A278" s="241"/>
+      <c r="B278" s="241"/>
     </row>
     <row r="279" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A279" s="38"/>
@@ -9069,33 +9081,33 @@
       </c>
     </row>
     <row r="284" spans="1:7" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A284" s="245" t="s">
+      <c r="A284" s="244" t="s">
         <v>210</v>
       </c>
-      <c r="B284" s="245"/>
-      <c r="C284" s="245"/>
-      <c r="D284" s="245"/>
+      <c r="B284" s="244"/>
+      <c r="C284" s="244"/>
+      <c r="D284" s="244"/>
     </row>
     <row r="285" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A285" s="211" t="s">
+      <c r="A285" s="209" t="s">
         <v>90</v>
       </c>
-      <c r="B285" s="212" t="s">
+      <c r="B285" s="210" t="s">
         <v>211</v>
       </c>
-      <c r="C285" s="212"/>
-      <c r="D285" s="212"/>
-      <c r="E285" s="212"/>
-      <c r="F285" s="212"/>
-      <c r="G285" s="181"/>
+      <c r="C285" s="210"/>
+      <c r="D285" s="210"/>
+      <c r="E285" s="210"/>
+      <c r="F285" s="210"/>
+      <c r="G285" s="179"/>
     </row>
     <row r="287" spans="1:7" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A287" s="243" t="s">
-        <v>549</v>
-      </c>
-      <c r="B287" s="243"/>
-      <c r="C287" s="243"/>
-      <c r="D287" s="243"/>
+      <c r="A287" s="242" t="s">
+        <v>548</v>
+      </c>
+      <c r="B287" s="242"/>
+      <c r="C287" s="242"/>
+      <c r="D287" s="242"/>
     </row>
     <row r="289" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A289" s="47" t="s">
@@ -9113,7 +9125,7 @@
     </row>
     <row r="290" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A290" s="22" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B290" s="22"/>
       <c r="C290" s="22"/>
@@ -9242,23 +9254,23 @@
   <dimension ref="A1:AMI116"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="C36" sqref="C36"/>
+      <selection pane="bottomLeft" activeCell="C81" sqref="C81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.140625" style="191" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" style="191" customWidth="1"/>
-    <col min="3" max="3" width="142.140625" style="192" customWidth="1"/>
-    <col min="4" max="6" width="5.7109375" style="193" customWidth="1"/>
-    <col min="7" max="11" width="8.7109375" style="193" customWidth="1"/>
-    <col min="12" max="12" width="78.7109375" style="193" customWidth="1"/>
-    <col min="13" max="13" width="36.85546875" style="191" customWidth="1"/>
-    <col min="14" max="14" width="29" style="191" customWidth="1"/>
-    <col min="15" max="15" width="73.7109375" style="191" customWidth="1"/>
-    <col min="16" max="1023" width="11.42578125" style="191"/>
+    <col min="1" max="1" width="11.140625" style="189" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" style="189" customWidth="1"/>
+    <col min="3" max="3" width="142.140625" style="190" customWidth="1"/>
+    <col min="4" max="6" width="5.7109375" style="191" customWidth="1"/>
+    <col min="7" max="11" width="8.7109375" style="191" customWidth="1"/>
+    <col min="12" max="12" width="78.7109375" style="191" customWidth="1"/>
+    <col min="13" max="13" width="36.85546875" style="189" customWidth="1"/>
+    <col min="14" max="14" width="29" style="189" customWidth="1"/>
+    <col min="15" max="15" width="73.7109375" style="189" customWidth="1"/>
+    <col min="16" max="1023" width="11.42578125" style="189"/>
     <col min="1024" max="16384" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
@@ -9272,11 +9284,11 @@
       <c r="C1" s="52" t="s">
         <v>215</v>
       </c>
-      <c r="D1" s="255" t="s">
+      <c r="D1" s="254" t="s">
         <v>216</v>
       </c>
-      <c r="E1" s="255"/>
-      <c r="F1" s="255"/>
+      <c r="E1" s="254"/>
+      <c r="F1" s="254"/>
       <c r="G1" s="53"/>
       <c r="H1" s="53"/>
       <c r="I1" s="53"/>
@@ -9324,14 +9336,14 @@
       </c>
     </row>
     <row r="3" spans="1:19" s="54" customFormat="1" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="256" t="s">
+      <c r="A3" s="255" t="s">
         <v>233</v>
       </c>
-      <c r="B3" s="256"/>
-      <c r="C3" s="256"/>
-      <c r="D3" s="256"/>
-      <c r="E3" s="256"/>
-      <c r="F3" s="256"/>
+      <c r="B3" s="255"/>
+      <c r="C3" s="255"/>
+      <c r="D3" s="255"/>
+      <c r="E3" s="255"/>
+      <c r="F3" s="255"/>
       <c r="G3" s="62"/>
       <c r="H3" s="63"/>
       <c r="I3" s="63"/>
@@ -9350,7 +9362,7 @@
         <v>235</v>
       </c>
       <c r="C4" s="69" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="D4" s="70" t="s">
         <v>229</v>
@@ -9371,14 +9383,14 @@
       <c r="L4" s="75" t="s">
         <v>236</v>
       </c>
-      <c r="M4" s="217" t="s">
-        <v>648</v>
+      <c r="M4" s="215" t="s">
+        <v>647</v>
       </c>
       <c r="N4" s="77" t="s">
         <v>237</v>
       </c>
       <c r="O4" s="78" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="5" spans="1:19" s="54" customFormat="1" ht="90" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -9389,7 +9401,7 @@
         <v>239</v>
       </c>
       <c r="C5" s="81" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="D5" s="82" t="s">
         <v>229</v>
@@ -9406,7 +9418,7 @@
       <c r="J5" s="84"/>
       <c r="K5" s="85"/>
       <c r="L5" s="37" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="M5" s="86" t="s">
         <v>240</v>
@@ -9415,7 +9427,7 @@
         <v>86</v>
       </c>
       <c r="O5" s="88" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="P5" s="3"/>
       <c r="Q5" s="3"/>
@@ -9430,7 +9442,7 @@
         <v>239</v>
       </c>
       <c r="C6" s="81" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="D6" s="59" t="s">
         <v>229</v>
@@ -9441,7 +9453,7 @@
         <v>230</v>
       </c>
       <c r="H6" s="90" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="I6" s="91"/>
       <c r="J6" s="91"/>
@@ -9456,7 +9468,7 @@
         <v>86</v>
       </c>
       <c r="O6" s="94" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="P6" s="3"/>
       <c r="Q6" s="3"/>
@@ -9471,7 +9483,7 @@
         <v>235</v>
       </c>
       <c r="C7" s="81" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="D7" s="59" t="s">
         <v>229</v>
@@ -9488,7 +9500,7 @@
       <c r="J7" s="95"/>
       <c r="K7" s="96"/>
       <c r="L7" s="37" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="M7" s="76" t="s">
         <v>86</v>
@@ -9512,7 +9524,7 @@
         <v>235</v>
       </c>
       <c r="C8" s="81" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="D8" s="59" t="s">
         <v>229</v>
@@ -9551,7 +9563,7 @@
         <v>235</v>
       </c>
       <c r="C9" s="81" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="D9" s="59" t="s">
         <v>229</v>
@@ -9566,7 +9578,7 @@
       <c r="J9" s="95"/>
       <c r="K9" s="96"/>
       <c r="L9" s="98" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="M9" s="95" t="s">
         <v>249</v>
@@ -9620,7 +9632,7 @@
         <v>235</v>
       </c>
       <c r="C11" s="81" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="D11" s="59" t="s">
         <v>229</v>
@@ -9636,7 +9648,7 @@
       <c r="I11" s="91"/>
       <c r="J11" s="91"/>
       <c r="K11" s="86"/>
-      <c r="L11" s="195" t="s">
+      <c r="L11" s="193" t="s">
         <v>255</v>
       </c>
       <c r="M11" s="98" t="s">
@@ -9661,7 +9673,7 @@
         <v>235</v>
       </c>
       <c r="C12" s="81" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="D12" s="59" t="s">
         <v>229</v>
@@ -9682,7 +9694,7 @@
       </c>
       <c r="K12" s="86"/>
       <c r="L12" s="112" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="M12" s="95" t="s">
         <v>249</v>
@@ -9805,7 +9817,7 @@
         <v>235</v>
       </c>
       <c r="C16" s="81" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D16" s="59" t="s">
         <v>229</v>
@@ -9846,7 +9858,7 @@
         <v>239</v>
       </c>
       <c r="C17" s="81" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="D17" s="121" t="s">
         <v>229</v>
@@ -9982,7 +9994,7 @@
         <v>239</v>
       </c>
       <c r="C21" s="81" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="D21" s="59" t="s">
         <v>229</v>
@@ -9999,16 +10011,16 @@
       <c r="J21" s="126"/>
       <c r="K21" s="126"/>
       <c r="L21" s="112" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="M21" s="76" t="s">
         <v>86</v>
       </c>
       <c r="N21" s="127" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="O21" s="128" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="22" spans="1:15" s="54" customFormat="1" ht="264" customHeight="1" x14ac:dyDescent="0.25">
@@ -10019,7 +10031,7 @@
         <v>289</v>
       </c>
       <c r="C22" s="81" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="D22" s="129" t="s">
         <v>229</v>
@@ -10041,13 +10053,13 @@
         <v>290</v>
       </c>
       <c r="M22" s="112" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="N22" s="85" t="s">
         <v>237</v>
       </c>
       <c r="O22" s="128" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="23" spans="1:15" s="54" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10058,7 +10070,7 @@
         <v>292</v>
       </c>
       <c r="C23" s="81" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="D23" s="129" t="s">
         <v>229</v>
@@ -10075,7 +10087,7 @@
       <c r="J23" s="126"/>
       <c r="K23" s="126"/>
       <c r="L23" s="112" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="M23" s="126" t="s">
         <v>240</v>
@@ -10084,7 +10096,7 @@
         <v>237</v>
       </c>
       <c r="O23" s="128" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="24" spans="1:15" s="104" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10154,14 +10166,14 @@
       </c>
     </row>
     <row r="26" spans="1:15" s="54" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="257" t="s">
+      <c r="A26" s="256" t="s">
         <v>299</v>
       </c>
-      <c r="B26" s="257"/>
-      <c r="C26" s="257"/>
-      <c r="D26" s="257"/>
-      <c r="E26" s="257"/>
-      <c r="F26" s="257"/>
+      <c r="B26" s="256"/>
+      <c r="C26" s="256"/>
+      <c r="D26" s="256"/>
+      <c r="E26" s="256"/>
+      <c r="F26" s="256"/>
       <c r="G26" s="134"/>
       <c r="H26" s="135"/>
       <c r="I26" s="135"/>
@@ -10180,7 +10192,7 @@
         <v>235</v>
       </c>
       <c r="C27" s="81" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="D27" s="129" t="s">
         <v>229</v>
@@ -10195,7 +10207,7 @@
       <c r="J27" s="86"/>
       <c r="K27" s="86"/>
       <c r="L27" s="112" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="M27" s="76" t="s">
         <v>86</v>
@@ -10215,7 +10227,7 @@
         <v>235</v>
       </c>
       <c r="C28" s="81" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="D28" s="129" t="s">
         <v>229</v>
@@ -10233,8 +10245,8 @@
       </c>
       <c r="J28" s="126"/>
       <c r="K28" s="126"/>
-      <c r="L28" s="194" t="s">
-        <v>621</v>
+      <c r="L28" s="192" t="s">
+        <v>620</v>
       </c>
       <c r="M28" s="126" t="s">
         <v>240</v>
@@ -10254,7 +10266,7 @@
         <v>235</v>
       </c>
       <c r="C29" s="81" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="D29" s="129" t="s">
         <v>229</v>
@@ -10291,7 +10303,7 @@
         <v>235</v>
       </c>
       <c r="C30" s="144" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D30" s="145"/>
       <c r="E30" s="145" t="s">
@@ -10324,7 +10336,7 @@
         <v>235</v>
       </c>
       <c r="C31" s="81" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="D31" s="129" t="s">
         <v>229</v>
@@ -10361,7 +10373,7 @@
         <v>235</v>
       </c>
       <c r="C32" s="81" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="D32" s="129" t="s">
         <v>229</v>
@@ -10396,7 +10408,7 @@
         <v>235</v>
       </c>
       <c r="C33" s="81" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="D33" s="129" t="s">
         <v>229</v>
@@ -10424,7 +10436,7 @@
         <v>411</v>
       </c>
       <c r="O33" s="128" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="Q33" s="53"/>
     </row>
@@ -10436,7 +10448,7 @@
         <v>235</v>
       </c>
       <c r="C34" s="81" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="D34" s="129" t="s">
         <v>229</v>
@@ -10466,14 +10478,14 @@
       </c>
     </row>
     <row r="35" spans="1:17" s="54" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="257" t="s">
+      <c r="A35" s="256" t="s">
         <v>315</v>
       </c>
-      <c r="B35" s="257"/>
-      <c r="C35" s="257"/>
-      <c r="D35" s="257"/>
-      <c r="E35" s="257"/>
-      <c r="F35" s="257"/>
+      <c r="B35" s="256"/>
+      <c r="C35" s="256"/>
+      <c r="D35" s="256"/>
+      <c r="E35" s="256"/>
+      <c r="F35" s="256"/>
       <c r="G35" s="134"/>
       <c r="H35" s="135"/>
       <c r="I35" s="135"/>
@@ -10492,7 +10504,7 @@
         <v>235</v>
       </c>
       <c r="C36" s="81" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="D36" s="129" t="s">
         <v>229</v>
@@ -10515,7 +10527,7 @@
         <v>318</v>
       </c>
       <c r="N36" s="127" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="O36" s="153" t="s">
         <v>319</v>
@@ -10529,7 +10541,7 @@
         <v>292</v>
       </c>
       <c r="C37" s="81" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="D37" s="129" t="s">
         <v>229</v>
@@ -10559,11 +10571,11 @@
       </c>
     </row>
     <row r="38" spans="1:17" s="54" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="258" t="s">
+      <c r="A38" s="257" t="s">
         <v>322</v>
       </c>
-      <c r="B38" s="258"/>
-      <c r="C38" s="258"/>
+      <c r="B38" s="257"/>
+      <c r="C38" s="257"/>
       <c r="D38" s="154"/>
       <c r="E38" s="154"/>
       <c r="F38" s="155"/>
@@ -10600,7 +10612,7 @@
       <c r="J39" s="126"/>
       <c r="K39" s="126"/>
       <c r="L39" s="112" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="M39" s="112" t="s">
         <v>318</v>
@@ -10620,7 +10632,7 @@
         <v>235</v>
       </c>
       <c r="C40" s="159" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="D40" s="156" t="s">
         <v>229</v>
@@ -10659,7 +10671,7 @@
         <v>239</v>
       </c>
       <c r="C41" s="81" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="D41" s="156" t="s">
         <v>229</v>
@@ -10677,13 +10689,13 @@
         <v>329</v>
       </c>
       <c r="M41" s="112" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="N41" s="127" t="s">
         <v>411</v>
       </c>
       <c r="O41" s="128" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="42" spans="1:17" s="54" customFormat="1" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -10694,7 +10706,7 @@
         <v>235</v>
       </c>
       <c r="C42" s="81" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="D42" s="156" t="s">
         <v>229</v>
@@ -10762,7 +10774,7 @@
         <v>239</v>
       </c>
       <c r="C44" s="81" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="D44" s="156" t="s">
         <v>229</v>
@@ -10776,8 +10788,8 @@
       <c r="I44" s="86"/>
       <c r="J44" s="86"/>
       <c r="K44" s="86"/>
-      <c r="L44" s="76" t="s">
-        <v>86</v>
+      <c r="L44" s="215" t="s">
+        <v>654</v>
       </c>
       <c r="M44" s="112" t="s">
         <v>240</v>
@@ -10789,7 +10801,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="45" spans="1:17" s="54" customFormat="1" ht="193.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" s="54" customFormat="1" ht="193.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="79" t="s">
         <v>339</v>
       </c>
@@ -10797,7 +10809,7 @@
         <v>239</v>
       </c>
       <c r="C45" s="81" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="D45" s="156" t="s">
         <v>229</v>
@@ -10834,7 +10846,7 @@
         <v>235</v>
       </c>
       <c r="C46" s="81" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="D46" s="156" t="s">
         <v>229</v>
@@ -10849,7 +10861,7 @@
       <c r="J46" s="126"/>
       <c r="K46" s="126"/>
       <c r="L46" s="112" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="M46" s="76" t="s">
         <v>86</v>
@@ -10902,7 +10914,7 @@
         <v>235</v>
       </c>
       <c r="C48" s="81" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="D48" s="156" t="s">
         <v>229</v>
@@ -10917,7 +10929,7 @@
       <c r="J48" s="126"/>
       <c r="K48" s="126"/>
       <c r="L48" s="112" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="M48" s="76" t="s">
         <v>86</v>
@@ -10937,7 +10949,7 @@
         <v>235</v>
       </c>
       <c r="C49" s="81" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="D49" s="164" t="s">
         <v>229</v>
@@ -10966,7 +10978,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="50" spans="1:15" s="54" customFormat="1" ht="209.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" s="54" customFormat="1" ht="209.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="79" t="s">
         <v>353</v>
       </c>
@@ -11003,14 +11015,14 @@
         <v>358</v>
       </c>
     </row>
-    <row r="51" spans="1:15" s="54" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" s="54" customFormat="1" ht="99" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="79" t="s">
         <v>359</v>
       </c>
       <c r="B51" s="140" t="s">
         <v>292</v>
       </c>
-      <c r="C51" s="14" t="s">
+      <c r="C51" s="216" t="s">
         <v>360</v>
       </c>
       <c r="D51" s="156" t="s">
@@ -11040,7 +11052,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="52" spans="1:15" s="54" customFormat="1" ht="235.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" s="54" customFormat="1" ht="235.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="79" t="s">
         <v>363</v>
       </c>
@@ -11048,7 +11060,7 @@
         <v>278</v>
       </c>
       <c r="C52" s="81" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="D52" s="156" t="s">
         <v>229</v>
@@ -11083,7 +11095,7 @@
         <v>235</v>
       </c>
       <c r="C53" s="81" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="D53" s="156" t="s">
         <v>229</v>
@@ -11282,7 +11294,7 @@
         <v>381</v>
       </c>
       <c r="C59" s="81" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="D59" s="156" t="s">
         <v>229</v>
@@ -11302,7 +11314,7 @@
         <v>382</v>
       </c>
       <c r="M59" s="126" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="N59" s="127" t="s">
         <v>357</v>
@@ -11352,7 +11364,7 @@
         <v>388</v>
       </c>
       <c r="C61" s="81" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="D61" s="156" t="s">
         <v>229</v>
@@ -11372,7 +11384,7 @@
         <v>389</v>
       </c>
       <c r="M61" s="126" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="N61" s="127" t="s">
         <v>357</v>
@@ -11381,7 +11393,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="62" spans="1:15" s="54" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" s="54" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="79" t="s">
         <v>391</v>
       </c>
@@ -11389,7 +11401,7 @@
         <v>235</v>
       </c>
       <c r="C62" s="81" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="D62" s="156" t="s">
         <v>229</v>
@@ -11424,7 +11436,7 @@
         <v>235</v>
       </c>
       <c r="C63" s="81" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D63" s="156" t="s">
         <v>229</v>
@@ -11459,7 +11471,7 @@
         <v>235</v>
       </c>
       <c r="C64" s="81" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D64" s="156" t="s">
         <v>229</v>
@@ -11529,7 +11541,7 @@
         <v>235</v>
       </c>
       <c r="C66" s="81" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="D66" s="156" t="s">
         <v>229</v>
@@ -11549,7 +11561,7 @@
         <v>402</v>
       </c>
       <c r="M66" s="126" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="N66" s="127" t="s">
         <v>357</v>
@@ -11566,7 +11578,7 @@
         <v>235</v>
       </c>
       <c r="C67" s="81" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D67" s="156" t="s">
         <v>229</v>
@@ -11586,13 +11598,13 @@
         <v>405</v>
       </c>
       <c r="M67" s="112" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="N67" s="127" t="s">
         <v>357</v>
       </c>
       <c r="O67" s="128" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="68" spans="1:15" s="54" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11603,7 +11615,7 @@
         <v>239</v>
       </c>
       <c r="C68" s="81" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="D68" s="156" t="s">
         <v>229</v>
@@ -11621,13 +11633,13 @@
         <v>407</v>
       </c>
       <c r="M68" s="126" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="N68" s="127" t="s">
         <v>357</v>
       </c>
       <c r="O68" s="128" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="69" spans="1:15" s="54" customFormat="1" ht="87" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -11638,7 +11650,7 @@
         <v>239</v>
       </c>
       <c r="C69" s="81" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="D69" s="156" t="s">
         <v>229</v>
@@ -11666,14 +11678,14 @@
       </c>
     </row>
     <row r="70" spans="1:15" s="54" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="257" t="s">
+      <c r="A70" s="256" t="s">
         <v>413</v>
       </c>
-      <c r="B70" s="257"/>
-      <c r="C70" s="257"/>
-      <c r="D70" s="257"/>
-      <c r="E70" s="257"/>
-      <c r="F70" s="257"/>
+      <c r="B70" s="256"/>
+      <c r="C70" s="256"/>
+      <c r="D70" s="256"/>
+      <c r="E70" s="256"/>
+      <c r="F70" s="256"/>
       <c r="G70" s="134"/>
       <c r="H70" s="135"/>
       <c r="I70" s="135"/>
@@ -11692,7 +11704,7 @@
         <v>235</v>
       </c>
       <c r="C71" s="81" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="D71" s="156" t="s">
         <v>229</v>
@@ -11727,7 +11739,7 @@
         <v>235</v>
       </c>
       <c r="C72" s="81" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="D72" s="156" t="s">
         <v>229</v>
@@ -11820,7 +11832,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="75" spans="1:15" s="54" customFormat="1" ht="59.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:15" s="54" customFormat="1" ht="178.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="79" t="s">
         <v>425</v>
       </c>
@@ -11828,62 +11840,62 @@
         <v>235</v>
       </c>
       <c r="C75" s="81" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="D75" s="156" t="s">
         <v>229</v>
       </c>
       <c r="E75" s="129"/>
       <c r="F75" s="130"/>
-      <c r="G75" s="174" t="s">
-        <v>232</v>
+      <c r="G75" s="172" t="s">
+        <v>231</v>
       </c>
       <c r="H75" s="126"/>
       <c r="I75" s="126"/>
       <c r="J75" s="126"/>
       <c r="K75" s="126"/>
       <c r="L75" s="112" t="s">
-        <v>426</v>
+        <v>656</v>
       </c>
       <c r="M75" s="126" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="N75" s="127" t="s">
         <v>53</v>
       </c>
       <c r="O75" s="153" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15" s="54" customFormat="1" ht="71.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="79" t="s">
         <v>427</v>
-      </c>
-    </row>
-    <row r="76" spans="1:15" s="54" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="79" t="s">
-        <v>428</v>
       </c>
       <c r="B76" s="80" t="s">
         <v>239</v>
       </c>
       <c r="C76" s="81" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="D76" s="156" t="s">
         <v>229</v>
       </c>
       <c r="E76" s="129"/>
       <c r="F76" s="130"/>
-      <c r="G76" s="175" t="s">
-        <v>232</v>
-      </c>
-      <c r="H76" s="175" t="s">
-        <v>232</v>
+      <c r="G76" s="172" t="s">
+        <v>231</v>
+      </c>
+      <c r="H76" s="172" t="s">
+        <v>231</v>
       </c>
       <c r="I76" s="126"/>
       <c r="J76" s="126"/>
       <c r="K76" s="126"/>
       <c r="L76" s="112" t="s">
-        <v>426</v>
+        <v>655</v>
       </c>
       <c r="M76" s="126" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="N76" s="127" t="s">
         <v>53</v>
@@ -11892,30 +11904,30 @@
         <v>86</v>
       </c>
     </row>
-    <row r="77" spans="1:15" s="54" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:15" s="54" customFormat="1" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="79" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B77" s="80" t="s">
         <v>292</v>
       </c>
       <c r="C77" s="81" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="D77" s="156" t="s">
         <v>229</v>
       </c>
       <c r="E77" s="129"/>
       <c r="F77" s="130"/>
-      <c r="G77" s="175" t="s">
-        <v>232</v>
+      <c r="G77" s="172" t="s">
+        <v>231</v>
       </c>
       <c r="H77" s="126"/>
       <c r="I77" s="126"/>
       <c r="J77" s="126"/>
       <c r="K77" s="126"/>
       <c r="L77" s="112" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="M77" s="76" t="s">
         <v>86</v>
@@ -11924,33 +11936,33 @@
         <v>411</v>
       </c>
       <c r="O77" s="153" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="78" spans="1:15" s="54" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="78" spans="1:15" s="54" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="79" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B78" s="80" t="s">
         <v>278</v>
       </c>
       <c r="C78" s="81" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="D78" s="156" t="s">
         <v>229</v>
       </c>
       <c r="E78" s="129"/>
       <c r="F78" s="130"/>
-      <c r="G78" s="175" t="s">
-        <v>232</v>
+      <c r="G78" s="172" t="s">
+        <v>231</v>
       </c>
       <c r="H78" s="126"/>
       <c r="I78" s="126"/>
       <c r="J78" s="126"/>
       <c r="K78" s="126"/>
-      <c r="L78" s="176" t="s">
-        <v>86</v>
+      <c r="L78" s="174" t="s">
+        <v>657</v>
       </c>
       <c r="M78" s="76" t="s">
         <v>86</v>
@@ -11959,18 +11971,18 @@
         <v>411</v>
       </c>
       <c r="O78" s="128" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="79" spans="1:15" s="54" customFormat="1" ht="195" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="79" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B79" s="80" t="s">
         <v>235</v>
       </c>
       <c r="C79" s="81" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="D79" s="156" t="s">
         <v>229</v>
@@ -11985,7 +11997,7 @@
       <c r="J79" s="126"/>
       <c r="K79" s="126"/>
       <c r="L79" s="112" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="M79" s="76" t="s">
         <v>86</v>
@@ -11994,24 +12006,24 @@
         <v>86</v>
       </c>
       <c r="O79" s="153" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="80" spans="1:15" s="54" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="79" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B80" s="80" t="s">
         <v>235</v>
       </c>
       <c r="C80" s="81" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="D80" s="151" t="s">
         <v>229</v>
       </c>
       <c r="E80" s="129"/>
-      <c r="F80" s="177"/>
+      <c r="F80" s="175"/>
       <c r="G80" s="72" t="s">
         <v>230</v>
       </c>
@@ -12020,7 +12032,7 @@
       <c r="J80" s="126"/>
       <c r="K80" s="126"/>
       <c r="L80" s="112" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="M80" s="76" t="s">
         <v>86</v>
@@ -12034,13 +12046,13 @@
     </row>
     <row r="81" spans="1:15" s="54" customFormat="1" ht="192.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="79" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B81" s="80" t="s">
         <v>235</v>
       </c>
       <c r="C81" s="81" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="D81" s="156" t="s">
         <v>229</v>
@@ -12055,7 +12067,7 @@
       <c r="J81" s="126"/>
       <c r="K81" s="126"/>
       <c r="L81" s="131" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="M81" s="76" t="s">
         <v>86</v>
@@ -12064,18 +12076,18 @@
         <v>86</v>
       </c>
       <c r="O81" s="128" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="82" spans="1:15" s="54" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="257" t="s">
+      <c r="A82" s="256" t="s">
         <v>167</v>
       </c>
-      <c r="B82" s="257"/>
-      <c r="C82" s="257"/>
-      <c r="D82" s="257"/>
-      <c r="E82" s="257"/>
-      <c r="F82" s="257"/>
+      <c r="B82" s="256"/>
+      <c r="C82" s="256"/>
+      <c r="D82" s="256"/>
+      <c r="E82" s="256"/>
+      <c r="F82" s="256"/>
       <c r="G82" s="134"/>
       <c r="H82" s="135"/>
       <c r="I82" s="135"/>
@@ -12088,13 +12100,13 @@
     </row>
     <row r="83" spans="1:15" s="54" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="120" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B83" s="80" t="s">
         <v>235</v>
       </c>
       <c r="C83" s="81" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="D83" s="156" t="s">
         <v>229</v>
@@ -12111,27 +12123,27 @@
       <c r="J83" s="126"/>
       <c r="K83" s="126"/>
       <c r="L83" s="112" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="M83" s="126" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="N83" s="127" t="s">
         <v>357</v>
       </c>
       <c r="O83" s="128" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="84" spans="1:15" s="54" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A84" s="79" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B84" s="80" t="s">
         <v>235</v>
       </c>
       <c r="C84" s="81" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="D84" s="156" t="s">
         <v>229</v>
@@ -12145,8 +12157,8 @@
       <c r="I84" s="126"/>
       <c r="J84" s="126"/>
       <c r="K84" s="126"/>
-      <c r="L84" s="178" t="s">
-        <v>443</v>
+      <c r="L84" s="176" t="s">
+        <v>442</v>
       </c>
       <c r="M84" s="76" t="s">
         <v>86</v>
@@ -12155,18 +12167,18 @@
         <v>357</v>
       </c>
       <c r="O84" s="128" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="85" spans="1:15" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="79" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B85" s="80" t="s">
         <v>292</v>
       </c>
       <c r="C85" s="81" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="D85" s="156" t="s">
         <v>229</v>
@@ -12180,7 +12192,7 @@
       <c r="I85" s="126"/>
       <c r="J85" s="126"/>
       <c r="K85" s="126"/>
-      <c r="L85" s="176" t="s">
+      <c r="L85" s="174" t="s">
         <v>86</v>
       </c>
       <c r="M85" s="76" t="s">
@@ -12190,18 +12202,18 @@
         <v>411</v>
       </c>
       <c r="O85" s="153" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="86" spans="1:15" s="54" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A86" s="79" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B86" s="80" t="s">
         <v>235</v>
       </c>
       <c r="C86" s="81" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="D86" s="156" t="s">
         <v>229</v>
@@ -12215,8 +12227,8 @@
       <c r="I86" s="126"/>
       <c r="J86" s="126"/>
       <c r="K86" s="126"/>
-      <c r="L86" s="178" t="s">
-        <v>443</v>
+      <c r="L86" s="176" t="s">
+        <v>442</v>
       </c>
       <c r="M86" s="76" t="s">
         <v>86</v>
@@ -12225,18 +12237,18 @@
         <v>411</v>
       </c>
       <c r="O86" s="128" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="87" spans="1:15" s="54" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A87" s="79" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B87" s="80" t="s">
         <v>381</v>
       </c>
       <c r="C87" s="81" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D87" s="156" t="s">
         <v>229</v>
@@ -12252,7 +12264,7 @@
       <c r="I87" s="126"/>
       <c r="J87" s="126"/>
       <c r="K87" s="126"/>
-      <c r="L87" s="176" t="s">
+      <c r="L87" s="174" t="s">
         <v>86</v>
       </c>
       <c r="M87" s="76" t="s">
@@ -12262,18 +12274,18 @@
         <v>411</v>
       </c>
       <c r="O87" s="128" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="88" spans="1:15" s="54" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="256" t="s">
         <v>450</v>
       </c>
-    </row>
-    <row r="88" spans="1:15" s="54" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="257" t="s">
-        <v>451</v>
-      </c>
-      <c r="B88" s="257"/>
-      <c r="C88" s="257"/>
-      <c r="D88" s="257"/>
-      <c r="E88" s="257"/>
-      <c r="F88" s="257"/>
+      <c r="B88" s="256"/>
+      <c r="C88" s="256"/>
+      <c r="D88" s="256"/>
+      <c r="E88" s="256"/>
+      <c r="F88" s="256"/>
       <c r="G88" s="134"/>
       <c r="H88" s="135"/>
       <c r="I88" s="135"/>
@@ -12286,13 +12298,13 @@
     </row>
     <row r="89" spans="1:15" s="54" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="120" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B89" s="80" t="s">
         <v>239</v>
       </c>
       <c r="C89" s="81" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="D89" s="156" t="s">
         <v>229</v>
@@ -12306,28 +12318,28 @@
       <c r="I89" s="126"/>
       <c r="J89" s="126"/>
       <c r="K89" s="126"/>
-      <c r="L89" s="176" t="s">
+      <c r="L89" s="174" t="s">
         <v>86</v>
       </c>
       <c r="M89" s="173" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="N89" s="127" t="s">
         <v>411</v>
       </c>
       <c r="O89" s="128" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="90" spans="1:15" s="54" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="120" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B90" s="80" t="s">
         <v>239</v>
       </c>
       <c r="C90" s="81" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="D90" s="156" t="s">
         <v>229</v>
@@ -12341,7 +12353,7 @@
       <c r="I90" s="126"/>
       <c r="J90" s="126"/>
       <c r="K90" s="126"/>
-      <c r="L90" s="176" t="s">
+      <c r="L90" s="174" t="s">
         <v>86</v>
       </c>
       <c r="M90" s="76" t="s">
@@ -12351,18 +12363,18 @@
         <v>357</v>
       </c>
       <c r="O90" s="128" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="91" spans="1:15" s="54" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A91" s="120" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B91" s="80" t="s">
         <v>235</v>
       </c>
       <c r="C91" s="81" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="D91" s="156" t="s">
         <v>229</v>
@@ -12377,27 +12389,27 @@
       <c r="J91" s="126"/>
       <c r="K91" s="126"/>
       <c r="L91" s="112" t="s">
+        <v>457</v>
+      </c>
+      <c r="M91" s="112" t="s">
         <v>458</v>
       </c>
-      <c r="M91" s="112" t="s">
+      <c r="N91" s="76" t="s">
+        <v>86</v>
+      </c>
+      <c r="O91" s="128" t="s">
         <v>459</v>
-      </c>
-      <c r="N91" s="76" t="s">
-        <v>86</v>
-      </c>
-      <c r="O91" s="128" t="s">
-        <v>460</v>
       </c>
     </row>
     <row r="92" spans="1:15" s="54" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A92" s="120" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B92" s="80" t="s">
         <v>235</v>
       </c>
       <c r="C92" s="81" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="D92" s="156" t="s">
         <v>229</v>
@@ -12411,41 +12423,41 @@
       <c r="I92" s="126"/>
       <c r="J92" s="126"/>
       <c r="K92" s="126"/>
-      <c r="L92" s="176" t="s">
+      <c r="L92" s="174" t="s">
         <v>86</v>
       </c>
       <c r="M92" s="126" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="N92" s="76" t="s">
         <v>86</v>
       </c>
       <c r="O92" s="128" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="93" spans="1:15" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="79" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B93" s="140" t="s">
         <v>235</v>
       </c>
       <c r="C93" s="81" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="D93" s="156"/>
       <c r="E93" s="129"/>
       <c r="F93" s="130"/>
-      <c r="G93" s="179" t="s">
-        <v>464</v>
+      <c r="G93" s="177" t="s">
+        <v>463</v>
       </c>
       <c r="H93" s="126"/>
       <c r="I93" s="126"/>
       <c r="J93" s="126"/>
       <c r="K93" s="126"/>
       <c r="L93" s="112" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="M93" s="76" t="s">
         <v>86</v>
@@ -12458,14 +12470,14 @@
       </c>
     </row>
     <row r="94" spans="1:15" s="54" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="257" t="s">
-        <v>465</v>
-      </c>
-      <c r="B94" s="257"/>
-      <c r="C94" s="257"/>
-      <c r="D94" s="257"/>
-      <c r="E94" s="257"/>
-      <c r="F94" s="257"/>
+      <c r="A94" s="256" t="s">
+        <v>464</v>
+      </c>
+      <c r="B94" s="256"/>
+      <c r="C94" s="256"/>
+      <c r="D94" s="256"/>
+      <c r="E94" s="256"/>
+      <c r="F94" s="256"/>
       <c r="G94" s="134"/>
       <c r="H94" s="135"/>
       <c r="I94" s="135"/>
@@ -12478,13 +12490,13 @@
     </row>
     <row r="95" spans="1:15" s="54" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A95" s="120" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B95" s="80" t="s">
         <v>235</v>
       </c>
       <c r="C95" s="81" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="D95" s="129" t="s">
         <v>229</v>
@@ -12499,27 +12511,27 @@
       <c r="J95" s="126"/>
       <c r="K95" s="126"/>
       <c r="L95" s="126" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="M95" s="126" t="s">
         <v>271</v>
       </c>
       <c r="N95" s="127" t="s">
+        <v>467</v>
+      </c>
+      <c r="O95" s="128" t="s">
         <v>468</v>
-      </c>
-      <c r="O95" s="128" t="s">
-        <v>469</v>
       </c>
     </row>
     <row r="96" spans="1:15" s="54" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A96" s="79" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B96" s="140" t="s">
         <v>239</v>
       </c>
       <c r="C96" s="81" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="D96" s="129" t="s">
         <v>229</v>
@@ -12536,27 +12548,27 @@
       <c r="J96" s="126"/>
       <c r="K96" s="126"/>
       <c r="L96" s="112" t="s">
+        <v>470</v>
+      </c>
+      <c r="M96" s="112" t="s">
         <v>471</v>
       </c>
-      <c r="M96" s="112" t="s">
+      <c r="N96" s="127" t="s">
+        <v>467</v>
+      </c>
+      <c r="O96" s="128" t="s">
         <v>472</v>
       </c>
-      <c r="N96" s="127" t="s">
-        <v>468</v>
-      </c>
-      <c r="O96" s="128" t="s">
+    </row>
+    <row r="97" spans="1:15" s="54" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="256" t="s">
         <v>473</v>
       </c>
-    </row>
-    <row r="97" spans="1:15" s="54" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="257" t="s">
-        <v>474</v>
-      </c>
-      <c r="B97" s="257"/>
-      <c r="C97" s="257"/>
-      <c r="D97" s="257"/>
-      <c r="E97" s="257"/>
-      <c r="F97" s="257"/>
+      <c r="B97" s="256"/>
+      <c r="C97" s="256"/>
+      <c r="D97" s="256"/>
+      <c r="E97" s="256"/>
+      <c r="F97" s="256"/>
       <c r="G97" s="134"/>
       <c r="H97" s="135"/>
       <c r="I97" s="135"/>
@@ -12569,13 +12581,13 @@
     </row>
     <row r="98" spans="1:15" s="54" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A98" s="79" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B98" s="140" t="s">
         <v>235</v>
       </c>
-      <c r="C98" s="180" t="s">
-        <v>616</v>
+      <c r="C98" s="178" t="s">
+        <v>615</v>
       </c>
       <c r="D98" s="129" t="s">
         <v>229</v>
@@ -12590,27 +12602,27 @@
       <c r="J98" s="126"/>
       <c r="K98" s="126"/>
       <c r="L98" s="173" t="s">
+        <v>475</v>
+      </c>
+      <c r="M98" s="112" t="s">
         <v>476</v>
       </c>
-      <c r="M98" s="112" t="s">
+      <c r="N98" s="127" t="s">
+        <v>467</v>
+      </c>
+      <c r="O98" s="128" t="s">
         <v>477</v>
       </c>
-      <c r="N98" s="127" t="s">
-        <v>468</v>
-      </c>
-      <c r="O98" s="128" t="s">
+    </row>
+    <row r="99" spans="1:15" s="54" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="256" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="99" spans="1:15" s="54" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="257" t="s">
-        <v>479</v>
-      </c>
-      <c r="B99" s="257"/>
-      <c r="C99" s="257"/>
-      <c r="D99" s="257"/>
-      <c r="E99" s="257"/>
-      <c r="F99" s="257"/>
+      <c r="B99" s="256"/>
+      <c r="C99" s="256"/>
+      <c r="D99" s="256"/>
+      <c r="E99" s="256"/>
+      <c r="F99" s="256"/>
       <c r="G99" s="134"/>
       <c r="H99" s="135"/>
       <c r="I99" s="135"/>
@@ -12623,13 +12635,13 @@
     </row>
     <row r="100" spans="1:15" s="54" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="120" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B100" s="80" t="s">
         <v>239</v>
       </c>
       <c r="C100" s="81" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="D100" s="164" t="s">
         <v>229</v>
@@ -12644,27 +12656,27 @@
       <c r="J100" s="126"/>
       <c r="K100" s="126"/>
       <c r="L100" s="112" t="s">
-        <v>481</v>
-      </c>
-      <c r="M100" s="176" t="s">
+        <v>480</v>
+      </c>
+      <c r="M100" s="174" t="s">
         <v>86</v>
       </c>
       <c r="N100" s="127" t="s">
         <v>357</v>
       </c>
       <c r="O100" s="128" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="101" spans="1:15" s="54" customFormat="1" ht="171" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="120" t="s">
+        <v>482</v>
+      </c>
+      <c r="B101" s="80" t="s">
         <v>483</v>
       </c>
-      <c r="B101" s="80" t="s">
-        <v>484</v>
-      </c>
       <c r="C101" s="81" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="D101" s="156" t="s">
         <v>229</v>
@@ -12679,27 +12691,27 @@
       <c r="J101" s="86"/>
       <c r="K101" s="86"/>
       <c r="L101" s="112" t="s">
+        <v>484</v>
+      </c>
+      <c r="M101" s="174" t="s">
+        <v>86</v>
+      </c>
+      <c r="N101" s="127" t="s">
+        <v>467</v>
+      </c>
+      <c r="O101" s="119" t="s">
         <v>485</v>
-      </c>
-      <c r="M101" s="176" t="s">
-        <v>86</v>
-      </c>
-      <c r="N101" s="127" t="s">
-        <v>468</v>
-      </c>
-      <c r="O101" s="119" t="s">
-        <v>486</v>
       </c>
     </row>
     <row r="102" spans="1:15" s="54" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="120" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B102" s="80" t="s">
         <v>292</v>
       </c>
       <c r="C102" s="81" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="D102" s="156" t="s">
         <v>229</v>
@@ -12714,27 +12726,27 @@
       <c r="J102" s="126"/>
       <c r="K102" s="126"/>
       <c r="L102" s="112" t="s">
+        <v>487</v>
+      </c>
+      <c r="M102" s="174" t="s">
+        <v>86</v>
+      </c>
+      <c r="N102" s="127" t="s">
+        <v>467</v>
+      </c>
+      <c r="O102" s="128" t="s">
         <v>488</v>
       </c>
-      <c r="M102" s="176" t="s">
-        <v>86</v>
-      </c>
-      <c r="N102" s="127" t="s">
-        <v>468</v>
-      </c>
-      <c r="O102" s="128" t="s">
-        <v>489</v>
-      </c>
     </row>
     <row r="103" spans="1:15" s="54" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="259" t="s">
+      <c r="A103" s="258" t="s">
         <v>200</v>
       </c>
-      <c r="B103" s="259"/>
-      <c r="C103" s="259"/>
-      <c r="D103" s="259"/>
-      <c r="E103" s="259"/>
-      <c r="F103" s="259"/>
+      <c r="B103" s="258"/>
+      <c r="C103" s="258"/>
+      <c r="D103" s="258"/>
+      <c r="E103" s="258"/>
+      <c r="F103" s="258"/>
       <c r="G103" s="134"/>
       <c r="H103" s="135"/>
       <c r="I103" s="135"/>
@@ -12747,26 +12759,26 @@
     </row>
     <row r="104" spans="1:15" s="104" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="123" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B104" s="100" t="s">
         <v>235</v>
       </c>
       <c r="C104" s="101" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="D104" s="163"/>
       <c r="E104" s="132" t="s">
         <v>229</v>
       </c>
       <c r="F104" s="133"/>
-      <c r="G104" s="181"/>
+      <c r="G104" s="179"/>
       <c r="H104" s="114"/>
       <c r="I104" s="114"/>
       <c r="J104" s="114"/>
       <c r="K104" s="114"/>
       <c r="L104" s="115" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="M104" s="106" t="s">
         <v>86</v>
@@ -12780,20 +12792,20 @@
     </row>
     <row r="105" spans="1:15" s="104" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A105" s="123" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B105" s="100" t="s">
         <v>235</v>
       </c>
       <c r="C105" s="101" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D105" s="163"/>
       <c r="E105" s="132" t="s">
         <v>229</v>
       </c>
       <c r="F105" s="133"/>
-      <c r="G105" s="181"/>
+      <c r="G105" s="179"/>
       <c r="H105" s="114"/>
       <c r="I105" s="114"/>
       <c r="J105" s="114"/>
@@ -12813,7 +12825,7 @@
     </row>
     <row r="106" spans="1:15" s="104" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A106" s="123" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B106" s="100" t="s">
         <v>292</v>
@@ -12826,7 +12838,7 @@
         <v>229</v>
       </c>
       <c r="F106" s="133"/>
-      <c r="G106" s="181"/>
+      <c r="G106" s="179"/>
       <c r="H106" s="114"/>
       <c r="I106" s="114"/>
       <c r="J106" s="114"/>
@@ -12845,21 +12857,21 @@
       </c>
     </row>
     <row r="107" spans="1:15" s="104" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="182" t="s">
-        <v>496</v>
+      <c r="A107" s="180" t="s">
+        <v>495</v>
       </c>
       <c r="B107" s="100" t="s">
         <v>235</v>
       </c>
-      <c r="C107" s="183" t="s">
-        <v>497</v>
-      </c>
-      <c r="D107" s="184"/>
+      <c r="C107" s="181" t="s">
+        <v>496</v>
+      </c>
+      <c r="D107" s="182"/>
       <c r="E107" s="100" t="s">
         <v>229</v>
       </c>
-      <c r="F107" s="185"/>
-      <c r="G107" s="181"/>
+      <c r="F107" s="183"/>
+      <c r="G107" s="179"/>
       <c r="H107" s="115"/>
       <c r="I107" s="115"/>
       <c r="J107" s="115"/>
@@ -12878,14 +12890,14 @@
       </c>
     </row>
     <row r="108" spans="1:15" s="54" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="257" t="s">
+      <c r="A108" s="256" t="s">
         <v>208</v>
       </c>
-      <c r="B108" s="257"/>
-      <c r="C108" s="257"/>
-      <c r="D108" s="257"/>
-      <c r="E108" s="257"/>
-      <c r="F108" s="257"/>
+      <c r="B108" s="256"/>
+      <c r="C108" s="256"/>
+      <c r="D108" s="256"/>
+      <c r="E108" s="256"/>
+      <c r="F108" s="256"/>
       <c r="G108" s="134"/>
       <c r="H108" s="135"/>
       <c r="I108" s="135"/>
@@ -12898,26 +12910,26 @@
     </row>
     <row r="109" spans="1:15" s="104" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A109" s="123" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B109" s="100" t="s">
         <v>239</v>
       </c>
       <c r="C109" s="101" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D109" s="163"/>
       <c r="E109" s="132" t="s">
         <v>229</v>
       </c>
       <c r="F109" s="133"/>
-      <c r="G109" s="181"/>
+      <c r="G109" s="179"/>
       <c r="H109" s="114"/>
       <c r="I109" s="114"/>
       <c r="J109" s="114"/>
       <c r="K109" s="114"/>
       <c r="L109" s="115" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="M109" s="106" t="s">
         <v>86</v>
@@ -12931,20 +12943,20 @@
     </row>
     <row r="110" spans="1:15" s="104" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A110" s="99" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B110" s="100" t="s">
         <v>292</v>
       </c>
       <c r="C110" s="101" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="D110" s="163"/>
       <c r="E110" s="132" t="s">
         <v>229</v>
       </c>
       <c r="F110" s="133"/>
-      <c r="G110" s="181"/>
+      <c r="G110" s="179"/>
       <c r="H110" s="114"/>
       <c r="I110" s="114"/>
       <c r="J110" s="114"/>
@@ -12964,18 +12976,18 @@
     </row>
     <row r="111" spans="1:15" s="104" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="99" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B111" s="100"/>
       <c r="C111" s="101" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="D111" s="163"/>
       <c r="E111" s="132" t="s">
         <v>229</v>
       </c>
       <c r="F111" s="133"/>
-      <c r="G111" s="181"/>
+      <c r="G111" s="179"/>
       <c r="H111" s="114"/>
       <c r="I111" s="114"/>
       <c r="J111" s="114"/>
@@ -12995,20 +13007,20 @@
     </row>
     <row r="112" spans="1:15" s="104" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A112" s="99" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B112" s="100" t="s">
         <v>235</v>
       </c>
       <c r="C112" s="101" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="D112" s="163"/>
       <c r="E112" s="132" t="s">
         <v>229</v>
       </c>
       <c r="F112" s="133"/>
-      <c r="G112" s="181"/>
+      <c r="G112" s="179"/>
       <c r="H112" s="114"/>
       <c r="I112" s="114"/>
       <c r="J112" s="114"/>
@@ -13027,14 +13039,14 @@
       </c>
     </row>
     <row r="113" spans="1:15" s="54" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="257" t="s">
+      <c r="A113" s="256" t="s">
         <v>209</v>
       </c>
-      <c r="B113" s="257"/>
-      <c r="C113" s="257"/>
-      <c r="D113" s="257"/>
-      <c r="E113" s="257"/>
-      <c r="F113" s="257"/>
+      <c r="B113" s="256"/>
+      <c r="C113" s="256"/>
+      <c r="D113" s="256"/>
+      <c r="E113" s="256"/>
+      <c r="F113" s="256"/>
       <c r="G113" s="134"/>
       <c r="H113" s="135"/>
       <c r="I113" s="135"/>
@@ -13047,26 +13059,26 @@
     </row>
     <row r="114" spans="1:15" s="104" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A114" s="123" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B114" s="100" t="s">
         <v>239</v>
       </c>
       <c r="C114" s="101" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="D114" s="163"/>
       <c r="E114" s="132" t="s">
         <v>229</v>
       </c>
       <c r="F114" s="133"/>
-      <c r="G114" s="181"/>
+      <c r="G114" s="179"/>
       <c r="H114" s="114"/>
       <c r="I114" s="114"/>
       <c r="J114" s="114"/>
       <c r="K114" s="114"/>
       <c r="L114" s="115" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="M114" s="106" t="s">
         <v>86</v>
@@ -13080,20 +13092,20 @@
     </row>
     <row r="115" spans="1:15" s="104" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A115" s="123" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B115" s="132" t="s">
         <v>239</v>
       </c>
       <c r="C115" s="101" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D115" s="163"/>
       <c r="E115" s="132" t="s">
         <v>229</v>
       </c>
       <c r="F115" s="133"/>
-      <c r="G115" s="181"/>
+      <c r="G115" s="179"/>
       <c r="H115" s="114"/>
       <c r="I115" s="114"/>
       <c r="J115" s="114"/>
@@ -13112,21 +13124,21 @@
       </c>
     </row>
     <row r="116" spans="1:15" s="104" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A116" s="186" t="s">
-        <v>512</v>
-      </c>
-      <c r="B116" s="187" t="s">
+      <c r="A116" s="184" t="s">
+        <v>511</v>
+      </c>
+      <c r="B116" s="185" t="s">
         <v>292</v>
       </c>
-      <c r="C116" s="188" t="s">
+      <c r="C116" s="186" t="s">
         <v>267</v>
       </c>
-      <c r="D116" s="189"/>
-      <c r="E116" s="187" t="s">
+      <c r="D116" s="187"/>
+      <c r="E116" s="185" t="s">
         <v>229</v>
       </c>
-      <c r="F116" s="190"/>
-      <c r="G116" s="181"/>
+      <c r="F116" s="188"/>
+      <c r="G116" s="179"/>
       <c r="H116" s="114"/>
       <c r="I116" s="114"/>
       <c r="J116" s="114"/>

</xml_diff>

<commit_message>
auto commit @21.12.2020: 20:08:28,29
</commit_message>
<xml_diff>
--- a/Bachelorarbeit/Weckermann_ICS_and_Test Documentation.xlsx
+++ b/Bachelorarbeit/Weckermann_ICS_and_Test Documentation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Benutzer\Henry\Downloads\Abschlussarbeit_H-BRS\Bachelorarbeit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA069E23-8A57-46B4-97EB-24DB7B180606}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D72D4F33-C665-49D8-B56F-162BA3E6BBCC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="7200" yWindow="1785" windowWidth="21600" windowHeight="11385" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Conformance Statement" sheetId="1" r:id="rId1"/>
@@ -1545,15 +1545,6 @@
     <t>diff</t>
   </si>
   <si>
-    <t>TP_I_1_1_backup_factory_settings.gz
-TP_I_1_1_backup_factory_settings_2.gz
-TP_I_1_1_backup_user_settings.tar.gz
-TP_I_1_1_diff_factory_user_settings.png
-TP_I_1_1_factory_reset_cli.PNG
-TP_I_1_1_factory_reset_cli_alternative.PNG
-TP_I_1_1_factory_reset_luci.PNG</t>
-  </si>
-  <si>
     <t>Module J - Internet Protocol version 6 (IPv6)</t>
   </si>
   <si>
@@ -4530,6 +4521,15 @@
 TP_A_3_1_nmap_openwrt_udp_initialized.xml
 TP_A_3_1_nmap_openwrt_udp_initialized.txt
 TP_A_3_2_with_USB_MSD.png</t>
+  </si>
+  <si>
+    <t>TP_I_1_1_backup_factory_settings.gz
+TP_I_1_1_backup_factory_settings_2.gz
+TP_I_1_1_backup_user_settings.tar.gz
+TP_I_1_1_diff_factory_settings_user_settings.png
+TP_I_1_1_factory_reset_cli.PNG
+TP_I_1_1_factory_reset_cli_alternative.PNG
+TP_I_1_1_factory_reset_luci.PNG</t>
   </si>
 </sst>
 </file>
@@ -6069,9 +6069,108 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -6081,104 +6180,13 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="21" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="34" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -6187,16 +6195,8 @@
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="21" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="23" fillId="4" borderId="40" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="34" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -6606,19 +6606,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="215" t="s">
+      <c r="A2" s="237" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="215"/>
-      <c r="C2" s="215"/>
-      <c r="D2" s="215"/>
-      <c r="E2" s="215"/>
-      <c r="F2" s="215"/>
-      <c r="G2" s="215"/>
-      <c r="H2" s="215"/>
-      <c r="I2" s="215"/>
-      <c r="J2" s="215"/>
-      <c r="K2" s="215"/>
+      <c r="B2" s="237"/>
+      <c r="C2" s="237"/>
+      <c r="D2" s="237"/>
+      <c r="E2" s="237"/>
+      <c r="F2" s="237"/>
+      <c r="G2" s="237"/>
+      <c r="H2" s="237"/>
+      <c r="I2" s="237"/>
+      <c r="J2" s="237"/>
+      <c r="K2" s="237"/>
     </row>
     <row r="4" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6627,10 +6627,10 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="216" t="s">
+      <c r="A6" s="249" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="216"/>
+      <c r="B6" s="249"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
@@ -6645,38 +6645,38 @@
       <c r="A7" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="217" t="s">
+      <c r="B7" s="250" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="217"/>
+      <c r="C7" s="250"/>
       <c r="D7" s="7"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>621</v>
-      </c>
-      <c r="B8" s="218" t="s">
+        <v>620</v>
+      </c>
+      <c r="B8" s="251" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="218"/>
+      <c r="C8" s="251"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="218" t="s">
+      <c r="B9" s="251" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="218"/>
+      <c r="C9" s="251"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="219" t="s">
+      <c r="B10" s="243" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="219"/>
+      <c r="C10" s="243"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11" s="8"/>
@@ -6688,108 +6688,108 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="64.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="220" t="s">
+      <c r="A14" s="244" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="221"/>
+      <c r="B14" s="245"/>
     </row>
     <row r="15" spans="1:11" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="224" t="s">
+      <c r="B15" s="246" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="225"/>
-      <c r="D15" s="225"/>
-      <c r="E15" s="225"/>
-      <c r="F15" s="225"/>
-      <c r="G15" s="225"/>
-      <c r="H15" s="226"/>
+      <c r="C15" s="247"/>
+      <c r="D15" s="247"/>
+      <c r="E15" s="247"/>
+      <c r="F15" s="247"/>
+      <c r="G15" s="247"/>
+      <c r="H15" s="248"/>
     </row>
     <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="222" t="s">
+      <c r="B16" s="215" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="227"/>
-      <c r="D16" s="227"/>
-      <c r="E16" s="227"/>
-      <c r="F16" s="227"/>
-      <c r="G16" s="227"/>
-      <c r="H16" s="228"/>
+      <c r="C16" s="216"/>
+      <c r="D16" s="216"/>
+      <c r="E16" s="216"/>
+      <c r="F16" s="216"/>
+      <c r="G16" s="216"/>
+      <c r="H16" s="217"/>
     </row>
     <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="222" t="s">
+      <c r="B17" s="215" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="222"/>
-      <c r="D17" s="222"/>
-      <c r="E17" s="222"/>
-      <c r="F17" s="222"/>
-      <c r="G17" s="222"/>
-      <c r="H17" s="223"/>
+      <c r="C17" s="215"/>
+      <c r="D17" s="215"/>
+      <c r="E17" s="215"/>
+      <c r="F17" s="215"/>
+      <c r="G17" s="215"/>
+      <c r="H17" s="240"/>
     </row>
     <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="222" t="s">
+      <c r="B18" s="215" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="222"/>
-      <c r="D18" s="222"/>
-      <c r="E18" s="222"/>
-      <c r="F18" s="222"/>
-      <c r="G18" s="222"/>
-      <c r="H18" s="223"/>
+      <c r="C18" s="215"/>
+      <c r="D18" s="215"/>
+      <c r="E18" s="215"/>
+      <c r="F18" s="215"/>
+      <c r="G18" s="215"/>
+      <c r="H18" s="240"/>
     </row>
     <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="222" t="s">
+      <c r="B19" s="215" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="227"/>
-      <c r="D19" s="227"/>
-      <c r="E19" s="227"/>
-      <c r="F19" s="227"/>
-      <c r="G19" s="227"/>
-      <c r="H19" s="228"/>
+      <c r="C19" s="216"/>
+      <c r="D19" s="216"/>
+      <c r="E19" s="216"/>
+      <c r="F19" s="216"/>
+      <c r="G19" s="216"/>
+      <c r="H19" s="217"/>
     </row>
     <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="230" t="s">
+      <c r="B20" s="218" t="s">
         <v>22</v>
       </c>
-      <c r="C20" s="231"/>
-      <c r="D20" s="231"/>
-      <c r="E20" s="231"/>
-      <c r="F20" s="231"/>
-      <c r="G20" s="231"/>
-      <c r="H20" s="232"/>
+      <c r="C20" s="219"/>
+      <c r="D20" s="219"/>
+      <c r="E20" s="219"/>
+      <c r="F20" s="219"/>
+      <c r="G20" s="219"/>
+      <c r="H20" s="220"/>
     </row>
     <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="11" t="s">
-        <v>622</v>
-      </c>
-      <c r="B21" s="222" t="s">
-        <v>649</v>
-      </c>
-      <c r="C21" s="227"/>
-      <c r="D21" s="227"/>
-      <c r="E21" s="227"/>
-      <c r="F21" s="227"/>
-      <c r="G21" s="227"/>
-      <c r="H21" s="228"/>
+        <v>621</v>
+      </c>
+      <c r="B21" s="215" t="s">
+        <v>648</v>
+      </c>
+      <c r="C21" s="216"/>
+      <c r="D21" s="216"/>
+      <c r="E21" s="216"/>
+      <c r="F21" s="216"/>
+      <c r="G21" s="216"/>
+      <c r="H21" s="217"/>
     </row>
     <row r="24" spans="1:8" ht="21" x14ac:dyDescent="0.35">
       <c r="A24" s="211" t="s">
@@ -6797,70 +6797,70 @@
       </c>
     </row>
     <row r="25" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="229" t="s">
+      <c r="A25" s="242" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="229"/>
+      <c r="B25" s="242"/>
     </row>
     <row r="26" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B26" s="233" t="s">
+      <c r="B26" s="241" t="s">
         <v>13</v>
       </c>
-      <c r="C26" s="233"/>
-      <c r="D26" s="233"/>
+      <c r="C26" s="241"/>
+      <c r="D26" s="241"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="223" t="s">
+      <c r="B27" s="240" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="223"/>
-      <c r="D27" s="223"/>
+      <c r="C27" s="240"/>
+      <c r="D27" s="240"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="223" t="s">
+      <c r="B28" s="240" t="s">
         <v>28</v>
       </c>
-      <c r="C28" s="223"/>
-      <c r="D28" s="223"/>
+      <c r="C28" s="240"/>
+      <c r="D28" s="240"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="223" t="s">
+      <c r="B29" s="240" t="s">
         <v>30</v>
       </c>
-      <c r="C29" s="223"/>
-      <c r="D29" s="223"/>
+      <c r="C29" s="240"/>
+      <c r="D29" s="240"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B30" s="223" t="s">
+      <c r="B30" s="240" t="s">
         <v>32</v>
       </c>
-      <c r="C30" s="223"/>
-      <c r="D30" s="223"/>
+      <c r="C30" s="240"/>
+      <c r="D30" s="240"/>
     </row>
     <row r="31" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="B31" s="223" t="s">
+      <c r="B31" s="240" t="s">
         <v>34</v>
       </c>
-      <c r="C31" s="223"/>
-      <c r="D31" s="223"/>
+      <c r="C31" s="240"/>
+      <c r="D31" s="240"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="15"/>
@@ -6878,13 +6878,13 @@
       </c>
     </row>
     <row r="35" spans="1:11" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="215" t="s">
+      <c r="A35" s="237" t="s">
         <v>35</v>
       </c>
-      <c r="B35" s="215"/>
-      <c r="C35" s="215"/>
-      <c r="D35" s="215"/>
-      <c r="E35" s="215"/>
+      <c r="B35" s="237"/>
+      <c r="C35" s="237"/>
+      <c r="D35" s="237"/>
+      <c r="E35" s="237"/>
     </row>
     <row r="37" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="38" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6903,14 +6903,14 @@
       <c r="E38" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="F38" s="249" t="s">
-        <v>585</v>
-      </c>
-      <c r="G38" s="250"/>
-      <c r="H38" s="250"/>
-      <c r="I38" s="250"/>
-      <c r="J38" s="250"/>
-      <c r="K38" s="251"/>
+      <c r="F38" s="221" t="s">
+        <v>584</v>
+      </c>
+      <c r="G38" s="222"/>
+      <c r="H38" s="222"/>
+      <c r="I38" s="222"/>
+      <c r="J38" s="222"/>
+      <c r="K38" s="223"/>
     </row>
     <row r="39" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="14" t="s">
@@ -6928,14 +6928,14 @@
       <c r="E39" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="F39" s="222" t="s">
+      <c r="F39" s="215" t="s">
         <v>46</v>
       </c>
-      <c r="G39" s="227"/>
-      <c r="H39" s="227"/>
-      <c r="I39" s="227"/>
-      <c r="J39" s="227"/>
-      <c r="K39" s="228"/>
+      <c r="G39" s="216"/>
+      <c r="H39" s="216"/>
+      <c r="I39" s="216"/>
+      <c r="J39" s="216"/>
+      <c r="K39" s="217"/>
     </row>
     <row r="40" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="14" t="s">
@@ -6953,14 +6953,14 @@
       <c r="E40" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="F40" s="222" t="s">
+      <c r="F40" s="215" t="s">
         <v>48</v>
       </c>
-      <c r="G40" s="227"/>
-      <c r="H40" s="227"/>
-      <c r="I40" s="227"/>
-      <c r="J40" s="227"/>
-      <c r="K40" s="228"/>
+      <c r="G40" s="216"/>
+      <c r="H40" s="216"/>
+      <c r="I40" s="216"/>
+      <c r="J40" s="216"/>
+      <c r="K40" s="217"/>
     </row>
     <row r="41" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="14" t="s">
@@ -6978,12 +6978,12 @@
       <c r="E41" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="F41" s="222"/>
-      <c r="G41" s="227"/>
-      <c r="H41" s="227"/>
-      <c r="I41" s="227"/>
-      <c r="J41" s="227"/>
-      <c r="K41" s="228"/>
+      <c r="F41" s="215"/>
+      <c r="G41" s="216"/>
+      <c r="H41" s="216"/>
+      <c r="I41" s="216"/>
+      <c r="J41" s="216"/>
+      <c r="K41" s="217"/>
     </row>
     <row r="42" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="14" t="s">
@@ -7001,12 +7001,12 @@
       <c r="E42" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="F42" s="230"/>
-      <c r="G42" s="231"/>
-      <c r="H42" s="231"/>
-      <c r="I42" s="231"/>
-      <c r="J42" s="231"/>
-      <c r="K42" s="232"/>
+      <c r="F42" s="218"/>
+      <c r="G42" s="219"/>
+      <c r="H42" s="219"/>
+      <c r="I42" s="219"/>
+      <c r="J42" s="219"/>
+      <c r="K42" s="220"/>
     </row>
     <row r="43" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="14" t="s">
@@ -7024,12 +7024,12 @@
       <c r="E43" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="F43" s="222"/>
-      <c r="G43" s="227"/>
-      <c r="H43" s="227"/>
-      <c r="I43" s="227"/>
-      <c r="J43" s="227"/>
-      <c r="K43" s="228"/>
+      <c r="F43" s="215"/>
+      <c r="G43" s="216"/>
+      <c r="H43" s="216"/>
+      <c r="I43" s="216"/>
+      <c r="J43" s="216"/>
+      <c r="K43" s="217"/>
     </row>
     <row r="44" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="14" t="s">
@@ -7047,12 +7047,12 @@
       <c r="E44" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="F44" s="222"/>
-      <c r="G44" s="227"/>
-      <c r="H44" s="227"/>
-      <c r="I44" s="227"/>
-      <c r="J44" s="227"/>
-      <c r="K44" s="228"/>
+      <c r="F44" s="215"/>
+      <c r="G44" s="216"/>
+      <c r="H44" s="216"/>
+      <c r="I44" s="216"/>
+      <c r="J44" s="216"/>
+      <c r="K44" s="217"/>
     </row>
     <row r="45" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="14" t="s">
@@ -7068,16 +7068,16 @@
         <v>52</v>
       </c>
       <c r="E45" s="14" t="s">
-        <v>623</v>
-      </c>
-      <c r="F45" s="222" t="s">
+        <v>622</v>
+      </c>
+      <c r="F45" s="215" t="s">
         <v>53</v>
       </c>
-      <c r="G45" s="227"/>
-      <c r="H45" s="227"/>
-      <c r="I45" s="227"/>
-      <c r="J45" s="227"/>
-      <c r="K45" s="228"/>
+      <c r="G45" s="216"/>
+      <c r="H45" s="216"/>
+      <c r="I45" s="216"/>
+      <c r="J45" s="216"/>
+      <c r="K45" s="217"/>
     </row>
     <row r="46" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="14" t="s">
@@ -7093,14 +7093,14 @@
         <v>52</v>
       </c>
       <c r="E46" s="14" t="s">
-        <v>623</v>
-      </c>
-      <c r="F46" s="222"/>
-      <c r="G46" s="227"/>
-      <c r="H46" s="227"/>
-      <c r="I46" s="227"/>
-      <c r="J46" s="227"/>
-      <c r="K46" s="228"/>
+        <v>622</v>
+      </c>
+      <c r="F46" s="215"/>
+      <c r="G46" s="216"/>
+      <c r="H46" s="216"/>
+      <c r="I46" s="216"/>
+      <c r="J46" s="216"/>
+      <c r="K46" s="217"/>
     </row>
     <row r="47" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="14" t="s">
@@ -7116,14 +7116,14 @@
         <v>52</v>
       </c>
       <c r="E47" s="14" t="s">
-        <v>623</v>
-      </c>
-      <c r="F47" s="222"/>
-      <c r="G47" s="227"/>
-      <c r="H47" s="227"/>
-      <c r="I47" s="227"/>
-      <c r="J47" s="227"/>
-      <c r="K47" s="228"/>
+        <v>622</v>
+      </c>
+      <c r="F47" s="215"/>
+      <c r="G47" s="216"/>
+      <c r="H47" s="216"/>
+      <c r="I47" s="216"/>
+      <c r="J47" s="216"/>
+      <c r="K47" s="217"/>
     </row>
     <row r="48" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="14" t="s">
@@ -7139,14 +7139,14 @@
         <v>52</v>
       </c>
       <c r="E48" s="14" t="s">
-        <v>623</v>
-      </c>
-      <c r="F48" s="230"/>
-      <c r="G48" s="231"/>
-      <c r="H48" s="231"/>
-      <c r="I48" s="231"/>
-      <c r="J48" s="231"/>
-      <c r="K48" s="232"/>
+        <v>622</v>
+      </c>
+      <c r="F48" s="218"/>
+      <c r="G48" s="219"/>
+      <c r="H48" s="219"/>
+      <c r="I48" s="219"/>
+      <c r="J48" s="219"/>
+      <c r="K48" s="220"/>
     </row>
     <row r="49" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="14" t="s">
@@ -7162,14 +7162,14 @@
         <v>52</v>
       </c>
       <c r="E49" s="14" t="s">
-        <v>623</v>
-      </c>
-      <c r="F49" s="222"/>
-      <c r="G49" s="227"/>
-      <c r="H49" s="227"/>
-      <c r="I49" s="227"/>
-      <c r="J49" s="227"/>
-      <c r="K49" s="228"/>
+        <v>622</v>
+      </c>
+      <c r="F49" s="215"/>
+      <c r="G49" s="216"/>
+      <c r="H49" s="216"/>
+      <c r="I49" s="216"/>
+      <c r="J49" s="216"/>
+      <c r="K49" s="217"/>
     </row>
     <row r="50" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="14" t="s">
@@ -7185,14 +7185,14 @@
         <v>52</v>
       </c>
       <c r="E50" s="14" t="s">
-        <v>623</v>
-      </c>
-      <c r="F50" s="222"/>
-      <c r="G50" s="227"/>
-      <c r="H50" s="227"/>
-      <c r="I50" s="227"/>
-      <c r="J50" s="227"/>
-      <c r="K50" s="228"/>
+        <v>622</v>
+      </c>
+      <c r="F50" s="215"/>
+      <c r="G50" s="216"/>
+      <c r="H50" s="216"/>
+      <c r="I50" s="216"/>
+      <c r="J50" s="216"/>
+      <c r="K50" s="217"/>
     </row>
     <row r="51" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="14" t="s">
@@ -7210,14 +7210,14 @@
       <c r="E51" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="F51" s="222" t="s">
+      <c r="F51" s="215" t="s">
         <v>57</v>
       </c>
-      <c r="G51" s="227"/>
-      <c r="H51" s="227"/>
-      <c r="I51" s="227"/>
-      <c r="J51" s="227"/>
-      <c r="K51" s="228"/>
+      <c r="G51" s="216"/>
+      <c r="H51" s="216"/>
+      <c r="I51" s="216"/>
+      <c r="J51" s="216"/>
+      <c r="K51" s="217"/>
     </row>
     <row r="52" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="14" t="s">
@@ -7235,12 +7235,12 @@
       <c r="E52" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="F52" s="222"/>
-      <c r="G52" s="227"/>
-      <c r="H52" s="227"/>
-      <c r="I52" s="227"/>
-      <c r="J52" s="227"/>
-      <c r="K52" s="228"/>
+      <c r="F52" s="215"/>
+      <c r="G52" s="216"/>
+      <c r="H52" s="216"/>
+      <c r="I52" s="216"/>
+      <c r="J52" s="216"/>
+      <c r="K52" s="217"/>
     </row>
     <row r="53" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="14" t="s">
@@ -7258,12 +7258,12 @@
       <c r="E53" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="F53" s="222"/>
-      <c r="G53" s="227"/>
-      <c r="H53" s="227"/>
-      <c r="I53" s="227"/>
-      <c r="J53" s="227"/>
-      <c r="K53" s="228"/>
+      <c r="F53" s="215"/>
+      <c r="G53" s="216"/>
+      <c r="H53" s="216"/>
+      <c r="I53" s="216"/>
+      <c r="J53" s="216"/>
+      <c r="K53" s="217"/>
     </row>
     <row r="54" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="14" t="s">
@@ -7281,12 +7281,12 @@
       <c r="E54" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="F54" s="222"/>
-      <c r="G54" s="227"/>
-      <c r="H54" s="227"/>
-      <c r="I54" s="227"/>
-      <c r="J54" s="227"/>
-      <c r="K54" s="228"/>
+      <c r="F54" s="215"/>
+      <c r="G54" s="216"/>
+      <c r="H54" s="216"/>
+      <c r="I54" s="216"/>
+      <c r="J54" s="216"/>
+      <c r="K54" s="217"/>
     </row>
     <row r="55" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="14" t="s">
@@ -7304,12 +7304,12 @@
       <c r="E55" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="F55" s="222"/>
-      <c r="G55" s="227"/>
-      <c r="H55" s="227"/>
-      <c r="I55" s="227"/>
-      <c r="J55" s="227"/>
-      <c r="K55" s="228"/>
+      <c r="F55" s="215"/>
+      <c r="G55" s="216"/>
+      <c r="H55" s="216"/>
+      <c r="I55" s="216"/>
+      <c r="J55" s="216"/>
+      <c r="K55" s="217"/>
     </row>
     <row r="56" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="14" t="s">
@@ -7327,21 +7327,21 @@
       <c r="E56" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="F56" s="222"/>
-      <c r="G56" s="227"/>
-      <c r="H56" s="227"/>
-      <c r="I56" s="227"/>
-      <c r="J56" s="227"/>
-      <c r="K56" s="228"/>
+      <c r="F56" s="215"/>
+      <c r="G56" s="216"/>
+      <c r="H56" s="216"/>
+      <c r="I56" s="216"/>
+      <c r="J56" s="216"/>
+      <c r="K56" s="217"/>
     </row>
     <row r="59" spans="1:11" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="215" t="s">
+      <c r="A59" s="237" t="s">
         <v>58</v>
       </c>
-      <c r="B59" s="215"/>
-      <c r="C59" s="215"/>
-      <c r="D59" s="215"/>
-      <c r="E59" s="215"/>
+      <c r="B59" s="237"/>
+      <c r="C59" s="237"/>
+      <c r="D59" s="237"/>
+      <c r="E59" s="237"/>
     </row>
     <row r="60" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="61" spans="1:11" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -7452,13 +7452,13 @@
       </c>
     </row>
     <row r="70" spans="1:5" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="215" t="s">
-        <v>624</v>
-      </c>
-      <c r="B70" s="215"/>
-      <c r="C70" s="215"/>
-      <c r="D70" s="215"/>
-      <c r="E70" s="215"/>
+      <c r="A70" s="237" t="s">
+        <v>623</v>
+      </c>
+      <c r="B70" s="237"/>
+      <c r="C70" s="237"/>
+      <c r="D70" s="237"/>
+      <c r="E70" s="237"/>
     </row>
     <row r="71" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="25"/>
@@ -7471,7 +7471,7 @@
         <v>65</v>
       </c>
       <c r="C72" s="192" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="D72" s="193"/>
     </row>
@@ -7484,12 +7484,12 @@
       <c r="D73" s="196"/>
     </row>
     <row r="75" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="215" t="s">
-        <v>650</v>
-      </c>
-      <c r="B75" s="215"/>
-      <c r="C75" s="215"/>
-      <c r="D75" s="215"/>
+      <c r="A75" s="237" t="s">
+        <v>649</v>
+      </c>
+      <c r="B75" s="237"/>
+      <c r="C75" s="237"/>
+      <c r="D75" s="237"/>
       <c r="E75" s="26"/>
     </row>
     <row r="76" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -7498,16 +7498,16 @@
         <v>64</v>
       </c>
       <c r="B77" s="177" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="215" t="s">
+      <c r="A80" s="237" t="s">
         <v>67</v>
       </c>
-      <c r="B80" s="215"/>
-      <c r="C80" s="215"/>
-      <c r="D80" s="215"/>
+      <c r="B80" s="237"/>
+      <c r="C80" s="237"/>
+      <c r="D80" s="237"/>
     </row>
     <row r="82" spans="1:5" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="27" t="s">
@@ -7522,24 +7522,24 @@
     </row>
     <row r="83" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="14" t="s">
+        <v>646</v>
+      </c>
+      <c r="B83" s="14" t="s">
+        <v>651</v>
+      </c>
+      <c r="C83" s="202" t="s">
         <v>647</v>
-      </c>
-      <c r="B83" s="14" t="s">
-        <v>652</v>
-      </c>
-      <c r="C83" s="202" t="s">
-        <v>648</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="14" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="B84" s="14" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="C84" s="202" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -7587,13 +7587,13 @@
       </c>
     </row>
     <row r="91" spans="1:5" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="234" t="s">
-        <v>637</v>
-      </c>
-      <c r="B91" s="234"/>
-      <c r="C91" s="234"/>
-      <c r="D91" s="234"/>
-      <c r="E91" s="234"/>
+      <c r="A91" s="238" t="s">
+        <v>636</v>
+      </c>
+      <c r="B91" s="238"/>
+      <c r="C91" s="238"/>
+      <c r="D91" s="238"/>
+      <c r="E91" s="238"/>
     </row>
     <row r="93" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="19" t="s">
@@ -7620,7 +7620,7 @@
         <v>76</v>
       </c>
       <c r="D94" s="29" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -7634,7 +7634,7 @@
         <v>76</v>
       </c>
       <c r="D95" s="29" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
@@ -7694,10 +7694,10 @@
       </c>
     </row>
     <row r="102" spans="1:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="235" t="s">
+      <c r="A102" s="239" t="s">
         <v>78</v>
       </c>
-      <c r="B102" s="235"/>
+      <c r="B102" s="239"/>
     </row>
     <row r="103" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="104" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7714,12 +7714,12 @@
       </c>
     </row>
     <row r="108" spans="1:4" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="234" t="s">
-        <v>502</v>
-      </c>
-      <c r="B108" s="234"/>
-      <c r="C108" s="234"/>
-      <c r="D108" s="234"/>
+      <c r="A108" s="238" t="s">
+        <v>501</v>
+      </c>
+      <c r="B108" s="238"/>
+      <c r="C108" s="238"/>
+      <c r="D108" s="238"/>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
@@ -7829,12 +7829,12 @@
       <c r="B117" s="31"/>
     </row>
     <row r="120" spans="1:4" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="236" t="s">
+      <c r="A120" s="233" t="s">
         <v>86</v>
       </c>
-      <c r="B120" s="236"/>
-      <c r="C120" s="236"/>
-      <c r="D120" s="236"/>
+      <c r="B120" s="233"/>
+      <c r="C120" s="233"/>
+      <c r="D120" s="233"/>
     </row>
     <row r="121" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A121" s="9" t="s">
@@ -7935,9 +7935,9 @@
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A128" s="237"/>
-      <c r="B128" s="237"/>
-      <c r="C128" s="237"/>
+      <c r="A128" s="236"/>
+      <c r="B128" s="236"/>
+      <c r="C128" s="236"/>
     </row>
     <row r="130" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A130" s="32" t="s">
@@ -7945,12 +7945,12 @@
       </c>
     </row>
     <row r="131" spans="1:4" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="238" t="s">
-        <v>626</v>
-      </c>
-      <c r="B131" s="238"/>
-      <c r="C131" s="238"/>
-      <c r="D131" s="238"/>
+      <c r="A131" s="228" t="s">
+        <v>625</v>
+      </c>
+      <c r="B131" s="228"/>
+      <c r="C131" s="228"/>
+      <c r="D131" s="228"/>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="9" t="s">
@@ -7968,21 +7968,21 @@
         <v>91</v>
       </c>
       <c r="B133" s="20" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C133" s="21" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="20" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="B134" s="20" t="s">
         <v>92</v>
       </c>
       <c r="C134" s="21" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="135" spans="1:4" ht="150" x14ac:dyDescent="0.25">
@@ -7990,7 +7990,7 @@
         <v>93</v>
       </c>
       <c r="B135" s="20" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C135" s="21" t="s">
         <v>94</v>
@@ -8001,7 +8001,7 @@
         <v>95</v>
       </c>
       <c r="B136" s="20" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C136" s="21" t="s">
         <v>96</v>
@@ -8012,10 +8012,10 @@
         <v>97</v>
       </c>
       <c r="B137" s="20" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C137" s="21" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="138" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8023,21 +8023,21 @@
         <v>98</v>
       </c>
       <c r="B138" s="20" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C138" s="21" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="139" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A139" s="30" t="s">
+        <v>600</v>
+      </c>
+      <c r="B139" s="20" t="s">
+        <v>586</v>
+      </c>
+      <c r="C139" s="30" t="s">
         <v>601</v>
-      </c>
-      <c r="B139" s="20" t="s">
-        <v>587</v>
-      </c>
-      <c r="C139" s="30" t="s">
-        <v>602</v>
       </c>
     </row>
     <row r="141" spans="1:4" ht="21" x14ac:dyDescent="0.25">
@@ -8046,12 +8046,12 @@
       </c>
     </row>
     <row r="142" spans="1:4" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A142" s="238" t="s">
+      <c r="A142" s="228" t="s">
         <v>99</v>
       </c>
-      <c r="B142" s="238"/>
-      <c r="C142" s="238"/>
-      <c r="D142" s="238"/>
+      <c r="B142" s="228"/>
+      <c r="C142" s="228"/>
+      <c r="D142" s="228"/>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" s="9" t="s">
@@ -8087,18 +8087,18 @@
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A146" s="239" t="s">
+      <c r="A146" s="226" t="s">
         <v>107</v>
       </c>
-      <c r="B146" s="239"/>
+      <c r="B146" s="226"/>
     </row>
     <row r="148" spans="1:4" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="238" t="s">
+      <c r="A148" s="228" t="s">
         <v>108</v>
       </c>
-      <c r="B148" s="238"/>
-      <c r="C148" s="238"/>
-      <c r="D148" s="238"/>
+      <c r="B148" s="228"/>
+      <c r="C148" s="228"/>
+      <c r="D148" s="228"/>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" s="9" t="s">
@@ -8113,7 +8113,7 @@
         <v>104</v>
       </c>
       <c r="B150" s="21" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
@@ -8129,12 +8129,12 @@
       <c r="B153" s="24"/>
     </row>
     <row r="155" spans="1:4" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A155" s="236" t="s">
+      <c r="A155" s="233" t="s">
         <v>109</v>
       </c>
-      <c r="B155" s="236"/>
-      <c r="C155" s="236"/>
-      <c r="D155" s="236"/>
+      <c r="B155" s="233"/>
+      <c r="C155" s="233"/>
+      <c r="D155" s="233"/>
     </row>
     <row r="156" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A156" s="9" t="s">
@@ -8216,10 +8216,10 @@
       <c r="A162" s="35"/>
     </row>
     <row r="163" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A163" s="240" t="s">
+      <c r="A163" s="225" t="s">
         <v>113</v>
       </c>
-      <c r="B163" s="240"/>
+      <c r="B163" s="225"/>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164" s="9" t="s">
@@ -8234,7 +8234,7 @@
         <v>115</v>
       </c>
       <c r="B165" s="21" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="166" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8242,40 +8242,40 @@
         <v>116</v>
       </c>
       <c r="B166" s="21" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A167" s="239" t="s">
+      <c r="A167" s="226" t="s">
         <v>117</v>
       </c>
-      <c r="B167" s="239"/>
+      <c r="B167" s="226"/>
     </row>
     <row r="169" spans="1:7" ht="53.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A169" s="238" t="s">
+      <c r="A169" s="228" t="s">
         <v>118</v>
       </c>
-      <c r="B169" s="238"/>
-      <c r="C169" s="238"/>
-      <c r="D169" s="238"/>
+      <c r="B169" s="228"/>
+      <c r="C169" s="228"/>
+      <c r="D169" s="228"/>
     </row>
     <row r="170" spans="1:7" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A170" s="206" t="s">
         <v>119</v>
       </c>
-      <c r="B170" s="241" t="s">
+      <c r="B170" s="235" t="s">
         <v>120</v>
       </c>
-      <c r="C170" s="241"/>
-      <c r="D170" s="241"/>
+      <c r="C170" s="235"/>
+      <c r="D170" s="235"/>
     </row>
     <row r="172" spans="1:7" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A172" s="244" t="s">
+      <c r="A172" s="232" t="s">
         <v>121</v>
       </c>
-      <c r="B172" s="244"/>
-      <c r="C172" s="244"/>
-      <c r="D172" s="244"/>
+      <c r="B172" s="232"/>
+      <c r="C172" s="232"/>
+      <c r="D172" s="232"/>
     </row>
     <row r="174" spans="1:7" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A174" s="36" t="s">
@@ -8313,20 +8313,20 @@
       <c r="G176" s="15"/>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A177" s="239"/>
-      <c r="B177" s="239"/>
+      <c r="A177" s="226"/>
+      <c r="B177" s="226"/>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" s="38"/>
       <c r="B178" s="38"/>
     </row>
     <row r="179" spans="1:4" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A179" s="236" t="s">
-        <v>503</v>
-      </c>
-      <c r="B179" s="236"/>
-      <c r="C179" s="236"/>
-      <c r="D179" s="236"/>
+      <c r="A179" s="233" t="s">
+        <v>502</v>
+      </c>
+      <c r="B179" s="233"/>
+      <c r="C179" s="233"/>
+      <c r="D179" s="233"/>
     </row>
     <row r="180" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" s="9" t="s">
@@ -8367,20 +8367,20 @@
       <c r="D183" s="21"/>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A184" s="245"/>
-      <c r="B184" s="245"/>
+      <c r="A184" s="234"/>
+      <c r="B184" s="234"/>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" s="39"/>
       <c r="B185" s="39"/>
     </row>
     <row r="186" spans="1:4" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A186" s="238" t="s">
+      <c r="A186" s="228" t="s">
         <v>134</v>
       </c>
-      <c r="B186" s="238"/>
-      <c r="C186" s="238"/>
-      <c r="D186" s="238"/>
+      <c r="B186" s="228"/>
+      <c r="C186" s="228"/>
+      <c r="D186" s="228"/>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" s="9" t="s">
@@ -8392,48 +8392,48 @@
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" s="20" t="s">
+        <v>587</v>
+      </c>
+      <c r="B189" s="21" t="s">
         <v>588</v>
-      </c>
-      <c r="B189" s="21" t="s">
-        <v>589</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" s="20" t="s">
+        <v>589</v>
+      </c>
+      <c r="B190" s="21" t="s">
         <v>590</v>
-      </c>
-      <c r="B190" s="21" t="s">
-        <v>591</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" s="20" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="B191" s="21" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="192" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A192" s="20" t="s">
+        <v>591</v>
+      </c>
+      <c r="B192" s="21" t="s">
         <v>592</v>
-      </c>
-      <c r="B192" s="21" t="s">
-        <v>593</v>
       </c>
     </row>
     <row r="194" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A194" s="40" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="195" spans="1:4" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A195" s="248" t="s">
+      <c r="A195" s="229" t="s">
         <v>136</v>
       </c>
-      <c r="B195" s="248"/>
-      <c r="C195" s="248"/>
-      <c r="D195" s="248"/>
+      <c r="B195" s="229"/>
+      <c r="C195" s="229"/>
+      <c r="D195" s="229"/>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" s="41" t="s">
@@ -8445,7 +8445,7 @@
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" s="20" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="B197" s="21" t="s">
         <v>138</v>
@@ -8464,20 +8464,20 @@
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A200" s="239"/>
-      <c r="B200" s="239"/>
+      <c r="A200" s="226"/>
+      <c r="B200" s="226"/>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" s="38"/>
       <c r="B201" s="38"/>
     </row>
     <row r="202" spans="1:4" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A202" s="242" t="s">
+      <c r="A202" s="224" t="s">
         <v>141</v>
       </c>
-      <c r="B202" s="242"/>
-      <c r="C202" s="242"/>
-      <c r="D202" s="242"/>
+      <c r="B202" s="224"/>
+      <c r="C202" s="224"/>
+      <c r="D202" s="224"/>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" s="9" t="s">
@@ -8492,7 +8492,7 @@
         <v>143</v>
       </c>
       <c r="B205" s="21" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="206" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -8500,15 +8500,15 @@
         <v>144</v>
       </c>
       <c r="B206" s="21" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="207" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A207" s="20" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="B207" s="21" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="208" spans="1:4" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -8520,12 +8520,12 @@
       <c r="A210" s="43"/>
     </row>
     <row r="211" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A211" s="243" t="s">
-        <v>505</v>
-      </c>
-      <c r="B211" s="243"/>
-      <c r="C211" s="243"/>
-      <c r="D211" s="243"/>
+      <c r="A211" s="231" t="s">
+        <v>504</v>
+      </c>
+      <c r="B211" s="231"/>
+      <c r="C211" s="231"/>
+      <c r="D211" s="231"/>
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A212" s="9" t="s">
@@ -8543,7 +8543,7 @@
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A213" s="20" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B213" s="20"/>
       <c r="C213" s="20"/>
@@ -8551,7 +8551,7 @@
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A214" s="20" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B214" s="20"/>
       <c r="C214" s="20"/>
@@ -8559,7 +8559,7 @@
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A215" s="20" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B215" s="20"/>
       <c r="C215" s="20"/>
@@ -8574,12 +8574,12 @@
       <c r="B217" s="38"/>
     </row>
     <row r="218" spans="1:6" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A218" s="238" t="s">
+      <c r="A218" s="228" t="s">
         <v>145</v>
       </c>
-      <c r="B218" s="238"/>
-      <c r="C218" s="238"/>
-      <c r="D218" s="238"/>
+      <c r="B218" s="228"/>
+      <c r="C218" s="228"/>
+      <c r="D218" s="228"/>
     </row>
     <row r="219" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A219" s="207" t="s">
@@ -8590,12 +8590,12 @@
       </c>
     </row>
     <row r="221" spans="1:6" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A221" s="242" t="s">
+      <c r="A221" s="224" t="s">
         <v>148</v>
       </c>
-      <c r="B221" s="242"/>
-      <c r="C221" s="242"/>
-      <c r="D221" s="242"/>
+      <c r="B221" s="224"/>
+      <c r="C221" s="224"/>
+      <c r="D221" s="224"/>
     </row>
     <row r="222" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A222" s="207" t="s">
@@ -8615,19 +8615,19 @@
       </c>
     </row>
     <row r="225" spans="1:11" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A225" s="242" t="s">
+      <c r="A225" s="224" t="s">
         <v>151</v>
       </c>
-      <c r="B225" s="242"/>
-      <c r="C225" s="242"/>
-      <c r="D225" s="242"/>
+      <c r="B225" s="224"/>
+      <c r="C225" s="224"/>
+      <c r="D225" s="224"/>
     </row>
     <row r="226" spans="1:11" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A226" s="207" t="s">
         <v>146</v>
       </c>
       <c r="B226" s="203" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="228" spans="1:11" ht="21" x14ac:dyDescent="0.25">
@@ -8636,19 +8636,19 @@
       </c>
     </row>
     <row r="229" spans="1:11" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A229" s="242" t="s">
+      <c r="A229" s="224" t="s">
         <v>152</v>
       </c>
-      <c r="B229" s="242"/>
-      <c r="C229" s="242"/>
-      <c r="D229" s="242"/>
+      <c r="B229" s="224"/>
+      <c r="C229" s="224"/>
+      <c r="D229" s="224"/>
     </row>
     <row r="230" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A230" s="209" t="s">
         <v>146</v>
       </c>
       <c r="B230" s="192" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="C230" s="192"/>
       <c r="D230" s="192"/>
@@ -8663,14 +8663,14 @@
     <row r="231" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A231" s="210"/>
       <c r="B231" s="201" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="C231" s="15" t="s">
         <v>153</v>
       </c>
       <c r="D231" s="15"/>
       <c r="E231" s="15" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="F231" s="15"/>
       <c r="G231" s="15"/>
@@ -8695,23 +8695,23 @@
       <c r="K232" s="196"/>
     </row>
     <row r="234" spans="1:11" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A234" s="242" t="s">
+      <c r="A234" s="224" t="s">
         <v>154</v>
       </c>
-      <c r="B234" s="242"/>
-      <c r="C234" s="242"/>
-      <c r="D234" s="242"/>
+      <c r="B234" s="224"/>
+      <c r="C234" s="224"/>
+      <c r="D234" s="224"/>
     </row>
     <row r="235" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A235" s="209" t="s">
         <v>146</v>
       </c>
       <c r="B235" s="192" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="C235" s="192"/>
       <c r="D235" s="192" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="E235" s="192"/>
       <c r="F235" s="192"/>
@@ -8723,10 +8723,10 @@
       <c r="A236" s="210"/>
       <c r="B236" s="15"/>
       <c r="C236" s="15"/>
-      <c r="D236" s="247" t="s">
-        <v>644</v>
-      </c>
-      <c r="E236" s="247"/>
+      <c r="D236" s="227" t="s">
+        <v>643</v>
+      </c>
+      <c r="E236" s="227"/>
       <c r="F236" s="15"/>
       <c r="G236" s="15"/>
       <c r="H236" s="15"/>
@@ -8737,7 +8737,7 @@
       <c r="B237" s="15"/>
       <c r="C237" s="15"/>
       <c r="D237" s="15" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="E237" s="15" t="s">
         <v>155</v>
@@ -8761,35 +8761,35 @@
       <c r="I238" s="196"/>
     </row>
     <row r="240" spans="1:11" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A240" s="242" t="s">
+      <c r="A240" s="224" t="s">
         <v>157</v>
       </c>
-      <c r="B240" s="242"/>
-      <c r="C240" s="242"/>
-      <c r="D240" s="242"/>
+      <c r="B240" s="224"/>
+      <c r="C240" s="224"/>
+      <c r="D240" s="224"/>
     </row>
     <row r="241" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A241" s="207" t="s">
         <v>146</v>
       </c>
       <c r="B241" s="203" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="243" spans="1:7" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A243" s="238" t="s">
+      <c r="A243" s="228" t="s">
         <v>158</v>
       </c>
-      <c r="B243" s="238"/>
-      <c r="C243" s="238"/>
-      <c r="D243" s="238"/>
+      <c r="B243" s="228"/>
+      <c r="C243" s="228"/>
+      <c r="D243" s="228"/>
     </row>
     <row r="244" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A244" s="207" t="s">
         <v>146</v>
       </c>
       <c r="B244" s="177" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="246" spans="1:7" ht="21" x14ac:dyDescent="0.25">
@@ -8798,26 +8798,26 @@
       </c>
     </row>
     <row r="247" spans="1:7" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A247" s="242" t="s">
+      <c r="A247" s="224" t="s">
         <v>160</v>
       </c>
-      <c r="B247" s="242"/>
-      <c r="C247" s="242"/>
-      <c r="D247" s="242"/>
+      <c r="B247" s="224"/>
+      <c r="C247" s="224"/>
+      <c r="D247" s="224"/>
     </row>
     <row r="248" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A248" s="209" t="s">
         <v>146</v>
       </c>
       <c r="B248" s="192" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="C248" s="192" t="s">
         <v>57</v>
       </c>
       <c r="D248" s="192"/>
       <c r="E248" s="192" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="F248" s="192"/>
       <c r="G248" s="193"/>
@@ -8843,12 +8843,12 @@
       </c>
     </row>
     <row r="252" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A252" s="242" t="s">
+      <c r="A252" s="224" t="s">
         <v>165</v>
       </c>
-      <c r="B252" s="242"/>
-      <c r="C252" s="242"/>
-      <c r="D252" s="242"/>
+      <c r="B252" s="224"/>
+      <c r="C252" s="224"/>
+      <c r="D252" s="224"/>
     </row>
     <row r="254" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A254" s="9" t="s">
@@ -8872,7 +8872,7 @@
         <v>169</v>
       </c>
       <c r="B256" s="21" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
     <row r="257" spans="1:5" ht="231.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -8880,7 +8880,7 @@
         <v>170</v>
       </c>
       <c r="B257" s="21" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="258" spans="1:5" ht="148.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8888,11 +8888,11 @@
         <v>171</v>
       </c>
       <c r="B258" s="21" t="s">
-        <v>635</v>
-      </c>
-      <c r="C258" s="246"/>
-      <c r="D258" s="246"/>
-      <c r="E258" s="246"/>
+        <v>634</v>
+      </c>
+      <c r="C258" s="230"/>
+      <c r="D258" s="230"/>
+      <c r="E258" s="230"/>
     </row>
     <row r="259" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A259" s="38"/>
@@ -8904,10 +8904,10 @@
       </c>
     </row>
     <row r="261" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A261" s="242" t="s">
+      <c r="A261" s="224" t="s">
         <v>173</v>
       </c>
-      <c r="B261" s="242"/>
+      <c r="B261" s="224"/>
     </row>
     <row r="262" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A262" s="44"/>
@@ -8918,12 +8918,12 @@
       </c>
     </row>
     <row r="264" spans="1:5" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A264" s="242" t="s">
+      <c r="A264" s="224" t="s">
         <v>175</v>
       </c>
-      <c r="B264" s="242"/>
-      <c r="C264" s="242"/>
-      <c r="D264" s="242"/>
+      <c r="B264" s="224"/>
+      <c r="C264" s="224"/>
+      <c r="D264" s="224"/>
     </row>
     <row r="265" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A265" s="207" t="s">
@@ -8934,12 +8934,12 @@
       </c>
     </row>
     <row r="267" spans="1:5" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A267" s="242" t="s">
+      <c r="A267" s="224" t="s">
         <v>177</v>
       </c>
-      <c r="B267" s="242"/>
-      <c r="C267" s="242"/>
-      <c r="D267" s="242"/>
+      <c r="B267" s="224"/>
+      <c r="C267" s="224"/>
+      <c r="D267" s="224"/>
     </row>
     <row r="268" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A268" s="207" t="s">
@@ -8951,16 +8951,16 @@
     </row>
     <row r="269" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="270" spans="1:5" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A270" s="242" t="s">
+      <c r="A270" s="224" t="s">
         <v>178</v>
       </c>
-      <c r="B270" s="242"/>
+      <c r="B270" s="224"/>
     </row>
     <row r="271" spans="1:5" ht="59.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A271" s="242" t="s">
+      <c r="A271" s="224" t="s">
         <v>179</v>
       </c>
-      <c r="B271" s="242"/>
+      <c r="B271" s="224"/>
     </row>
     <row r="272" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A272" s="207" t="s">
@@ -8971,12 +8971,12 @@
       </c>
     </row>
     <row r="274" spans="1:7" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A274" s="240" t="s">
-        <v>508</v>
-      </c>
-      <c r="B274" s="240"/>
-      <c r="C274" s="240"/>
-      <c r="D274" s="240"/>
+      <c r="A274" s="225" t="s">
+        <v>507</v>
+      </c>
+      <c r="B274" s="225"/>
+      <c r="C274" s="225"/>
+      <c r="D274" s="225"/>
     </row>
     <row r="275" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A275" s="9" t="s">
@@ -8994,7 +8994,7 @@
     </row>
     <row r="276" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A276" s="22" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B276" s="45"/>
       <c r="C276" s="22"/>
@@ -9002,15 +9002,15 @@
     </row>
     <row r="277" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A277" s="22" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B277" s="22"/>
       <c r="C277" s="22"/>
       <c r="D277" s="23"/>
     </row>
     <row r="278" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A278" s="239"/>
-      <c r="B278" s="239"/>
+      <c r="A278" s="226"/>
+      <c r="B278" s="226"/>
     </row>
     <row r="279" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A279" s="38"/>
@@ -9035,19 +9035,19 @@
       </c>
     </row>
     <row r="284" spans="1:7" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A284" s="242" t="s">
+      <c r="A284" s="224" t="s">
         <v>184</v>
       </c>
-      <c r="B284" s="242"/>
-      <c r="C284" s="242"/>
-      <c r="D284" s="242"/>
+      <c r="B284" s="224"/>
+      <c r="C284" s="224"/>
+      <c r="D284" s="224"/>
     </row>
     <row r="285" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A285" s="207" t="s">
         <v>79</v>
       </c>
       <c r="B285" s="208" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="C285" s="208"/>
       <c r="D285" s="208"/>
@@ -9056,12 +9056,12 @@
       <c r="G285" s="177"/>
     </row>
     <row r="287" spans="1:7" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A287" s="240" t="s">
-        <v>511</v>
-      </c>
-      <c r="B287" s="240"/>
-      <c r="C287" s="240"/>
-      <c r="D287" s="240"/>
+      <c r="A287" s="225" t="s">
+        <v>510</v>
+      </c>
+      <c r="B287" s="225"/>
+      <c r="C287" s="225"/>
+      <c r="D287" s="225"/>
     </row>
     <row r="289" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A289" s="47" t="s">
@@ -9079,7 +9079,7 @@
     </row>
     <row r="290" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A290" s="22" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B290" s="22"/>
       <c r="C290" s="22"/>
@@ -9103,23 +9103,61 @@
     </row>
   </sheetData>
   <mergeCells count="88">
-    <mergeCell ref="F55:K55"/>
-    <mergeCell ref="F56:K56"/>
-    <mergeCell ref="F50:K50"/>
-    <mergeCell ref="F51:K51"/>
-    <mergeCell ref="F52:K52"/>
-    <mergeCell ref="F53:K53"/>
-    <mergeCell ref="F54:K54"/>
-    <mergeCell ref="F45:K45"/>
-    <mergeCell ref="F46:K46"/>
-    <mergeCell ref="F47:K47"/>
-    <mergeCell ref="F48:K48"/>
-    <mergeCell ref="F49:K49"/>
-    <mergeCell ref="F38:K38"/>
-    <mergeCell ref="F39:K39"/>
-    <mergeCell ref="F40:K40"/>
-    <mergeCell ref="F41:K41"/>
-    <mergeCell ref="F42:K42"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="B17:H17"/>
+    <mergeCell ref="B15:H15"/>
+    <mergeCell ref="B16:H16"/>
+    <mergeCell ref="B18:H18"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="B19:H19"/>
+    <mergeCell ref="B20:H20"/>
+    <mergeCell ref="B21:H21"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="A35:E35"/>
+    <mergeCell ref="A59:E59"/>
+    <mergeCell ref="A70:E70"/>
+    <mergeCell ref="A75:D75"/>
+    <mergeCell ref="A80:D80"/>
+    <mergeCell ref="A91:E91"/>
+    <mergeCell ref="A102:B102"/>
+    <mergeCell ref="A108:D108"/>
+    <mergeCell ref="A120:D120"/>
+    <mergeCell ref="A128:C128"/>
+    <mergeCell ref="A131:D131"/>
+    <mergeCell ref="A142:D142"/>
+    <mergeCell ref="A146:B146"/>
+    <mergeCell ref="A148:D148"/>
+    <mergeCell ref="A155:D155"/>
+    <mergeCell ref="A163:B163"/>
+    <mergeCell ref="A167:B167"/>
+    <mergeCell ref="A169:D169"/>
+    <mergeCell ref="B170:D170"/>
+    <mergeCell ref="A200:B200"/>
+    <mergeCell ref="A202:D202"/>
+    <mergeCell ref="A211:D211"/>
+    <mergeCell ref="A172:D172"/>
+    <mergeCell ref="A177:B177"/>
+    <mergeCell ref="A179:D179"/>
+    <mergeCell ref="A184:B184"/>
+    <mergeCell ref="A186:D186"/>
+    <mergeCell ref="A284:D284"/>
+    <mergeCell ref="A287:D287"/>
+    <mergeCell ref="C258:E258"/>
+    <mergeCell ref="A261:B261"/>
+    <mergeCell ref="A264:D264"/>
+    <mergeCell ref="A267:D267"/>
+    <mergeCell ref="A270:B270"/>
     <mergeCell ref="F43:K43"/>
     <mergeCell ref="F44:K44"/>
     <mergeCell ref="A271:B271"/>
@@ -9136,61 +9174,23 @@
     <mergeCell ref="A229:D229"/>
     <mergeCell ref="A234:D234"/>
     <mergeCell ref="A195:D195"/>
-    <mergeCell ref="A284:D284"/>
-    <mergeCell ref="A287:D287"/>
-    <mergeCell ref="C258:E258"/>
-    <mergeCell ref="A261:B261"/>
-    <mergeCell ref="A264:D264"/>
-    <mergeCell ref="A267:D267"/>
-    <mergeCell ref="A270:B270"/>
-    <mergeCell ref="A200:B200"/>
-    <mergeCell ref="A202:D202"/>
-    <mergeCell ref="A211:D211"/>
-    <mergeCell ref="A172:D172"/>
-    <mergeCell ref="A177:B177"/>
-    <mergeCell ref="A179:D179"/>
-    <mergeCell ref="A184:B184"/>
-    <mergeCell ref="A186:D186"/>
-    <mergeCell ref="A155:D155"/>
-    <mergeCell ref="A163:B163"/>
-    <mergeCell ref="A167:B167"/>
-    <mergeCell ref="A169:D169"/>
-    <mergeCell ref="B170:D170"/>
-    <mergeCell ref="A128:C128"/>
-    <mergeCell ref="A131:D131"/>
-    <mergeCell ref="A142:D142"/>
-    <mergeCell ref="A146:B146"/>
-    <mergeCell ref="A148:D148"/>
-    <mergeCell ref="A80:D80"/>
-    <mergeCell ref="A91:E91"/>
-    <mergeCell ref="A102:B102"/>
-    <mergeCell ref="A108:D108"/>
-    <mergeCell ref="A120:D120"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="A35:E35"/>
-    <mergeCell ref="A59:E59"/>
-    <mergeCell ref="A70:E70"/>
-    <mergeCell ref="A75:D75"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="B18:H18"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="B19:H19"/>
-    <mergeCell ref="B20:H20"/>
-    <mergeCell ref="B21:H21"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="B17:H17"/>
-    <mergeCell ref="B15:H15"/>
-    <mergeCell ref="B16:H16"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="F38:K38"/>
+    <mergeCell ref="F39:K39"/>
+    <mergeCell ref="F40:K40"/>
+    <mergeCell ref="F41:K41"/>
+    <mergeCell ref="F42:K42"/>
+    <mergeCell ref="F45:K45"/>
+    <mergeCell ref="F46:K46"/>
+    <mergeCell ref="F47:K47"/>
+    <mergeCell ref="F48:K48"/>
+    <mergeCell ref="F49:K49"/>
+    <mergeCell ref="F55:K55"/>
+    <mergeCell ref="F56:K56"/>
+    <mergeCell ref="F50:K50"/>
+    <mergeCell ref="F51:K51"/>
+    <mergeCell ref="F52:K52"/>
+    <mergeCell ref="F53:K53"/>
+    <mergeCell ref="F54:K54"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C133" r:id="rId1" display="dnsmasq, odhcpd-ipv6only_x000a_https://openwrt.org/docs/guide-user/base-system/dhcp" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -9207,10 +9207,10 @@
   </sheetPr>
   <dimension ref="A1:AMI116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A102" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="L98" sqref="L98"/>
+      <selection pane="bottomLeft" activeCell="C93" sqref="C93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9238,11 +9238,11 @@
       <c r="C1" s="52" t="s">
         <v>188</v>
       </c>
-      <c r="D1" s="252" t="s">
+      <c r="D1" s="254" t="s">
         <v>189</v>
       </c>
-      <c r="E1" s="252"/>
-      <c r="F1" s="252"/>
+      <c r="E1" s="254"/>
+      <c r="F1" s="254"/>
       <c r="G1" s="53"/>
       <c r="H1" s="53"/>
       <c r="I1" s="53"/>
@@ -9290,14 +9290,14 @@
       </c>
     </row>
     <row r="3" spans="1:19" s="54" customFormat="1" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="253" t="s">
+      <c r="A3" s="255" t="s">
         <v>206</v>
       </c>
-      <c r="B3" s="253"/>
-      <c r="C3" s="253"/>
-      <c r="D3" s="253"/>
-      <c r="E3" s="253"/>
-      <c r="F3" s="253"/>
+      <c r="B3" s="255"/>
+      <c r="C3" s="255"/>
+      <c r="D3" s="255"/>
+      <c r="E3" s="255"/>
+      <c r="F3" s="255"/>
       <c r="G3" s="62"/>
       <c r="H3" s="63"/>
       <c r="I3" s="63"/>
@@ -9316,7 +9316,7 @@
         <v>208</v>
       </c>
       <c r="C4" s="69" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D4" s="70" t="s">
         <v>202</v>
@@ -9338,13 +9338,13 @@
         <v>209</v>
       </c>
       <c r="M4" s="213" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="N4" s="77" t="s">
         <v>210</v>
       </c>
       <c r="O4" s="78" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="5" spans="1:19" s="54" customFormat="1" ht="90" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -9355,7 +9355,7 @@
         <v>212</v>
       </c>
       <c r="C5" s="81" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="D5" s="82" t="s">
         <v>202</v>
@@ -9372,7 +9372,7 @@
       <c r="J5" s="84"/>
       <c r="K5" s="85"/>
       <c r="L5" s="37" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="M5" s="86" t="s">
         <v>213</v>
@@ -9381,7 +9381,7 @@
         <v>76</v>
       </c>
       <c r="O5" s="88" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="P5" s="3"/>
       <c r="Q5" s="3"/>
@@ -9396,7 +9396,7 @@
         <v>212</v>
       </c>
       <c r="C6" s="81" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="D6" s="59" t="s">
         <v>202</v>
@@ -9422,7 +9422,7 @@
         <v>76</v>
       </c>
       <c r="O6" s="93" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="P6" s="3"/>
       <c r="Q6" s="3"/>
@@ -9437,7 +9437,7 @@
         <v>208</v>
       </c>
       <c r="C7" s="81" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="D7" s="59" t="s">
         <v>202</v>
@@ -9454,7 +9454,7 @@
       <c r="J7" s="94"/>
       <c r="K7" s="95"/>
       <c r="L7" s="37" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="M7" s="76" t="s">
         <v>76</v>
@@ -9478,7 +9478,7 @@
         <v>208</v>
       </c>
       <c r="C8" s="81" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="D8" s="59" t="s">
         <v>202</v>
@@ -9517,7 +9517,7 @@
         <v>208</v>
       </c>
       <c r="C9" s="81" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="D9" s="59" t="s">
         <v>202</v>
@@ -9532,7 +9532,7 @@
       <c r="J9" s="94"/>
       <c r="K9" s="95"/>
       <c r="L9" s="97" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="M9" s="94" t="s">
         <v>222</v>
@@ -9586,7 +9586,7 @@
         <v>208</v>
       </c>
       <c r="C11" s="81" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D11" s="59" t="s">
         <v>202</v>
@@ -9627,7 +9627,7 @@
         <v>208</v>
       </c>
       <c r="C12" s="81" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="D12" s="59" t="s">
         <v>202</v>
@@ -9648,7 +9648,7 @@
       </c>
       <c r="K12" s="86"/>
       <c r="L12" s="111" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="M12" s="94" t="s">
         <v>222</v>
@@ -9771,7 +9771,7 @@
         <v>208</v>
       </c>
       <c r="C16" s="81" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="D16" s="59" t="s">
         <v>202</v>
@@ -9812,7 +9812,7 @@
         <v>212</v>
       </c>
       <c r="C17" s="81" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="D17" s="120" t="s">
         <v>202</v>
@@ -9948,7 +9948,7 @@
         <v>212</v>
       </c>
       <c r="C21" s="81" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="D21" s="59" t="s">
         <v>202</v>
@@ -9965,16 +9965,16 @@
       <c r="J21" s="125"/>
       <c r="K21" s="125"/>
       <c r="L21" s="111" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="M21" s="76" t="s">
         <v>76</v>
       </c>
       <c r="N21" s="126" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="O21" s="127" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="22" spans="1:15" s="54" customFormat="1" ht="264" customHeight="1" x14ac:dyDescent="0.25">
@@ -9985,7 +9985,7 @@
         <v>262</v>
       </c>
       <c r="C22" s="81" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="D22" s="128" t="s">
         <v>202</v>
@@ -10007,13 +10007,13 @@
         <v>263</v>
       </c>
       <c r="M22" s="111" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="N22" s="85" t="s">
         <v>210</v>
       </c>
       <c r="O22" s="127" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="23" spans="1:15" s="54" customFormat="1" ht="117" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -10024,7 +10024,7 @@
         <v>265</v>
       </c>
       <c r="C23" s="81" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D23" s="128" t="s">
         <v>202</v>
@@ -10041,7 +10041,7 @@
       <c r="J23" s="125"/>
       <c r="K23" s="125"/>
       <c r="L23" s="111" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="M23" s="125" t="s">
         <v>213</v>
@@ -10050,7 +10050,7 @@
         <v>210</v>
       </c>
       <c r="O23" s="127" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="24" spans="1:15" s="103" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10120,14 +10120,14 @@
       </c>
     </row>
     <row r="26" spans="1:15" s="54" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="254" t="s">
+      <c r="A26" s="252" t="s">
         <v>272</v>
       </c>
-      <c r="B26" s="254"/>
-      <c r="C26" s="254"/>
-      <c r="D26" s="254"/>
-      <c r="E26" s="254"/>
-      <c r="F26" s="254"/>
+      <c r="B26" s="252"/>
+      <c r="C26" s="252"/>
+      <c r="D26" s="252"/>
+      <c r="E26" s="252"/>
+      <c r="F26" s="252"/>
       <c r="G26" s="133"/>
       <c r="H26" s="134"/>
       <c r="I26" s="134"/>
@@ -10146,7 +10146,7 @@
         <v>208</v>
       </c>
       <c r="C27" s="81" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="D27" s="128" t="s">
         <v>202</v>
@@ -10161,7 +10161,7 @@
       <c r="J27" s="86"/>
       <c r="K27" s="86"/>
       <c r="L27" s="111" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="M27" s="76" t="s">
         <v>76</v>
@@ -10181,7 +10181,7 @@
         <v>208</v>
       </c>
       <c r="C28" s="81" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="D28" s="128" t="s">
         <v>202</v>
@@ -10200,7 +10200,7 @@
       <c r="J28" s="125"/>
       <c r="K28" s="125"/>
       <c r="L28" s="190" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="M28" s="125" t="s">
         <v>213</v>
@@ -10220,7 +10220,7 @@
         <v>208</v>
       </c>
       <c r="C29" s="81" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="D29" s="128" t="s">
         <v>202</v>
@@ -10257,7 +10257,7 @@
         <v>208</v>
       </c>
       <c r="C30" s="143" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="D30" s="144"/>
       <c r="E30" s="144" t="s">
@@ -10290,7 +10290,7 @@
         <v>208</v>
       </c>
       <c r="C31" s="81" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="D31" s="128" t="s">
         <v>202</v>
@@ -10327,7 +10327,7 @@
         <v>208</v>
       </c>
       <c r="C32" s="81" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="D32" s="128" t="s">
         <v>202</v>
@@ -10362,7 +10362,7 @@
         <v>208</v>
       </c>
       <c r="C33" s="81" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="D33" s="128" t="s">
         <v>202</v>
@@ -10390,7 +10390,7 @@
         <v>382</v>
       </c>
       <c r="O33" s="127" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="Q33" s="53"/>
     </row>
@@ -10402,7 +10402,7 @@
         <v>208</v>
       </c>
       <c r="C34" s="81" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="D34" s="128" t="s">
         <v>202</v>
@@ -10432,14 +10432,14 @@
       </c>
     </row>
     <row r="35" spans="1:17" s="54" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="254" t="s">
+      <c r="A35" s="252" t="s">
         <v>288</v>
       </c>
-      <c r="B35" s="254"/>
-      <c r="C35" s="254"/>
-      <c r="D35" s="254"/>
-      <c r="E35" s="254"/>
-      <c r="F35" s="254"/>
+      <c r="B35" s="252"/>
+      <c r="C35" s="252"/>
+      <c r="D35" s="252"/>
+      <c r="E35" s="252"/>
+      <c r="F35" s="252"/>
       <c r="G35" s="133"/>
       <c r="H35" s="134"/>
       <c r="I35" s="134"/>
@@ -10458,7 +10458,7 @@
         <v>208</v>
       </c>
       <c r="C36" s="81" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="D36" s="128" t="s">
         <v>202</v>
@@ -10481,7 +10481,7 @@
         <v>291</v>
       </c>
       <c r="N36" s="126" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="O36" s="152" t="s">
         <v>292</v>
@@ -10495,7 +10495,7 @@
         <v>265</v>
       </c>
       <c r="C37" s="81" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="D37" s="128" t="s">
         <v>202</v>
@@ -10525,11 +10525,11 @@
       </c>
     </row>
     <row r="38" spans="1:17" s="54" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="255" t="s">
+      <c r="A38" s="256" t="s">
         <v>295</v>
       </c>
-      <c r="B38" s="255"/>
-      <c r="C38" s="255"/>
+      <c r="B38" s="256"/>
+      <c r="C38" s="256"/>
       <c r="D38" s="153"/>
       <c r="E38" s="153"/>
       <c r="F38" s="154"/>
@@ -10566,7 +10566,7 @@
       <c r="J39" s="125"/>
       <c r="K39" s="125"/>
       <c r="L39" s="111" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="M39" s="111" t="s">
         <v>291</v>
@@ -10586,7 +10586,7 @@
         <v>208</v>
       </c>
       <c r="C40" s="158" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="D40" s="155" t="s">
         <v>202</v>
@@ -10625,7 +10625,7 @@
         <v>212</v>
       </c>
       <c r="C41" s="81" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="D41" s="155" t="s">
         <v>202</v>
@@ -10643,13 +10643,13 @@
         <v>302</v>
       </c>
       <c r="M41" s="111" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="N41" s="126" t="s">
         <v>382</v>
       </c>
       <c r="O41" s="127" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="42" spans="1:17" s="54" customFormat="1" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -10660,7 +10660,7 @@
         <v>208</v>
       </c>
       <c r="C42" s="81" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D42" s="155" t="s">
         <v>202</v>
@@ -10728,7 +10728,7 @@
         <v>212</v>
       </c>
       <c r="C44" s="81" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="D44" s="155" t="s">
         <v>202</v>
@@ -10743,7 +10743,7 @@
       <c r="J44" s="86"/>
       <c r="K44" s="86"/>
       <c r="L44" s="213" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="M44" s="111" t="s">
         <v>213</v>
@@ -10763,7 +10763,7 @@
         <v>212</v>
       </c>
       <c r="C45" s="81" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="D45" s="155" t="s">
         <v>202</v>
@@ -10800,7 +10800,7 @@
         <v>208</v>
       </c>
       <c r="C46" s="81" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="D46" s="155" t="s">
         <v>202</v>
@@ -10815,7 +10815,7 @@
       <c r="J46" s="125"/>
       <c r="K46" s="125"/>
       <c r="L46" s="111" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="M46" s="76" t="s">
         <v>76</v>
@@ -10827,7 +10827,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="47" spans="1:17" s="103" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:17" s="103" customFormat="1" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="98" t="s">
         <v>317</v>
       </c>
@@ -10868,7 +10868,7 @@
         <v>208</v>
       </c>
       <c r="C48" s="81" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="D48" s="155" t="s">
         <v>202</v>
@@ -10883,7 +10883,7 @@
       <c r="J48" s="125"/>
       <c r="K48" s="125"/>
       <c r="L48" s="111" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="M48" s="76" t="s">
         <v>76</v>
@@ -10903,7 +10903,7 @@
         <v>208</v>
       </c>
       <c r="C49" s="81" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="D49" s="163" t="s">
         <v>202</v>
@@ -10957,7 +10957,7 @@
       <c r="J50" s="125"/>
       <c r="K50" s="125"/>
       <c r="L50" s="111" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="M50" s="111" t="s">
         <v>328</v>
@@ -11014,7 +11014,7 @@
         <v>251</v>
       </c>
       <c r="C52" s="81" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="D52" s="155" t="s">
         <v>202</v>
@@ -11049,7 +11049,7 @@
         <v>208</v>
       </c>
       <c r="C53" s="81" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="D53" s="155" t="s">
         <v>202</v>
@@ -11248,7 +11248,7 @@
         <v>353</v>
       </c>
       <c r="C59" s="81" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="D59" s="155" t="s">
         <v>202</v>
@@ -11268,7 +11268,7 @@
         <v>354</v>
       </c>
       <c r="M59" s="125" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="N59" s="126" t="s">
         <v>329</v>
@@ -11318,7 +11318,7 @@
         <v>360</v>
       </c>
       <c r="C61" s="81" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="D61" s="155" t="s">
         <v>202</v>
@@ -11338,7 +11338,7 @@
         <v>361</v>
       </c>
       <c r="M61" s="125" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="N61" s="126" t="s">
         <v>329</v>
@@ -11355,7 +11355,7 @@
         <v>208</v>
       </c>
       <c r="C62" s="81" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="D62" s="155" t="s">
         <v>202</v>
@@ -11390,7 +11390,7 @@
         <v>208</v>
       </c>
       <c r="C63" s="81" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="D63" s="155" t="s">
         <v>202</v>
@@ -11425,7 +11425,7 @@
         <v>208</v>
       </c>
       <c r="C64" s="81" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="D64" s="155" t="s">
         <v>202</v>
@@ -11495,7 +11495,7 @@
         <v>208</v>
       </c>
       <c r="C66" s="81" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="D66" s="155" t="s">
         <v>202</v>
@@ -11515,7 +11515,7 @@
         <v>374</v>
       </c>
       <c r="M66" s="125" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="N66" s="126" t="s">
         <v>329</v>
@@ -11532,7 +11532,7 @@
         <v>208</v>
       </c>
       <c r="C67" s="81" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="D67" s="155" t="s">
         <v>202</v>
@@ -11552,13 +11552,13 @@
         <v>377</v>
       </c>
       <c r="M67" s="111" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="N67" s="126" t="s">
         <v>329</v>
       </c>
       <c r="O67" s="127" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="68" spans="1:15" s="54" customFormat="1" ht="102" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -11569,7 +11569,7 @@
         <v>212</v>
       </c>
       <c r="C68" s="81" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="D68" s="155" t="s">
         <v>202</v>
@@ -11587,13 +11587,13 @@
         <v>379</v>
       </c>
       <c r="M68" s="125" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="N68" s="126" t="s">
         <v>329</v>
       </c>
       <c r="O68" s="127" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="69" spans="1:15" s="54" customFormat="1" ht="87" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -11604,7 +11604,7 @@
         <v>212</v>
       </c>
       <c r="C69" s="81" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="D69" s="155" t="s">
         <v>202</v>
@@ -11619,7 +11619,7 @@
       <c r="J69" s="125"/>
       <c r="K69" s="125"/>
       <c r="L69" s="111" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="M69" s="111" t="s">
         <v>381</v>
@@ -11632,14 +11632,14 @@
       </c>
     </row>
     <row r="70" spans="1:15" s="54" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="254" t="s">
+      <c r="A70" s="252" t="s">
         <v>384</v>
       </c>
-      <c r="B70" s="254"/>
-      <c r="C70" s="254"/>
-      <c r="D70" s="254"/>
-      <c r="E70" s="254"/>
-      <c r="F70" s="254"/>
+      <c r="B70" s="252"/>
+      <c r="C70" s="252"/>
+      <c r="D70" s="252"/>
+      <c r="E70" s="252"/>
+      <c r="F70" s="252"/>
       <c r="G70" s="133"/>
       <c r="H70" s="134"/>
       <c r="I70" s="134"/>
@@ -11658,7 +11658,7 @@
         <v>208</v>
       </c>
       <c r="C71" s="81" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="D71" s="155" t="s">
         <v>202</v>
@@ -11693,7 +11693,7 @@
         <v>208</v>
       </c>
       <c r="C72" s="81" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="D72" s="155" t="s">
         <v>202</v>
@@ -11794,7 +11794,7 @@
         <v>208</v>
       </c>
       <c r="C75" s="81" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D75" s="155" t="s">
         <v>202</v>
@@ -11809,10 +11809,10 @@
       <c r="J75" s="125"/>
       <c r="K75" s="125"/>
       <c r="L75" s="111" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="M75" s="125" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="N75" s="126" t="s">
         <v>51</v>
@@ -11829,7 +11829,7 @@
         <v>212</v>
       </c>
       <c r="C76" s="81" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="D76" s="155" t="s">
         <v>202</v>
@@ -11846,10 +11846,10 @@
       <c r="J76" s="125"/>
       <c r="K76" s="125"/>
       <c r="L76" s="111" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="M76" s="125" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="N76" s="126" t="s">
         <v>51</v>
@@ -11866,7 +11866,7 @@
         <v>265</v>
       </c>
       <c r="C77" s="81" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="D77" s="155" t="s">
         <v>202</v>
@@ -11890,7 +11890,7 @@
         <v>382</v>
       </c>
       <c r="O77" s="152" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="78" spans="1:15" s="54" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11901,7 +11901,7 @@
         <v>251</v>
       </c>
       <c r="C78" s="81" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="D78" s="155" t="s">
         <v>202</v>
@@ -11916,7 +11916,7 @@
       <c r="J78" s="125"/>
       <c r="K78" s="125"/>
       <c r="L78" s="173" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="M78" s="76" t="s">
         <v>76</v>
@@ -11936,7 +11936,7 @@
         <v>208</v>
       </c>
       <c r="C79" s="81" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="D79" s="155" t="s">
         <v>202</v>
@@ -11951,7 +11951,7 @@
       <c r="J79" s="125"/>
       <c r="K79" s="125"/>
       <c r="L79" s="111" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="M79" s="76" t="s">
         <v>76</v>
@@ -11971,7 +11971,7 @@
         <v>208</v>
       </c>
       <c r="C80" s="81" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="D80" s="150" t="s">
         <v>202</v>
@@ -12006,7 +12006,7 @@
         <v>208</v>
       </c>
       <c r="C81" s="81" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="D81" s="155" t="s">
         <v>202</v>
@@ -12021,7 +12021,7 @@
       <c r="J81" s="125"/>
       <c r="K81" s="125"/>
       <c r="L81" s="130" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="M81" s="76" t="s">
         <v>76</v>
@@ -12034,14 +12034,14 @@
       </c>
     </row>
     <row r="82" spans="1:15" s="54" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="254" t="s">
+      <c r="A82" s="252" t="s">
         <v>150</v>
       </c>
-      <c r="B82" s="254"/>
-      <c r="C82" s="254"/>
-      <c r="D82" s="254"/>
-      <c r="E82" s="254"/>
-      <c r="F82" s="254"/>
+      <c r="B82" s="252"/>
+      <c r="C82" s="252"/>
+      <c r="D82" s="252"/>
+      <c r="E82" s="252"/>
+      <c r="F82" s="252"/>
       <c r="G82" s="133"/>
       <c r="H82" s="134"/>
       <c r="I82" s="134"/>
@@ -12060,7 +12060,7 @@
         <v>208</v>
       </c>
       <c r="C83" s="81" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="D83" s="155" t="s">
         <v>202</v>
@@ -12080,7 +12080,7 @@
         <v>410</v>
       </c>
       <c r="M83" s="125" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="N83" s="126" t="s">
         <v>329</v>
@@ -12097,7 +12097,7 @@
         <v>208</v>
       </c>
       <c r="C84" s="81" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="D84" s="155" t="s">
         <v>202</v>
@@ -12132,7 +12132,7 @@
         <v>265</v>
       </c>
       <c r="C85" s="81" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="D85" s="155" t="s">
         <v>202</v>
@@ -12167,7 +12167,7 @@
         <v>208</v>
       </c>
       <c r="C86" s="81" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="D86" s="155" t="s">
         <v>202</v>
@@ -12202,7 +12202,7 @@
         <v>353</v>
       </c>
       <c r="C87" s="81" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="D87" s="155" t="s">
         <v>202</v>
@@ -12232,14 +12232,14 @@
       </c>
     </row>
     <row r="88" spans="1:15" s="54" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="254" t="s">
+      <c r="A88" s="252" t="s">
         <v>421</v>
       </c>
-      <c r="B88" s="254"/>
-      <c r="C88" s="254"/>
-      <c r="D88" s="254"/>
-      <c r="E88" s="254"/>
-      <c r="F88" s="254"/>
+      <c r="B88" s="252"/>
+      <c r="C88" s="252"/>
+      <c r="D88" s="252"/>
+      <c r="E88" s="252"/>
+      <c r="F88" s="252"/>
       <c r="G88" s="133"/>
       <c r="H88" s="134"/>
       <c r="I88" s="134"/>
@@ -12258,7 +12258,7 @@
         <v>212</v>
       </c>
       <c r="C89" s="81" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="D89" s="155" t="s">
         <v>202</v>
@@ -12293,7 +12293,7 @@
         <v>212</v>
       </c>
       <c r="C90" s="81" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="D90" s="155" t="s">
         <v>202</v>
@@ -12328,7 +12328,7 @@
         <v>208</v>
       </c>
       <c r="C91" s="81" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="D91" s="155" t="s">
         <v>202</v>
@@ -12343,7 +12343,7 @@
       <c r="J91" s="125"/>
       <c r="K91" s="125"/>
       <c r="L91" s="111" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="M91" s="111" t="s">
         <v>428</v>
@@ -12363,7 +12363,7 @@
         <v>208</v>
       </c>
       <c r="C92" s="81" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="D92" s="155" t="s">
         <v>202</v>
@@ -12381,7 +12381,7 @@
         <v>76</v>
       </c>
       <c r="M92" s="125" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="N92" s="76" t="s">
         <v>76</v>
@@ -12398,7 +12398,7 @@
         <v>208</v>
       </c>
       <c r="C93" s="81" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="D93" s="155"/>
       <c r="E93" s="128"/>
@@ -12411,7 +12411,7 @@
       <c r="J93" s="125"/>
       <c r="K93" s="125"/>
       <c r="L93" s="111" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="M93" s="76" t="s">
         <v>76</v>
@@ -12424,14 +12424,14 @@
       </c>
     </row>
     <row r="94" spans="1:15" s="54" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="254" t="s">
+      <c r="A94" s="252" t="s">
         <v>433</v>
       </c>
-      <c r="B94" s="254"/>
-      <c r="C94" s="254"/>
-      <c r="D94" s="254"/>
-      <c r="E94" s="254"/>
-      <c r="F94" s="254"/>
+      <c r="B94" s="252"/>
+      <c r="C94" s="252"/>
+      <c r="D94" s="252"/>
+      <c r="E94" s="252"/>
+      <c r="F94" s="252"/>
       <c r="G94" s="133"/>
       <c r="H94" s="134"/>
       <c r="I94" s="134"/>
@@ -12450,7 +12450,7 @@
         <v>208</v>
       </c>
       <c r="C95" s="81" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="D95" s="128" t="s">
         <v>202</v>
@@ -12485,7 +12485,7 @@
         <v>212</v>
       </c>
       <c r="C96" s="81" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="D96" s="128" t="s">
         <v>202</v>
@@ -12515,14 +12515,14 @@
       </c>
     </row>
     <row r="97" spans="1:15" s="54" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="254" t="s">
+      <c r="A97" s="252" t="s">
         <v>442</v>
       </c>
-      <c r="B97" s="254"/>
-      <c r="C97" s="254"/>
-      <c r="D97" s="254"/>
-      <c r="E97" s="254"/>
-      <c r="F97" s="254"/>
+      <c r="B97" s="252"/>
+      <c r="C97" s="252"/>
+      <c r="D97" s="252"/>
+      <c r="E97" s="252"/>
+      <c r="F97" s="252"/>
       <c r="G97" s="133"/>
       <c r="H97" s="134"/>
       <c r="I97" s="134"/>
@@ -12541,7 +12541,7 @@
         <v>208</v>
       </c>
       <c r="C98" s="176" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="D98" s="128" t="s">
         <v>202</v>
@@ -12565,18 +12565,18 @@
         <v>436</v>
       </c>
       <c r="O98" s="127" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="99" spans="1:15" s="54" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="252" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="99" spans="1:15" s="54" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="254" t="s">
-        <v>447</v>
-      </c>
-      <c r="B99" s="254"/>
-      <c r="C99" s="254"/>
-      <c r="D99" s="254"/>
-      <c r="E99" s="254"/>
-      <c r="F99" s="254"/>
+      <c r="B99" s="252"/>
+      <c r="C99" s="252"/>
+      <c r="D99" s="252"/>
+      <c r="E99" s="252"/>
+      <c r="F99" s="252"/>
       <c r="G99" s="133"/>
       <c r="H99" s="134"/>
       <c r="I99" s="134"/>
@@ -12589,13 +12589,13 @@
     </row>
     <row r="100" spans="1:15" s="54" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="119" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B100" s="80" t="s">
         <v>212</v>
       </c>
       <c r="C100" s="81" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="D100" s="163" t="s">
         <v>202</v>
@@ -12610,7 +12610,7 @@
       <c r="J100" s="125"/>
       <c r="K100" s="125"/>
       <c r="L100" s="111" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="M100" s="173" t="s">
         <v>76</v>
@@ -12619,18 +12619,18 @@
         <v>329</v>
       </c>
       <c r="O100" s="127" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="101" spans="1:15" s="54" customFormat="1" ht="171" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="119" t="s">
+        <v>449</v>
+      </c>
+      <c r="B101" s="80" t="s">
         <v>450</v>
       </c>
-      <c r="B101" s="80" t="s">
-        <v>451</v>
-      </c>
       <c r="C101" s="81" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="D101" s="155" t="s">
         <v>202</v>
@@ -12645,7 +12645,7 @@
       <c r="J101" s="86"/>
       <c r="K101" s="86"/>
       <c r="L101" s="111" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="M101" s="173" t="s">
         <v>76</v>
@@ -12654,18 +12654,18 @@
         <v>436</v>
       </c>
       <c r="O101" s="118" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="102" spans="1:15" s="54" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="119" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B102" s="80" t="s">
         <v>265</v>
       </c>
       <c r="C102" s="81" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="D102" s="155" t="s">
         <v>202</v>
@@ -12680,7 +12680,7 @@
       <c r="J102" s="125"/>
       <c r="K102" s="125"/>
       <c r="L102" s="111" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="M102" s="173" t="s">
         <v>76</v>
@@ -12689,18 +12689,18 @@
         <v>436</v>
       </c>
       <c r="O102" s="127" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="103" spans="1:15" s="54" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="256" t="s">
+      <c r="A103" s="253" t="s">
         <v>174</v>
       </c>
-      <c r="B103" s="256"/>
-      <c r="C103" s="256"/>
-      <c r="D103" s="256"/>
-      <c r="E103" s="256"/>
-      <c r="F103" s="256"/>
+      <c r="B103" s="253"/>
+      <c r="C103" s="253"/>
+      <c r="D103" s="253"/>
+      <c r="E103" s="253"/>
+      <c r="F103" s="253"/>
       <c r="G103" s="133"/>
       <c r="H103" s="134"/>
       <c r="I103" s="134"/>
@@ -12713,13 +12713,13 @@
     </row>
     <row r="104" spans="1:15" s="103" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="122" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B104" s="99" t="s">
         <v>208</v>
       </c>
       <c r="C104" s="100" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="D104" s="162"/>
       <c r="E104" s="131" t="s">
@@ -12732,7 +12732,7 @@
       <c r="J104" s="113"/>
       <c r="K104" s="113"/>
       <c r="L104" s="114" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="M104" s="105" t="s">
         <v>76</v>
@@ -12746,13 +12746,13 @@
     </row>
     <row r="105" spans="1:15" s="103" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A105" s="122" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B105" s="99" t="s">
         <v>208</v>
       </c>
       <c r="C105" s="100" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="D105" s="162"/>
       <c r="E105" s="131" t="s">
@@ -12779,7 +12779,7 @@
     </row>
     <row r="106" spans="1:15" s="103" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A106" s="122" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B106" s="99" t="s">
         <v>265</v>
@@ -12812,13 +12812,13 @@
     </row>
     <row r="107" spans="1:15" s="103" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="178" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B107" s="99" t="s">
         <v>208</v>
       </c>
       <c r="C107" s="179" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="D107" s="180"/>
       <c r="E107" s="99" t="s">
@@ -12844,14 +12844,14 @@
       </c>
     </row>
     <row r="108" spans="1:15" s="54" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="254" t="s">
+      <c r="A108" s="252" t="s">
         <v>182</v>
       </c>
-      <c r="B108" s="254"/>
-      <c r="C108" s="254"/>
-      <c r="D108" s="254"/>
-      <c r="E108" s="254"/>
-      <c r="F108" s="254"/>
+      <c r="B108" s="252"/>
+      <c r="C108" s="252"/>
+      <c r="D108" s="252"/>
+      <c r="E108" s="252"/>
+      <c r="F108" s="252"/>
       <c r="G108" s="133"/>
       <c r="H108" s="134"/>
       <c r="I108" s="134"/>
@@ -12864,13 +12864,13 @@
     </row>
     <row r="109" spans="1:15" s="103" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A109" s="122" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B109" s="99" t="s">
         <v>212</v>
       </c>
       <c r="C109" s="100" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="D109" s="162"/>
       <c r="E109" s="131" t="s">
@@ -12883,7 +12883,7 @@
       <c r="J109" s="113"/>
       <c r="K109" s="113"/>
       <c r="L109" s="114" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="M109" s="105" t="s">
         <v>76</v>
@@ -12897,13 +12897,13 @@
     </row>
     <row r="110" spans="1:15" s="103" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A110" s="98" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B110" s="99" t="s">
         <v>265</v>
       </c>
       <c r="C110" s="100" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D110" s="162"/>
       <c r="E110" s="131" t="s">
@@ -12930,11 +12930,11 @@
     </row>
     <row r="111" spans="1:15" s="103" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="98" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B111" s="99"/>
       <c r="C111" s="100" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="D111" s="162"/>
       <c r="E111" s="131" t="s">
@@ -12961,13 +12961,13 @@
     </row>
     <row r="112" spans="1:15" s="103" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A112" s="98" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B112" s="99" t="s">
         <v>208</v>
       </c>
       <c r="C112" s="100" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="D112" s="162"/>
       <c r="E112" s="131" t="s">
@@ -12993,14 +12993,14 @@
       </c>
     </row>
     <row r="113" spans="1:15" s="54" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="254" t="s">
+      <c r="A113" s="252" t="s">
         <v>183</v>
       </c>
-      <c r="B113" s="254"/>
-      <c r="C113" s="254"/>
-      <c r="D113" s="254"/>
-      <c r="E113" s="254"/>
-      <c r="F113" s="254"/>
+      <c r="B113" s="252"/>
+      <c r="C113" s="252"/>
+      <c r="D113" s="252"/>
+      <c r="E113" s="252"/>
+      <c r="F113" s="252"/>
       <c r="G113" s="133"/>
       <c r="H113" s="134"/>
       <c r="I113" s="134"/>
@@ -13013,13 +13013,13 @@
     </row>
     <row r="114" spans="1:15" s="103" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A114" s="122" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B114" s="99" t="s">
         <v>212</v>
       </c>
       <c r="C114" s="100" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="D114" s="162"/>
       <c r="E114" s="131" t="s">
@@ -13032,7 +13032,7 @@
       <c r="J114" s="113"/>
       <c r="K114" s="113"/>
       <c r="L114" s="114" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="M114" s="105" t="s">
         <v>76</v>
@@ -13046,13 +13046,13 @@
     </row>
     <row r="115" spans="1:15" s="103" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A115" s="122" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B115" s="131" t="s">
         <v>212</v>
       </c>
       <c r="C115" s="100" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="D115" s="162"/>
       <c r="E115" s="131" t="s">
@@ -13079,7 +13079,7 @@
     </row>
     <row r="116" spans="1:15" s="103" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A116" s="182" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B116" s="183" t="s">
         <v>265</v>
@@ -13113,6 +13113,11 @@
   </sheetData>
   <autoFilter ref="B1:B473" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <mergeCells count="14">
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A26:F26"/>
+    <mergeCell ref="A35:F35"/>
+    <mergeCell ref="A38:C38"/>
     <mergeCell ref="A99:F99"/>
     <mergeCell ref="A103:F103"/>
     <mergeCell ref="A108:F108"/>
@@ -13122,11 +13127,6 @@
     <mergeCell ref="A88:F88"/>
     <mergeCell ref="A94:F94"/>
     <mergeCell ref="A97:F97"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A26:F26"/>
-    <mergeCell ref="A35:F35"/>
-    <mergeCell ref="A38:C38"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="L41" r:id="rId1" display="in factory or initialized the DUT does not support HTTP over TLS. It must be noted that this feature can be added when compiling the firmware but for the DUT this feature has not been enabled while compilation. This could be because of storage concerns or reuse of other makefiles. _x000a_https://openwrt.org/docs/guide-user/services/webserver/uhttpd" xr:uid="{00000000-0004-0000-0100-000003000000}"/>

</xml_diff>

<commit_message>
auto commit @08.01.2021: 11:17:58,00
</commit_message>
<xml_diff>
--- a/Bachelorarbeit/Weckermann_ICS_and_Test Documentation.xlsx
+++ b/Bachelorarbeit/Weckermann_ICS_and_Test Documentation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Henry\Downloads\Abschlussarbeit_H-BRS\Bachelorarbeit\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Benutzer\Henry\Downloads\Abschlussarbeit_H-BRS\Bachelorarbeit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BFCC3D9-ED36-42C0-979E-67C97C124B5B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{938F0EEF-169A-4957-BBCF-C05DF1D19D68}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Conformance Statement" sheetId="1" r:id="rId1"/>
@@ -1475,15 +1475,6 @@
 dns-oarc.net</t>
   </si>
   <si>
-    <t>top-1000-websites.txt
-TP_G_3_1_ac8e72e2b2ada3b48edf1a96.et.dns-oarc.net.pdf
-analyze_pcap.py
-dns_dump.pcap
-TP_G_3_1_DNS_port_and_id_distribution_analytics.png
-TP_G_3_1_DNS_port_and_id_distribution_graph.png
-send_dns_requests.py</t>
-  </si>
-  <si>
     <t>TR.G.4</t>
   </si>
   <si>
@@ -4354,19 +4345,6 @@
     <t>The DUT offers support for IPv6 on all interfaces (LAN / WAN).</t>
   </si>
   <si>
-    <t>setup scripts:
-TP_A_19_1_dhcp.sh
-TP_A_19_1_encryption.sh
-TP_A_19_1_firewall.sh
-TP_A_19_1_full_setup.sh
-TP_A_19_1_icmp.sh
-TP_A_19_1_isolation.sh
-TP_A_19_1_network.sh
-TP_A_19_1_restriction.sh
-TP_A_19_1_wireless.sh
-TP_A_19_1_full_setup.sh</t>
-  </si>
-  <si>
     <t>Firewall rules indicated that this TP is passed. Functional testing showed that this assumption is true.</t>
   </si>
   <si>
@@ -4561,6 +4539,20 @@
 The "root" user is used in the quick start references for OpenWrt.
 The tester could not identify any other users configured on this device. 
 The FACT analysis supports this statement</t>
+  </si>
+  <si>
+    <t>analysis.txt
+analyze_pcap.py
+dns_dump.pcap
+send_dns_requests.py
+top-1000-websites.txt
+TP_G_3_1_ac8e72e2b2ada3b48edf1a96.et.dns-oarc.net.pdf
+TP_G_3_1_DNS_port_and_id_distribution_analytics.txt
+TP_G_3_1_DNS_port_and_id_distribution_graph.png</t>
+  </si>
+  <si>
+    <t>setup scripts:
+TP_A_19_1_full_setup.sh</t>
   </si>
 </sst>
 </file>
@@ -8280,18 +8272,18 @@
       <selection activeCell="D81" sqref="D81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.54296875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="62.81640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="38.81640625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="42.5703125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="62.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="38.85546875" style="3" customWidth="1"/>
     <col min="4" max="4" width="43" style="3" customWidth="1"/>
-    <col min="5" max="5" width="28.26953125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="10.7265625" style="3" customWidth="1"/>
-    <col min="7" max="16384" width="10.7265625" style="3"/>
+    <col min="5" max="5" width="28.28515625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" style="3" customWidth="1"/>
+    <col min="7" max="16384" width="10.7109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="88.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="236" t="s">
         <v>0</v>
       </c>
@@ -8306,13 +8298,13 @@
       <c r="J2" s="236"/>
       <c r="K2" s="236"/>
     </row>
-    <row r="4" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="205" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="248" t="s">
         <v>2</v>
       </c>
@@ -8327,7 +8319,7 @@
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
     </row>
-    <row r="7" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>3</v>
       </c>
@@ -8337,16 +8329,16 @@
       <c r="C7" s="249"/>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="B8" s="250" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="250"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>6</v>
       </c>
@@ -8355,7 +8347,7 @@
       </c>
       <c r="C9" s="250"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>8</v>
       </c>
@@ -8364,22 +8356,22 @@
       </c>
       <c r="C10" s="242"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
     </row>
-    <row r="13" spans="1:11" ht="21" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" ht="21" x14ac:dyDescent="0.25">
       <c r="A13" s="206" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="64.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:11" ht="64.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="243" t="s">
         <v>11</v>
       </c>
       <c r="B14" s="244"/>
     </row>
-    <row r="15" spans="1:11" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:11" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
         <v>12</v>
       </c>
@@ -8393,7 +8385,7 @@
       <c r="G15" s="246"/>
       <c r="H15" s="247"/>
     </row>
-    <row r="16" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
         <v>14</v>
       </c>
@@ -8407,7 +8399,7 @@
       <c r="G16" s="215"/>
       <c r="H16" s="216"/>
     </row>
-    <row r="17" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="11" t="s">
         <v>16</v>
       </c>
@@ -8421,7 +8413,7 @@
       <c r="G17" s="214"/>
       <c r="H17" s="239"/>
     </row>
-    <row r="18" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="11" t="s">
         <v>16</v>
       </c>
@@ -8435,7 +8427,7 @@
       <c r="G18" s="214"/>
       <c r="H18" s="239"/>
     </row>
-    <row r="19" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="11" t="s">
         <v>19</v>
       </c>
@@ -8449,7 +8441,7 @@
       <c r="G19" s="215"/>
       <c r="H19" s="216"/>
     </row>
-    <row r="20" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="12" t="s">
         <v>21</v>
       </c>
@@ -8463,12 +8455,12 @@
       <c r="G20" s="218"/>
       <c r="H20" s="219"/>
     </row>
-    <row r="21" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="11" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="B21" s="214" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="C21" s="215"/>
       <c r="D21" s="215"/>
@@ -8477,18 +8469,18 @@
       <c r="G21" s="215"/>
       <c r="H21" s="216"/>
     </row>
-    <row r="24" spans="1:8" ht="21" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:8" ht="21" x14ac:dyDescent="0.35">
       <c r="A24" s="205" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="241" t="s">
         <v>24</v>
       </c>
       <c r="B25" s="241"/>
     </row>
-    <row r="26" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>12</v>
       </c>
@@ -8498,7 +8490,7 @@
       <c r="C26" s="240"/>
       <c r="D26" s="240"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
         <v>25</v>
       </c>
@@ -8508,7 +8500,7 @@
       <c r="C27" s="239"/>
       <c r="D27" s="239"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
         <v>27</v>
       </c>
@@ -8518,7 +8510,7 @@
       <c r="C28" s="239"/>
       <c r="D28" s="239"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
         <v>29</v>
       </c>
@@ -8528,7 +8520,7 @@
       <c r="C29" s="239"/>
       <c r="D29" s="239"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
         <v>31</v>
       </c>
@@ -8538,7 +8530,7 @@
       <c r="C30" s="239"/>
       <c r="D30" s="239"/>
     </row>
-    <row r="31" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="14" t="s">
         <v>33</v>
       </c>
@@ -8548,22 +8540,22 @@
       <c r="C31" s="239"/>
       <c r="D31" s="239"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="15"/>
       <c r="B32" s="191"/>
       <c r="C32" s="191"/>
       <c r="D32" s="191"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="15"/>
       <c r="B33" s="15"/>
     </row>
-    <row r="34" spans="1:11" ht="21" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:11" ht="21" x14ac:dyDescent="0.35">
       <c r="A34" s="205" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="76.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:11" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="236" t="s">
         <v>35</v>
       </c>
@@ -8572,8 +8564,8 @@
       <c r="D35" s="236"/>
       <c r="E35" s="236"/>
     </row>
-    <row r="37" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="38" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="38" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="16" t="s">
         <v>36</v>
       </c>
@@ -8590,7 +8582,7 @@
         <v>40</v>
       </c>
       <c r="F38" s="220" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="G38" s="221"/>
       <c r="H38" s="221"/>
@@ -8598,7 +8590,7 @@
       <c r="J38" s="221"/>
       <c r="K38" s="222"/>
     </row>
-    <row r="39" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="14" t="s">
         <v>41</v>
       </c>
@@ -8623,7 +8615,7 @@
       <c r="J39" s="215"/>
       <c r="K39" s="216"/>
     </row>
-    <row r="40" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="14" t="s">
         <v>41</v>
       </c>
@@ -8648,7 +8640,7 @@
       <c r="J40" s="215"/>
       <c r="K40" s="216"/>
     </row>
-    <row r="41" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="14" t="s">
         <v>41</v>
       </c>
@@ -8671,7 +8663,7 @@
       <c r="J41" s="215"/>
       <c r="K41" s="216"/>
     </row>
-    <row r="42" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="14" t="s">
         <v>50</v>
       </c>
@@ -8694,7 +8686,7 @@
       <c r="J42" s="218"/>
       <c r="K42" s="219"/>
     </row>
-    <row r="43" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="14" t="s">
         <v>50</v>
       </c>
@@ -8717,7 +8709,7 @@
       <c r="J43" s="215"/>
       <c r="K43" s="216"/>
     </row>
-    <row r="44" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="14" t="s">
         <v>50</v>
       </c>
@@ -8740,7 +8732,7 @@
       <c r="J44" s="215"/>
       <c r="K44" s="216"/>
     </row>
-    <row r="45" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="14" t="s">
         <v>41</v>
       </c>
@@ -8754,7 +8746,7 @@
         <v>52</v>
       </c>
       <c r="E45" s="14" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="F45" s="214" t="s">
         <v>53</v>
@@ -8765,7 +8757,7 @@
       <c r="J45" s="215"/>
       <c r="K45" s="216"/>
     </row>
-    <row r="46" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="14" t="s">
         <v>41</v>
       </c>
@@ -8779,7 +8771,7 @@
         <v>52</v>
       </c>
       <c r="E46" s="14" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="F46" s="214"/>
       <c r="G46" s="215"/>
@@ -8788,7 +8780,7 @@
       <c r="J46" s="215"/>
       <c r="K46" s="216"/>
     </row>
-    <row r="47" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="14" t="s">
         <v>41</v>
       </c>
@@ -8802,7 +8794,7 @@
         <v>52</v>
       </c>
       <c r="E47" s="14" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="F47" s="214"/>
       <c r="G47" s="215"/>
@@ -8811,7 +8803,7 @@
       <c r="J47" s="215"/>
       <c r="K47" s="216"/>
     </row>
-    <row r="48" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="14" t="s">
         <v>50</v>
       </c>
@@ -8825,7 +8817,7 @@
         <v>52</v>
       </c>
       <c r="E48" s="14" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="F48" s="217"/>
       <c r="G48" s="218"/>
@@ -8834,7 +8826,7 @@
       <c r="J48" s="218"/>
       <c r="K48" s="219"/>
     </row>
-    <row r="49" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="14" t="s">
         <v>50</v>
       </c>
@@ -8848,7 +8840,7 @@
         <v>52</v>
       </c>
       <c r="E49" s="14" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="F49" s="214"/>
       <c r="G49" s="215"/>
@@ -8857,7 +8849,7 @@
       <c r="J49" s="215"/>
       <c r="K49" s="216"/>
     </row>
-    <row r="50" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="14" t="s">
         <v>50</v>
       </c>
@@ -8871,7 +8863,7 @@
         <v>52</v>
       </c>
       <c r="E50" s="14" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="F50" s="214"/>
       <c r="G50" s="215"/>
@@ -8880,7 +8872,7 @@
       <c r="J50" s="215"/>
       <c r="K50" s="216"/>
     </row>
-    <row r="51" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="14" t="s">
         <v>41</v>
       </c>
@@ -8905,7 +8897,7 @@
       <c r="J51" s="215"/>
       <c r="K51" s="216"/>
     </row>
-    <row r="52" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="14" t="s">
         <v>41</v>
       </c>
@@ -8928,7 +8920,7 @@
       <c r="J52" s="215"/>
       <c r="K52" s="216"/>
     </row>
-    <row r="53" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="14" t="s">
         <v>41</v>
       </c>
@@ -8951,7 +8943,7 @@
       <c r="J53" s="215"/>
       <c r="K53" s="216"/>
     </row>
-    <row r="54" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="14" t="s">
         <v>50</v>
       </c>
@@ -8974,7 +8966,7 @@
       <c r="J54" s="215"/>
       <c r="K54" s="216"/>
     </row>
-    <row r="55" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="14" t="s">
         <v>50</v>
       </c>
@@ -8997,7 +8989,7 @@
       <c r="J55" s="215"/>
       <c r="K55" s="216"/>
     </row>
-    <row r="56" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="14" t="s">
         <v>50</v>
       </c>
@@ -9020,7 +9012,7 @@
       <c r="J56" s="215"/>
       <c r="K56" s="216"/>
     </row>
-    <row r="59" spans="1:11" ht="57" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:11" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="236" t="s">
         <v>58</v>
       </c>
@@ -9029,8 +9021,8 @@
       <c r="D59" s="236"/>
       <c r="E59" s="236"/>
     </row>
-    <row r="60" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="61" spans="1:11" ht="44.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" spans="1:11" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
         <v>36</v>
       </c>
@@ -9044,7 +9036,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="62" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="22" t="s">
         <v>63</v>
       </c>
@@ -9058,7 +9050,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="22" t="s">
         <v>63</v>
       </c>
@@ -9072,7 +9064,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="22" t="s">
         <v>63</v>
       </c>
@@ -9086,7 +9078,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="22" t="s">
         <v>63</v>
       </c>
@@ -9100,7 +9092,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="22" t="s">
         <v>63</v>
       </c>
@@ -9114,7 +9106,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="22" t="s">
         <v>63</v>
       </c>
@@ -9128,28 +9120,28 @@
         <v>63</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="24"/>
       <c r="B68" s="24"/>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="70" spans="1:5" ht="39.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:5" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="236" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="B70" s="236"/>
       <c r="C70" s="236"/>
       <c r="D70" s="236"/>
       <c r="E70" s="236"/>
     </row>
-    <row r="71" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="25"/>
     </row>
-    <row r="72" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" s="12" t="s">
         <v>64</v>
       </c>
@@ -9157,11 +9149,11 @@
         <v>65</v>
       </c>
       <c r="C72" s="186" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="D72" s="187"/>
     </row>
-    <row r="73" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="193"/>
       <c r="B73" s="194"/>
       <c r="C73" s="189" t="s">
@@ -9169,25 +9161,25 @@
       </c>
       <c r="D73" s="190"/>
     </row>
-    <row r="75" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="236" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="B75" s="236"/>
       <c r="C75" s="236"/>
       <c r="D75" s="236"/>
       <c r="E75" s="26"/>
     </row>
-    <row r="76" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="77" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="77" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="11" t="s">
         <v>64</v>
       </c>
       <c r="B77" s="173" t="s">
-        <v>648</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="236" t="s">
         <v>67</v>
       </c>
@@ -9195,7 +9187,7 @@
       <c r="C80" s="236"/>
       <c r="D80" s="236"/>
     </row>
-    <row r="82" spans="1:5" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:5" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="27" t="s">
         <v>68</v>
       </c>
@@ -9206,29 +9198,29 @@
         <v>70</v>
       </c>
     </row>
-    <row r="83" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="14" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="B83" s="14" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="C83" s="196" t="s">
-        <v>645</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="14" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="B84" s="14" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="C84" s="196" t="s">
-        <v>645</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="198" t="s">
         <v>63</v>
       </c>
@@ -9239,7 +9231,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="198" t="s">
         <v>63</v>
       </c>
@@ -9250,7 +9242,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="198" t="s">
         <v>63</v>
       </c>
@@ -9261,7 +9253,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="198" t="s">
         <v>63</v>
       </c>
@@ -9272,16 +9264,16 @@
         <v>63</v>
       </c>
     </row>
-    <row r="91" spans="1:5" ht="39.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:5" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="237" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="B91" s="237"/>
       <c r="C91" s="237"/>
       <c r="D91" s="237"/>
       <c r="E91" s="237"/>
     </row>
-    <row r="93" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="19" t="s">
         <v>37</v>
       </c>
@@ -9295,7 +9287,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="94" spans="1:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="14" t="s">
         <v>47</v>
       </c>
@@ -9306,10 +9298,10 @@
         <v>76</v>
       </c>
       <c r="D94" s="29" t="s">
-        <v>622</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A95" s="14" t="s">
         <v>42</v>
       </c>
@@ -9320,10 +9312,10 @@
         <v>76</v>
       </c>
       <c r="D95" s="29" t="s">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="198" t="s">
         <v>63</v>
       </c>
@@ -9337,7 +9329,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="198" t="s">
         <v>63</v>
       </c>
@@ -9351,7 +9343,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="198" t="s">
         <v>63</v>
       </c>
@@ -9365,7 +9357,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="198" t="s">
         <v>63</v>
       </c>
@@ -9379,14 +9371,14 @@
         <v>63</v>
       </c>
     </row>
-    <row r="102" spans="1:4" ht="30.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="238" t="s">
         <v>78</v>
       </c>
       <c r="B102" s="238"/>
     </row>
-    <row r="103" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="104" spans="1:4" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="103" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="104" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="11" t="s">
         <v>79</v>
       </c>
@@ -9394,25 +9386,25 @@
         <v>80</v>
       </c>
     </row>
-    <row r="107" spans="1:4" ht="21" x14ac:dyDescent="0.5">
+    <row r="107" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A107" s="205" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="108" spans="1:4" ht="70.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:4" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="237" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B108" s="237"/>
       <c r="C108" s="237"/>
       <c r="D108" s="237"/>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="9" t="s">
         <v>36</v>
       </c>
@@ -9426,7 +9418,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="20" t="s">
         <v>62</v>
       </c>
@@ -9440,7 +9432,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="22" t="s">
         <v>63</v>
       </c>
@@ -9454,7 +9446,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="22" t="s">
         <v>63</v>
       </c>
@@ -9468,7 +9460,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="22" t="s">
         <v>63</v>
       </c>
@@ -9482,7 +9474,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="22" t="s">
         <v>63</v>
       </c>
@@ -9496,7 +9488,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="22" t="s">
         <v>63</v>
       </c>
@@ -9510,11 +9502,11 @@
         <v>63</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="31"/>
       <c r="B117" s="31"/>
     </row>
-    <row r="120" spans="1:4" ht="56.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:4" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="232" t="s">
         <v>86</v>
       </c>
@@ -9522,7 +9514,7 @@
       <c r="C120" s="232"/>
       <c r="D120" s="232"/>
     </row>
-    <row r="121" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="121" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A121" s="9" t="s">
         <v>36</v>
       </c>
@@ -9536,7 +9528,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="122" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="122" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A122" s="22" t="s">
         <v>63</v>
       </c>
@@ -9550,7 +9542,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="123" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="123" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A123" s="22" t="s">
         <v>63</v>
       </c>
@@ -9564,7 +9556,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="124" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="124" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A124" s="22" t="s">
         <v>63</v>
       </c>
@@ -9578,7 +9570,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="125" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="125" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A125" s="22" t="s">
         <v>63</v>
       </c>
@@ -9592,7 +9584,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="126" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="126" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A126" s="22" t="s">
         <v>63</v>
       </c>
@@ -9606,7 +9598,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="127" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="127" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A127" s="22" t="s">
         <v>63</v>
       </c>
@@ -9620,25 +9612,25 @@
         <v>63</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="235"/>
       <c r="B128" s="235"/>
       <c r="C128" s="235"/>
     </row>
-    <row r="130" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A130" s="32" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="131" spans="1:4" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:4" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="227" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="B131" s="227"/>
       <c r="C131" s="227"/>
       <c r="D131" s="227"/>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="9" t="s">
         <v>88</v>
       </c>
@@ -9649,89 +9641,89 @@
         <v>90</v>
       </c>
     </row>
-    <row r="133" spans="1:4" ht="54" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:4" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="20" t="s">
         <v>91</v>
       </c>
       <c r="B133" s="20" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="C133" s="21" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.35">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="20" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="B134" s="20" t="s">
         <v>92</v>
       </c>
       <c r="C134" s="21" t="s">
-        <v>652</v>
-      </c>
-    </row>
-    <row r="135" spans="1:4" ht="145" x14ac:dyDescent="0.35">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" ht="150" x14ac:dyDescent="0.25">
       <c r="A135" s="20" t="s">
         <v>93</v>
       </c>
       <c r="B135" s="20" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="C135" s="21" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="136" spans="1:4" ht="108.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:4" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="20" t="s">
         <v>95</v>
       </c>
       <c r="B136" s="20" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="C136" s="21" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="137" spans="1:4" ht="117" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:4" ht="117" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="20" t="s">
         <v>97</v>
       </c>
       <c r="B137" s="20" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="C137" s="21" t="s">
-        <v>603</v>
-      </c>
-    </row>
-    <row r="138" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A138" s="20" t="s">
         <v>98</v>
       </c>
       <c r="B138" s="20" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="C138" s="21" t="s">
-        <v>602</v>
-      </c>
-    </row>
-    <row r="139" spans="1:4" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A139" s="30" t="s">
+        <v>597</v>
+      </c>
+      <c r="B139" s="20" t="s">
+        <v>583</v>
+      </c>
+      <c r="C139" s="30" t="s">
         <v>598</v>
       </c>
-      <c r="B139" s="20" t="s">
-        <v>584</v>
-      </c>
-      <c r="C139" s="30" t="s">
-        <v>599</v>
-      </c>
-    </row>
-    <row r="141" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    </row>
+    <row r="141" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A141" s="32" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="142" spans="1:4" ht="38.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:4" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="227" t="s">
         <v>99</v>
       </c>
@@ -9739,7 +9731,7 @@
       <c r="C142" s="227"/>
       <c r="D142" s="227"/>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" s="9" t="s">
         <v>100</v>
       </c>
@@ -9750,7 +9742,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" s="20" t="s">
         <v>102</v>
       </c>
@@ -9761,7 +9753,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="145" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="145" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A145" s="20" t="s">
         <v>105</v>
       </c>
@@ -9772,13 +9764,13 @@
         <v>104</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" s="225" t="s">
         <v>107</v>
       </c>
       <c r="B146" s="225"/>
     </row>
-    <row r="148" spans="1:4" ht="45.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:4" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="227" t="s">
         <v>108</v>
       </c>
@@ -9786,7 +9778,7 @@
       <c r="C148" s="227"/>
       <c r="D148" s="227"/>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" s="9" t="s">
         <v>101</v>
       </c>
@@ -9794,27 +9786,27 @@
         <v>61</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" s="34" t="s">
         <v>104</v>
       </c>
       <c r="B150" s="21" t="s">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.35">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" s="20"/>
       <c r="B151" s="21"/>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" s="20"/>
       <c r="B152" s="21"/>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" s="24"/>
       <c r="B153" s="24"/>
     </row>
-    <row r="155" spans="1:4" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:4" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="232" t="s">
         <v>109</v>
       </c>
@@ -9822,7 +9814,7 @@
       <c r="C155" s="232"/>
       <c r="D155" s="232"/>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A156" s="9" t="s">
         <v>100</v>
       </c>
@@ -9836,7 +9828,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" s="22" t="s">
         <v>63</v>
       </c>
@@ -9850,7 +9842,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" s="22" t="s">
         <v>63</v>
       </c>
@@ -9864,7 +9856,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" s="22" t="s">
         <v>63</v>
       </c>
@@ -9878,7 +9870,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" s="22" t="s">
         <v>63</v>
       </c>
@@ -9892,22 +9884,22 @@
         <v>63</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161" s="24" t="s">
         <v>112</v>
       </c>
       <c r="B161" s="24"/>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162" s="35"/>
     </row>
-    <row r="163" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="224" t="s">
         <v>113</v>
       </c>
       <c r="B163" s="224"/>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164" s="9" t="s">
         <v>114</v>
       </c>
@@ -9915,29 +9907,29 @@
         <v>61</v>
       </c>
     </row>
-    <row r="165" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A165" s="20" t="s">
         <v>115</v>
       </c>
       <c r="B165" s="21" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="166" spans="1:7" ht="73" thickBot="1" x14ac:dyDescent="0.4">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A166" s="20" t="s">
         <v>116</v>
       </c>
       <c r="B166" s="21" t="s">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.35">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A167" s="225" t="s">
         <v>117</v>
       </c>
       <c r="B167" s="225"/>
     </row>
-    <row r="169" spans="1:7" ht="53.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="169" spans="1:7" ht="53.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A169" s="227" t="s">
         <v>118</v>
       </c>
@@ -9945,7 +9937,7 @@
       <c r="C169" s="227"/>
       <c r="D169" s="227"/>
     </row>
-    <row r="170" spans="1:7" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="170" spans="1:7" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A170" s="200" t="s">
         <v>119</v>
       </c>
@@ -9955,7 +9947,7 @@
       <c r="C170" s="234"/>
       <c r="D170" s="234"/>
     </row>
-    <row r="172" spans="1:7" ht="75.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:7" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="231" t="s">
         <v>121</v>
       </c>
@@ -9963,7 +9955,7 @@
       <c r="C172" s="231"/>
       <c r="D172" s="231"/>
     </row>
-    <row r="174" spans="1:7" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="174" spans="1:7" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A174" s="36" t="s">
         <v>122</v>
       </c>
@@ -9974,7 +9966,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="175" spans="1:7" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="175" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A175" s="20" t="s">
         <v>124</v>
       </c>
@@ -9986,7 +9978,7 @@
       </c>
       <c r="G175" s="15"/>
     </row>
-    <row r="176" spans="1:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="176" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A176" s="20" t="s">
         <v>127</v>
       </c>
@@ -9998,23 +9990,23 @@
       </c>
       <c r="G176" s="15"/>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" s="225"/>
       <c r="B177" s="225"/>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" s="38"/>
       <c r="B178" s="38"/>
     </row>
-    <row r="179" spans="1:4" ht="63" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:4" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" s="232" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B179" s="232"/>
       <c r="C179" s="232"/>
       <c r="D179" s="232"/>
     </row>
-    <row r="180" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" s="9" t="s">
         <v>37</v>
       </c>
@@ -10028,7 +10020,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" s="20" t="s">
         <v>131</v>
       </c>
@@ -10036,7 +10028,7 @@
       <c r="C181" s="20"/>
       <c r="D181" s="21"/>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" s="20" t="s">
         <v>132</v>
       </c>
@@ -10044,7 +10036,7 @@
       <c r="C182" s="20"/>
       <c r="D182" s="21"/>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" s="20" t="s">
         <v>133</v>
       </c>
@@ -10052,15 +10044,15 @@
       <c r="C183" s="20"/>
       <c r="D183" s="21"/>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" s="233"/>
       <c r="B184" s="233"/>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" s="39"/>
       <c r="B185" s="39"/>
     </row>
-    <row r="186" spans="1:4" ht="54.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:4" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" s="227" t="s">
         <v>134</v>
       </c>
@@ -10068,7 +10060,7 @@
       <c r="C186" s="227"/>
       <c r="D186" s="227"/>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" s="9" t="s">
         <v>135</v>
       </c>
@@ -10076,44 +10068,44 @@
         <v>61</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" s="20" t="s">
+        <v>584</v>
+      </c>
+      <c r="B189" s="21" t="s">
         <v>585</v>
       </c>
-      <c r="B189" s="21" t="s">
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A190" s="20" t="s">
         <v>586</v>
       </c>
-    </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A190" s="20" t="s">
+      <c r="B190" s="21" t="s">
         <v>587</v>
       </c>
-      <c r="B190" s="21" t="s">
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A191" s="20" t="s">
+        <v>625</v>
+      </c>
+      <c r="B191" s="21" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A192" s="20" t="s">
         <v>588</v>
       </c>
-    </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A191" s="20" t="s">
-        <v>627</v>
-      </c>
-      <c r="B191" s="21" t="s">
-        <v>626</v>
-      </c>
-    </row>
-    <row r="192" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A192" s="20" t="s">
+      <c r="B192" s="21" t="s">
         <v>589</v>
       </c>
-      <c r="B192" s="21" t="s">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="194" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    </row>
+    <row r="194" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A194" s="40" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="195" spans="1:4" ht="58.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A195" s="228" t="s">
         <v>136</v>
       </c>
@@ -10121,7 +10113,7 @@
       <c r="C195" s="228"/>
       <c r="D195" s="228"/>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" s="41" t="s">
         <v>137</v>
       </c>
@@ -10129,35 +10121,35 @@
         <v>90</v>
       </c>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" s="20" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="B197" s="21" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A198" s="20"/>
       <c r="B198" s="21" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="199" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="199" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A199" s="20"/>
       <c r="B199" s="21" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" s="225"/>
       <c r="B200" s="225"/>
     </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" s="38"/>
       <c r="B201" s="38"/>
     </row>
-    <row r="202" spans="1:4" ht="54.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:4" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A202" s="223" t="s">
         <v>141</v>
       </c>
@@ -10165,7 +10157,7 @@
       <c r="C202" s="223"/>
       <c r="D202" s="223"/>
     </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" s="9" t="s">
         <v>142</v>
       </c>
@@ -10173,47 +10165,47 @@
         <v>90</v>
       </c>
     </row>
-    <row r="205" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A205" s="20" t="s">
         <v>143</v>
       </c>
       <c r="B205" s="21" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="206" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A206" s="20" t="s">
         <v>144</v>
       </c>
       <c r="B206" s="21" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A207" s="20" t="s">
+        <v>590</v>
+      </c>
+      <c r="B207" s="21" t="s">
         <v>593</v>
       </c>
     </row>
-    <row r="207" spans="1:4" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A207" s="20" t="s">
-        <v>591</v>
-      </c>
-      <c r="B207" s="21" t="s">
-        <v>594</v>
-      </c>
-    </row>
-    <row r="208" spans="1:4" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A209"/>
       <c r="B209"/>
     </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A210" s="43"/>
     </row>
-    <row r="211" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A211" s="230" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B211" s="230"/>
       <c r="C211" s="230"/>
       <c r="D211" s="230"/>
     </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A212" s="9" t="s">
         <v>37</v>
       </c>
@@ -10227,39 +10219,39 @@
         <v>137</v>
       </c>
     </row>
-    <row r="213" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A213" s="20" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B213" s="20"/>
       <c r="C213" s="20"/>
       <c r="D213" s="21"/>
     </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A214" s="20" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B214" s="20"/>
       <c r="C214" s="20"/>
       <c r="D214" s="21"/>
     </row>
-    <row r="215" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A215" s="20" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B215" s="20"/>
       <c r="C215" s="20"/>
       <c r="D215" s="21"/>
     </row>
-    <row r="216" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A216" s="24"/>
       <c r="B216" s="24"/>
     </row>
-    <row r="217" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A217" s="38"/>
       <c r="B217" s="38"/>
     </row>
-    <row r="218" spans="1:6" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="218" spans="1:6" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A218" s="227" t="s">
         <v>145</v>
       </c>
@@ -10267,7 +10259,7 @@
       <c r="C218" s="227"/>
       <c r="D218" s="227"/>
     </row>
-    <row r="219" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="219" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A219" s="201" t="s">
         <v>146</v>
       </c>
@@ -10275,7 +10267,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="221" spans="1:6" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="221" spans="1:6" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A221" s="223" t="s">
         <v>148</v>
       </c>
@@ -10283,7 +10275,7 @@
       <c r="C221" s="223"/>
       <c r="D221" s="223"/>
     </row>
-    <row r="222" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="222" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A222" s="201" t="s">
         <v>146</v>
       </c>
@@ -10295,12 +10287,12 @@
       <c r="E222" s="202"/>
       <c r="F222" s="173"/>
     </row>
-    <row r="224" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A224" s="40" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="225" spans="1:11" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="225" spans="1:11" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A225" s="223" t="s">
         <v>151</v>
       </c>
@@ -10308,20 +10300,20 @@
       <c r="C225" s="223"/>
       <c r="D225" s="223"/>
     </row>
-    <row r="226" spans="1:11" ht="87.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="226" spans="1:11" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A226" s="201" t="s">
         <v>146</v>
       </c>
       <c r="B226" s="197" t="s">
-        <v>629</v>
-      </c>
-    </row>
-    <row r="228" spans="1:11" ht="21" x14ac:dyDescent="0.35">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="228" spans="1:11" ht="21" x14ac:dyDescent="0.25">
       <c r="A228" s="40" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="229" spans="1:11" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="229" spans="1:11" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A229" s="223" t="s">
         <v>152</v>
       </c>
@@ -10329,12 +10321,12 @@
       <c r="C229" s="223"/>
       <c r="D229" s="223"/>
     </row>
-    <row r="230" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A230" s="203" t="s">
         <v>146</v>
       </c>
       <c r="B230" s="186" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="C230" s="186"/>
       <c r="D230" s="186"/>
@@ -10346,17 +10338,17 @@
       <c r="J230" s="186"/>
       <c r="K230" s="187"/>
     </row>
-    <row r="231" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A231" s="204"/>
       <c r="B231" s="195" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="C231" s="15" t="s">
         <v>153</v>
       </c>
       <c r="D231" s="15"/>
       <c r="E231" s="15" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="F231" s="15"/>
       <c r="G231" s="15"/>
@@ -10365,7 +10357,7 @@
       <c r="J231" s="15"/>
       <c r="K231" s="188"/>
     </row>
-    <row r="232" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="232" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A232" s="193"/>
       <c r="B232" s="189"/>
       <c r="C232" s="189" t="s">
@@ -10380,7 +10372,7 @@
       <c r="J232" s="189"/>
       <c r="K232" s="190"/>
     </row>
-    <row r="234" spans="1:11" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="234" spans="1:11" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A234" s="223" t="s">
         <v>154</v>
       </c>
@@ -10388,16 +10380,16 @@
       <c r="C234" s="223"/>
       <c r="D234" s="223"/>
     </row>
-    <row r="235" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A235" s="203" t="s">
         <v>146</v>
       </c>
       <c r="B235" s="186" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="C235" s="186"/>
       <c r="D235" s="186" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="E235" s="186"/>
       <c r="F235" s="186"/>
@@ -10405,12 +10397,12 @@
       <c r="H235" s="186"/>
       <c r="I235" s="187"/>
     </row>
-    <row r="236" spans="1:11" ht="144.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:11" ht="144.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A236" s="204"/>
       <c r="B236" s="15"/>
       <c r="C236" s="15"/>
       <c r="D236" s="226" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="E236" s="226"/>
       <c r="F236" s="15"/>
@@ -10418,12 +10410,12 @@
       <c r="H236" s="15"/>
       <c r="I236" s="188"/>
     </row>
-    <row r="237" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A237" s="204"/>
       <c r="B237" s="15"/>
       <c r="C237" s="15"/>
       <c r="D237" s="15" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="E237" s="15" t="s">
         <v>155</v>
@@ -10433,7 +10425,7 @@
       <c r="H237" s="15"/>
       <c r="I237" s="188"/>
     </row>
-    <row r="238" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="238" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A238" s="193"/>
       <c r="B238" s="189"/>
       <c r="C238" s="189"/>
@@ -10446,7 +10438,7 @@
       <c r="H238" s="189"/>
       <c r="I238" s="190"/>
     </row>
-    <row r="240" spans="1:11" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="240" spans="1:11" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A240" s="223" t="s">
         <v>157</v>
       </c>
@@ -10454,15 +10446,15 @@
       <c r="C240" s="223"/>
       <c r="D240" s="223"/>
     </row>
-    <row r="241" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="241" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A241" s="201" t="s">
         <v>146</v>
       </c>
       <c r="B241" s="197" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="243" spans="1:7" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="243" spans="1:7" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A243" s="227" t="s">
         <v>158</v>
       </c>
@@ -10470,20 +10462,20 @@
       <c r="C243" s="227"/>
       <c r="D243" s="227"/>
     </row>
-    <row r="244" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="244" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A244" s="201" t="s">
         <v>146</v>
       </c>
       <c r="B244" s="173" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="246" spans="1:7" ht="21" x14ac:dyDescent="0.35">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="246" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A246" s="40" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="247" spans="1:7" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="247" spans="1:7" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A247" s="223" t="s">
         <v>160</v>
       </c>
@@ -10491,24 +10483,24 @@
       <c r="C247" s="223"/>
       <c r="D247" s="223"/>
     </row>
-    <row r="248" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A248" s="203" t="s">
         <v>146</v>
       </c>
       <c r="B248" s="186" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="C248" s="186" t="s">
         <v>57</v>
       </c>
       <c r="D248" s="186"/>
       <c r="E248" s="186" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="F248" s="186"/>
       <c r="G248" s="187"/>
     </row>
-    <row r="249" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="249" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A249" s="193"/>
       <c r="B249" s="189" t="s">
         <v>161</v>
@@ -10523,12 +10515,12 @@
       <c r="F249" s="189"/>
       <c r="G249" s="190"/>
     </row>
-    <row r="251" spans="1:7" ht="21" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A251" s="40" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="252" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A252" s="223" t="s">
         <v>165</v>
       </c>
@@ -10536,7 +10528,7 @@
       <c r="C252" s="223"/>
       <c r="D252" s="223"/>
     </row>
-    <row r="254" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A254" s="9" t="s">
         <v>166</v>
       </c>
@@ -10544,7 +10536,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="255" spans="1:7" ht="94.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:7" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A255" s="20" t="s">
         <v>167</v>
       </c>
@@ -10553,57 +10545,57 @@
       </c>
       <c r="C255" s="2"/>
     </row>
-    <row r="256" spans="1:7" ht="106.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:7" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A256" s="20" t="s">
         <v>169</v>
       </c>
       <c r="B256" s="21" t="s">
-        <v>631</v>
-      </c>
-    </row>
-    <row r="257" spans="1:5" ht="231.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="257" spans="1:5" ht="231.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A257" s="20" t="s">
         <v>170</v>
       </c>
       <c r="B257" s="21" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="258" spans="1:5" ht="148.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="258" spans="1:5" ht="148.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A258" s="20" t="s">
         <v>171</v>
       </c>
       <c r="B258" s="21" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="C258" s="229"/>
       <c r="D258" s="229"/>
       <c r="E258" s="229"/>
     </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A259" s="38"/>
       <c r="B259" s="38"/>
     </row>
-    <row r="260" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A260" s="40" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="261" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A261" s="223" t="s">
         <v>173</v>
       </c>
       <c r="B261" s="223"/>
     </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A262" s="44"/>
     </row>
-    <row r="263" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A263" s="40" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="264" spans="1:5" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="264" spans="1:5" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A264" s="223" t="s">
         <v>175</v>
       </c>
@@ -10611,7 +10603,7 @@
       <c r="C264" s="223"/>
       <c r="D264" s="223"/>
     </row>
-    <row r="265" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="265" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A265" s="201" t="s">
         <v>79</v>
       </c>
@@ -10619,7 +10611,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="267" spans="1:5" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="267" spans="1:5" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A267" s="223" t="s">
         <v>177</v>
       </c>
@@ -10627,7 +10619,7 @@
       <c r="C267" s="223"/>
       <c r="D267" s="223"/>
     </row>
-    <row r="268" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="268" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A268" s="201" t="s">
         <v>79</v>
       </c>
@@ -10635,20 +10627,20 @@
         <v>176</v>
       </c>
     </row>
-    <row r="269" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="270" spans="1:5" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="270" spans="1:5" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A270" s="223" t="s">
         <v>178</v>
       </c>
       <c r="B270" s="223"/>
     </row>
-    <row r="271" spans="1:5" ht="59.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="271" spans="1:5" ht="59.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A271" s="223" t="s">
         <v>179</v>
       </c>
       <c r="B271" s="223"/>
     </row>
-    <row r="272" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="272" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A272" s="201" t="s">
         <v>79</v>
       </c>
@@ -10656,15 +10648,15 @@
         <v>180</v>
       </c>
     </row>
-    <row r="274" spans="1:7" ht="55.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:7" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A274" s="224" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B274" s="224"/>
       <c r="C274" s="224"/>
       <c r="D274" s="224"/>
     </row>
-    <row r="275" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A275" s="9" t="s">
         <v>37</v>
       </c>
@@ -10678,49 +10670,49 @@
         <v>181</v>
       </c>
     </row>
-    <row r="276" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A276" s="22" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B276" s="45"/>
       <c r="C276" s="22"/>
       <c r="D276" s="23"/>
     </row>
-    <row r="277" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A277" s="22" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B277" s="22"/>
       <c r="C277" s="22"/>
       <c r="D277" s="23"/>
     </row>
-    <row r="278" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A278" s="225"/>
       <c r="B278" s="225"/>
     </row>
-    <row r="279" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A279" s="38"/>
       <c r="B279" s="38"/>
     </row>
-    <row r="280" spans="1:7" ht="21" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A280" s="40" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="281" spans="1:7" ht="28" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:7" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A281" s="44" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="282" spans="1:7" ht="21" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A282" s="46"/>
     </row>
-    <row r="283" spans="1:7" ht="21" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A283" s="40" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="284" spans="1:7" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="284" spans="1:7" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A284" s="223" t="s">
         <v>184</v>
       </c>
@@ -10728,12 +10720,12 @@
       <c r="C284" s="223"/>
       <c r="D284" s="223"/>
     </row>
-    <row r="285" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="285" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A285" s="201" t="s">
         <v>79</v>
       </c>
       <c r="B285" s="202" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="C285" s="202"/>
       <c r="D285" s="202"/>
@@ -10741,15 +10733,15 @@
       <c r="F285" s="202"/>
       <c r="G285" s="173"/>
     </row>
-    <row r="287" spans="1:7" ht="44.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:7" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A287" s="224" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B287" s="224"/>
       <c r="C287" s="224"/>
       <c r="D287" s="224"/>
     </row>
-    <row r="289" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A289" s="47" t="s">
         <v>37</v>
       </c>
@@ -10763,27 +10755,27 @@
         <v>185</v>
       </c>
     </row>
-    <row r="290" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A290" s="22" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B290" s="22"/>
       <c r="C290" s="22"/>
       <c r="D290" s="49"/>
     </row>
-    <row r="291" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A291" s="22"/>
       <c r="B291" s="45"/>
       <c r="C291" s="22"/>
       <c r="D291" s="23"/>
     </row>
-    <row r="292" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A292" s="22"/>
       <c r="B292" s="22"/>
       <c r="C292" s="22"/>
       <c r="D292" s="23"/>
     </row>
-    <row r="293" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="293" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A293" s="24"/>
       <c r="B293" s="24"/>
     </row>
@@ -10893,28 +10885,28 @@
   </sheetPr>
   <dimension ref="A1:AMI121"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="C45" sqref="C45"/>
+      <selection pane="bottomLeft" activeCell="Q21" sqref="Q21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.1796875" style="181" customWidth="1"/>
-    <col min="2" max="2" width="18.1796875" style="181" customWidth="1"/>
-    <col min="3" max="3" width="142.1796875" style="182" customWidth="1"/>
-    <col min="4" max="6" width="5.7265625" style="183" customWidth="1"/>
-    <col min="7" max="11" width="8.7265625" style="183" customWidth="1"/>
-    <col min="12" max="12" width="78.7265625" style="183" customWidth="1"/>
-    <col min="13" max="13" width="36.81640625" style="181" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" style="181" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" style="181" customWidth="1"/>
+    <col min="3" max="3" width="142.140625" style="182" customWidth="1"/>
+    <col min="4" max="6" width="5.7109375" style="183" customWidth="1"/>
+    <col min="7" max="11" width="8.7109375" style="183" customWidth="1"/>
+    <col min="12" max="12" width="78.7109375" style="183" customWidth="1"/>
+    <col min="13" max="13" width="36.85546875" style="181" customWidth="1"/>
     <col min="14" max="14" width="29" style="181" customWidth="1"/>
-    <col min="15" max="15" width="73.7265625" style="181" customWidth="1"/>
-    <col min="16" max="1023" width="11.453125" style="181"/>
-    <col min="1024" max="16384" width="11.453125" style="3"/>
+    <col min="15" max="15" width="73.7109375" style="181" customWidth="1"/>
+    <col min="16" max="1023" width="11.42578125" style="181"/>
+    <col min="1024" max="16384" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="54" customFormat="1" ht="51.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" s="54" customFormat="1" ht="51.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="50" t="s">
         <v>186</v>
       </c>
@@ -10936,7 +10928,7 @@
       <c r="K1" s="53"/>
       <c r="L1" s="53"/>
     </row>
-    <row r="2" spans="1:19" s="54" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:19" s="54" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C2" s="55"/>
       <c r="D2" s="56" t="s">
         <v>190</v>
@@ -10975,7 +10967,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="3" spans="1:19" s="54" customFormat="1" ht="17.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:19" s="54" customFormat="1" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="255" t="s">
         <v>206</v>
       </c>
@@ -10994,7 +10986,7 @@
       <c r="N3" s="65"/>
       <c r="O3" s="66"/>
     </row>
-    <row r="4" spans="1:19" s="54" customFormat="1" ht="219" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:19" s="54" customFormat="1" ht="219" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="67" t="s">
         <v>207</v>
       </c>
@@ -11002,7 +10994,7 @@
         <v>208</v>
       </c>
       <c r="C4" s="69" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="D4" s="70" t="s">
         <v>202</v>
@@ -11024,16 +11016,16 @@
         <v>209</v>
       </c>
       <c r="M4" s="207" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="N4" s="77" t="s">
         <v>210</v>
       </c>
       <c r="O4" s="78" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" s="54" customFormat="1" ht="90" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" s="54" customFormat="1" ht="90" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="79" t="s">
         <v>211</v>
       </c>
@@ -11041,7 +11033,7 @@
         <v>212</v>
       </c>
       <c r="C5" s="81" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D5" s="82" t="s">
         <v>202</v>
@@ -11058,7 +11050,7 @@
       <c r="J5" s="84"/>
       <c r="K5" s="85"/>
       <c r="L5" s="37" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="M5" s="86" t="s">
         <v>213</v>
@@ -11067,14 +11059,14 @@
         <v>76</v>
       </c>
       <c r="O5" s="88" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="P5" s="3"/>
       <c r="Q5" s="3"/>
       <c r="R5" s="3"/>
       <c r="S5" s="3"/>
     </row>
-    <row r="6" spans="1:19" s="54" customFormat="1" ht="148.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:19" s="54" customFormat="1" ht="148.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="79" t="s">
         <v>214</v>
       </c>
@@ -11082,7 +11074,7 @@
         <v>212</v>
       </c>
       <c r="C6" s="81" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="D6" s="59" t="s">
         <v>202</v>
@@ -11108,14 +11100,14 @@
         <v>76</v>
       </c>
       <c r="O6" s="93" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="P6" s="3"/>
       <c r="Q6" s="3"/>
       <c r="R6" s="3"/>
       <c r="S6" s="3"/>
     </row>
-    <row r="7" spans="1:19" s="54" customFormat="1" ht="87.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:19" s="54" customFormat="1" ht="87.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="79" t="s">
         <v>217</v>
       </c>
@@ -11123,7 +11115,7 @@
         <v>208</v>
       </c>
       <c r="C7" s="81" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D7" s="59" t="s">
         <v>202</v>
@@ -11140,7 +11132,7 @@
       <c r="J7" s="94"/>
       <c r="K7" s="95"/>
       <c r="L7" s="37" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="M7" s="76" t="s">
         <v>76</v>
@@ -11156,7 +11148,7 @@
       <c r="R7" s="3"/>
       <c r="S7" s="3"/>
     </row>
-    <row r="8" spans="1:19" s="54" customFormat="1" ht="80.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:19" s="54" customFormat="1" ht="80.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="79" t="s">
         <v>218</v>
       </c>
@@ -11164,7 +11156,7 @@
         <v>208</v>
       </c>
       <c r="C8" s="81" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="D8" s="59" t="s">
         <v>202</v>
@@ -11195,7 +11187,7 @@
       <c r="R8" s="3"/>
       <c r="S8" s="3"/>
     </row>
-    <row r="9" spans="1:19" s="54" customFormat="1" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:19" s="54" customFormat="1" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="79" t="s">
         <v>221</v>
       </c>
@@ -11203,7 +11195,7 @@
         <v>208</v>
       </c>
       <c r="C9" s="81" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="D9" s="59" t="s">
         <v>202</v>
@@ -11218,7 +11210,7 @@
       <c r="J9" s="94"/>
       <c r="K9" s="95"/>
       <c r="L9" s="97" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="M9" s="94" t="s">
         <v>222</v>
@@ -11232,7 +11224,7 @@
       <c r="R9" s="3"/>
       <c r="S9" s="3"/>
     </row>
-    <row r="10" spans="1:19" s="102" customFormat="1" ht="62.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:19" s="102" customFormat="1" ht="62.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="98" t="s">
         <v>224</v>
       </c>
@@ -11265,7 +11257,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:19" s="54" customFormat="1" ht="103.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:19" s="54" customFormat="1" ht="103.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="79" t="s">
         <v>227</v>
       </c>
@@ -11273,7 +11265,7 @@
         <v>208</v>
       </c>
       <c r="C11" s="81" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="D11" s="59" t="s">
         <v>202</v>
@@ -11306,7 +11298,7 @@
       <c r="R11" s="3"/>
       <c r="S11" s="3"/>
     </row>
-    <row r="12" spans="1:19" s="54" customFormat="1" ht="129" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:19" s="54" customFormat="1" ht="129" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="79" t="s">
         <v>230</v>
       </c>
@@ -11314,7 +11306,7 @@
         <v>208</v>
       </c>
       <c r="C12" s="81" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="D12" s="59" t="s">
         <v>202</v>
@@ -11335,7 +11327,7 @@
       </c>
       <c r="K12" s="86"/>
       <c r="L12" s="110" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="M12" s="94" t="s">
         <v>222</v>
@@ -11351,7 +11343,7 @@
       <c r="R12" s="3"/>
       <c r="S12" s="3"/>
     </row>
-    <row r="13" spans="1:19" s="102" customFormat="1" ht="23.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:19" s="102" customFormat="1" ht="23.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="98" t="s">
         <v>233</v>
       </c>
@@ -11384,7 +11376,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="1:19" s="102" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:19" s="102" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="98" t="s">
         <v>236</v>
       </c>
@@ -11417,7 +11409,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:19" s="102" customFormat="1" ht="19.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:19" s="102" customFormat="1" ht="19.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="98" t="s">
         <v>239</v>
       </c>
@@ -11450,7 +11442,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="16" spans="1:19" s="54" customFormat="1" ht="98.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:19" s="54" customFormat="1" ht="98.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="79" t="s">
         <v>242</v>
       </c>
@@ -11458,7 +11450,7 @@
         <v>208</v>
       </c>
       <c r="C16" s="81" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="D16" s="59" t="s">
         <v>202</v>
@@ -11491,7 +11483,7 @@
       <c r="R16" s="3"/>
       <c r="S16" s="3"/>
     </row>
-    <row r="17" spans="1:15" s="54" customFormat="1" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:15" s="54" customFormat="1" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="117" t="s">
         <v>246</v>
       </c>
@@ -11499,7 +11491,7 @@
         <v>212</v>
       </c>
       <c r="C17" s="81" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D17" s="118" t="s">
         <v>202</v>
@@ -11516,7 +11508,7 @@
       <c r="J17" s="86"/>
       <c r="K17" s="86"/>
       <c r="L17" s="110" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="M17" s="92" t="s">
         <v>247</v>
@@ -11528,7 +11520,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="18" spans="1:15" s="102" customFormat="1" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:15" s="102" customFormat="1" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="120" t="s">
         <v>249</v>
       </c>
@@ -11561,7 +11553,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="19" spans="1:15" s="102" customFormat="1" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:15" s="102" customFormat="1" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="120" t="s">
         <v>253</v>
       </c>
@@ -11594,7 +11586,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="20" spans="1:15" s="102" customFormat="1" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:15" s="102" customFormat="1" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="98" t="s">
         <v>256</v>
       </c>
@@ -11627,7 +11619,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="21" spans="1:15" s="54" customFormat="1" ht="186" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:15" s="54" customFormat="1" ht="186" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="79" t="s">
         <v>259</v>
       </c>
@@ -11635,7 +11627,7 @@
         <v>212</v>
       </c>
       <c r="C21" s="81" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="D21" s="59" t="s">
         <v>202</v>
@@ -11652,19 +11644,19 @@
       <c r="J21" s="123"/>
       <c r="K21" s="123"/>
       <c r="L21" s="110" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="M21" s="76" t="s">
         <v>76</v>
       </c>
       <c r="N21" s="124" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="O21" s="125" t="s">
-        <v>611</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" s="54" customFormat="1" ht="264" customHeight="1" x14ac:dyDescent="0.35">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" s="54" customFormat="1" ht="264" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="79" t="s">
         <v>260</v>
       </c>
@@ -11672,7 +11664,7 @@
         <v>261</v>
       </c>
       <c r="C22" s="81" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="D22" s="126" t="s">
         <v>202</v>
@@ -11694,16 +11686,16 @@
         <v>262</v>
       </c>
       <c r="M22" s="110" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="N22" s="85" t="s">
         <v>210</v>
       </c>
       <c r="O22" s="125" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" s="54" customFormat="1" ht="117" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" s="54" customFormat="1" ht="117" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="79" t="s">
         <v>263</v>
       </c>
@@ -11711,7 +11703,7 @@
         <v>264</v>
       </c>
       <c r="C23" s="81" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="D23" s="126" t="s">
         <v>202</v>
@@ -11728,7 +11720,7 @@
       <c r="J23" s="123"/>
       <c r="K23" s="123"/>
       <c r="L23" s="110" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="M23" s="123" t="s">
         <v>213</v>
@@ -11737,10 +11729,10 @@
         <v>210</v>
       </c>
       <c r="O23" s="125" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" s="102" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" s="102" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="120" t="s">
         <v>265</v>
       </c>
@@ -11773,7 +11765,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="25" spans="1:15" s="102" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:15" s="102" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="98" t="s">
         <v>269</v>
       </c>
@@ -11806,7 +11798,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="26" spans="1:15" s="54" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:15" s="54" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="251" t="s">
         <v>271</v>
       </c>
@@ -11825,7 +11817,7 @@
       <c r="N26" s="133"/>
       <c r="O26" s="134"/>
     </row>
-    <row r="27" spans="1:15" s="54" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:15" s="54" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="79" t="s">
         <v>272</v>
       </c>
@@ -11833,7 +11825,7 @@
         <v>208</v>
       </c>
       <c r="C27" s="81" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="D27" s="126" t="s">
         <v>202</v>
@@ -11848,7 +11840,7 @@
       <c r="J27" s="86"/>
       <c r="K27" s="86"/>
       <c r="L27" s="110" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="M27" s="76" t="s">
         <v>76</v>
@@ -11860,7 +11852,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="28" spans="1:15" s="54" customFormat="1" ht="119.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:15" s="54" customFormat="1" ht="119.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="79" t="s">
         <v>273</v>
       </c>
@@ -11868,7 +11860,7 @@
         <v>208</v>
       </c>
       <c r="C28" s="81" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="D28" s="126" t="s">
         <v>202</v>
@@ -11887,7 +11879,7 @@
       <c r="J28" s="123"/>
       <c r="K28" s="123"/>
       <c r="L28" s="184" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="M28" s="123" t="s">
         <v>213</v>
@@ -11899,7 +11891,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="29" spans="1:15" s="54" customFormat="1" ht="74.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:15" s="54" customFormat="1" ht="74.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="79" t="s">
         <v>275</v>
       </c>
@@ -11907,7 +11899,7 @@
         <v>208</v>
       </c>
       <c r="C29" s="81" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D29" s="126" t="s">
         <v>202</v>
@@ -11936,7 +11928,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="30" spans="1:15" s="145" customFormat="1" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:15" s="145" customFormat="1" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="138" t="s">
         <v>278</v>
       </c>
@@ -11944,7 +11936,7 @@
         <v>208</v>
       </c>
       <c r="C30" s="140" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="D30" s="141"/>
       <c r="E30" s="141" t="s">
@@ -11969,7 +11961,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="31" spans="1:15" s="54" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:15" s="54" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="79" t="s">
         <v>280</v>
       </c>
@@ -11977,7 +11969,7 @@
         <v>208</v>
       </c>
       <c r="C31" s="81" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D31" s="126" t="s">
         <v>202</v>
@@ -12006,7 +11998,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="32" spans="1:15" s="54" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:15" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="79" t="s">
         <v>282</v>
       </c>
@@ -12014,7 +12006,7 @@
         <v>208</v>
       </c>
       <c r="C32" s="81" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="D32" s="126" t="s">
         <v>202</v>
@@ -12041,7 +12033,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="33" spans="1:17" s="54" customFormat="1" ht="88" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:17" s="54" customFormat="1" ht="87.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="79" t="s">
         <v>283</v>
       </c>
@@ -12049,7 +12041,7 @@
         <v>208</v>
       </c>
       <c r="C33" s="81" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="D33" s="126" t="s">
         <v>202</v>
@@ -12077,11 +12069,11 @@
         <v>380</v>
       </c>
       <c r="O33" s="125" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="Q33" s="53"/>
     </row>
-    <row r="34" spans="1:17" s="54" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:17" s="54" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="79" t="s">
         <v>285</v>
       </c>
@@ -12089,7 +12081,7 @@
         <v>208</v>
       </c>
       <c r="C34" s="81" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="D34" s="80" t="s">
         <v>202</v>
@@ -12118,7 +12110,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="35" spans="1:17" s="54" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:17" s="54" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="251" t="s">
         <v>287</v>
       </c>
@@ -12137,7 +12129,7 @@
       <c r="N35" s="133"/>
       <c r="O35" s="134"/>
     </row>
-    <row r="36" spans="1:17" s="54" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:17" s="54" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="79" t="s">
         <v>288</v>
       </c>
@@ -12145,7 +12137,7 @@
         <v>208</v>
       </c>
       <c r="C36" s="81" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="D36" s="126" t="s">
         <v>202</v>
@@ -12168,13 +12160,13 @@
         <v>290</v>
       </c>
       <c r="N36" s="124" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="O36" s="148" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="37" spans="1:17" s="54" customFormat="1" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:17" s="54" customFormat="1" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="79" t="s">
         <v>292</v>
       </c>
@@ -12182,7 +12174,7 @@
         <v>264</v>
       </c>
       <c r="C37" s="81" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="D37" s="126" t="s">
         <v>202</v>
@@ -12211,7 +12203,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="38" spans="1:17" s="54" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:17" s="54" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="256" t="s">
         <v>294</v>
       </c>
@@ -12230,7 +12222,7 @@
       <c r="N38" s="133"/>
       <c r="O38" s="134"/>
     </row>
-    <row r="39" spans="1:17" s="54" customFormat="1" ht="89.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:17" s="54" customFormat="1" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="79" t="s">
         <v>295</v>
       </c>
@@ -12253,7 +12245,7 @@
       <c r="J39" s="123"/>
       <c r="K39" s="123"/>
       <c r="L39" s="110" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="M39" s="110" t="s">
         <v>290</v>
@@ -12265,7 +12257,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="40" spans="1:17" s="54" customFormat="1" ht="100" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:17" s="54" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="79" t="s">
         <v>297</v>
       </c>
@@ -12273,7 +12265,7 @@
         <v>208</v>
       </c>
       <c r="C40" s="154" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="D40" s="151" t="s">
         <v>202</v>
@@ -12304,7 +12296,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="41" spans="1:17" s="54" customFormat="1" ht="96" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:17" s="54" customFormat="1" ht="96" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="79" t="s">
         <v>300</v>
       </c>
@@ -12312,7 +12304,7 @@
         <v>212</v>
       </c>
       <c r="C41" s="81" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="D41" s="151" t="s">
         <v>202</v>
@@ -12330,16 +12322,16 @@
         <v>301</v>
       </c>
       <c r="M41" s="110" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="N41" s="124" t="s">
         <v>380</v>
       </c>
       <c r="O41" s="125" t="s">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="42" spans="1:17" s="54" customFormat="1" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" s="54" customFormat="1" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="79" t="s">
         <v>302</v>
       </c>
@@ -12347,7 +12339,7 @@
         <v>208</v>
       </c>
       <c r="C42" s="81" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="D42" s="151" t="s">
         <v>202</v>
@@ -12374,7 +12366,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="43" spans="1:17" s="102" customFormat="1" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:17" s="102" customFormat="1" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="98" t="s">
         <v>305</v>
       </c>
@@ -12407,7 +12399,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="44" spans="1:17" s="54" customFormat="1" ht="85.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:17" s="54" customFormat="1" ht="85.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="79" t="s">
         <v>308</v>
       </c>
@@ -12415,7 +12407,7 @@
         <v>212</v>
       </c>
       <c r="C44" s="81" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="D44" s="151" t="s">
         <v>202</v>
@@ -12430,7 +12422,7 @@
       <c r="J44" s="86"/>
       <c r="K44" s="86"/>
       <c r="L44" s="207" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="M44" s="110" t="s">
         <v>213</v>
@@ -12442,7 +12434,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="45" spans="1:17" s="54" customFormat="1" ht="193.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:17" s="54" customFormat="1" ht="193.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="79" t="s">
         <v>311</v>
       </c>
@@ -12450,7 +12442,7 @@
         <v>212</v>
       </c>
       <c r="C45" s="81" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="D45" s="151" t="s">
         <v>202</v>
@@ -12479,7 +12471,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="46" spans="1:17" s="54" customFormat="1" ht="167.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:17" s="54" customFormat="1" ht="167.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="79" t="s">
         <v>315</v>
       </c>
@@ -12487,7 +12479,7 @@
         <v>208</v>
       </c>
       <c r="C46" s="81" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D46" s="151" t="s">
         <v>202</v>
@@ -12502,7 +12494,7 @@
       <c r="J46" s="123"/>
       <c r="K46" s="123"/>
       <c r="L46" s="110" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="M46" s="76" t="s">
         <v>76</v>
@@ -12514,7 +12506,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="47" spans="1:17" s="102" customFormat="1" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:17" s="102" customFormat="1" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="98" t="s">
         <v>316</v>
       </c>
@@ -12547,7 +12539,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="48" spans="1:17" s="54" customFormat="1" ht="87.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:17" s="54" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="79" t="s">
         <v>319</v>
       </c>
@@ -12555,7 +12547,7 @@
         <v>208</v>
       </c>
       <c r="C48" s="81" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="D48" s="151" t="s">
         <v>202</v>
@@ -12570,7 +12562,7 @@
       <c r="J48" s="123"/>
       <c r="K48" s="123"/>
       <c r="L48" s="110" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="M48" s="76" t="s">
         <v>76</v>
@@ -12582,7 +12574,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="49" spans="1:15" s="54" customFormat="1" ht="171.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:15" s="54" customFormat="1" ht="171.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="79" t="s">
         <v>321</v>
       </c>
@@ -12590,7 +12582,7 @@
         <v>208</v>
       </c>
       <c r="C49" s="81" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="D49" s="159" t="s">
         <v>202</v>
@@ -12619,7 +12611,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="50" spans="1:15" s="54" customFormat="1" ht="250.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:15" s="54" customFormat="1" ht="250.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="79" t="s">
         <v>325</v>
       </c>
@@ -12644,7 +12636,7 @@
       <c r="J50" s="123"/>
       <c r="K50" s="123"/>
       <c r="L50" s="110" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="M50" s="110" t="s">
         <v>327</v>
@@ -12656,7 +12648,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="51" spans="1:15" s="54" customFormat="1" ht="99" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:15" s="54" customFormat="1" ht="99" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="79" t="s">
         <v>330</v>
       </c>
@@ -12681,7 +12673,7 @@
       <c r="J51" s="86"/>
       <c r="K51" s="86"/>
       <c r="L51" s="110" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="M51" s="76" t="s">
         <v>76</v>
@@ -12693,7 +12685,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="52" spans="1:15" s="54" customFormat="1" ht="235.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:15" s="54" customFormat="1" ht="235.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="79" t="s">
         <v>333</v>
       </c>
@@ -12701,7 +12693,7 @@
         <v>250</v>
       </c>
       <c r="C52" s="81" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="D52" s="151" t="s">
         <v>202</v>
@@ -12728,7 +12720,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="53" spans="1:15" s="54" customFormat="1" ht="61.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:15" s="54" customFormat="1" ht="61.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="79" t="s">
         <v>336</v>
       </c>
@@ -12736,7 +12728,7 @@
         <v>208</v>
       </c>
       <c r="C53" s="81" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="D53" s="151" t="s">
         <v>202</v>
@@ -12763,7 +12755,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="54" spans="1:15" s="102" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:15" s="102" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="98" t="s">
         <v>339</v>
       </c>
@@ -12796,7 +12788,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="55" spans="1:15" s="102" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:15" s="102" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="98" t="s">
         <v>341</v>
       </c>
@@ -12828,7 +12820,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="56" spans="1:15" s="102" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:15" s="102" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="98" t="s">
         <v>343</v>
       </c>
@@ -12861,7 +12853,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="57" spans="1:15" s="102" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:15" s="102" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="98" t="s">
         <v>347</v>
       </c>
@@ -12894,7 +12886,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="58" spans="1:15" s="102" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:15" s="102" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="98" t="s">
         <v>348</v>
       </c>
@@ -12927,7 +12919,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="59" spans="1:15" s="54" customFormat="1" ht="105.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:15" s="54" customFormat="1" ht="105.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="79" t="s">
         <v>350</v>
       </c>
@@ -12935,7 +12927,7 @@
         <v>351</v>
       </c>
       <c r="C59" s="81" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="D59" s="151" t="s">
         <v>202</v>
@@ -12955,7 +12947,7 @@
         <v>352</v>
       </c>
       <c r="M59" s="123" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="N59" s="124" t="s">
         <v>328</v>
@@ -12964,7 +12956,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="60" spans="1:15" s="102" customFormat="1" ht="70.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:15" s="102" customFormat="1" ht="70.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="98" t="s">
         <v>354</v>
       </c>
@@ -12997,7 +12989,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="61" spans="1:15" s="54" customFormat="1" ht="69.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:15" s="54" customFormat="1" ht="69.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="79" t="s">
         <v>357</v>
       </c>
@@ -13005,7 +12997,7 @@
         <v>358</v>
       </c>
       <c r="C61" s="81" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="D61" s="151" t="s">
         <v>202</v>
@@ -13025,7 +13017,7 @@
         <v>359</v>
       </c>
       <c r="M61" s="123" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="N61" s="124" t="s">
         <v>328</v>
@@ -13034,7 +13026,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="62" spans="1:15" s="54" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:15" s="54" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="79" t="s">
         <v>361</v>
       </c>
@@ -13042,7 +13034,7 @@
         <v>208</v>
       </c>
       <c r="C62" s="81" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="D62" s="151" t="s">
         <v>202</v>
@@ -13069,7 +13061,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="63" spans="1:15" s="54" customFormat="1" ht="43" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:15" s="54" customFormat="1" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="79" t="s">
         <v>363</v>
       </c>
@@ -13077,7 +13069,7 @@
         <v>208</v>
       </c>
       <c r="C63" s="81" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="D63" s="151" t="s">
         <v>202</v>
@@ -13104,7 +13096,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="64" spans="1:15" s="54" customFormat="1" ht="119.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:15" s="54" customFormat="1" ht="119.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="79" t="s">
         <v>366</v>
       </c>
@@ -13112,7 +13104,7 @@
         <v>208</v>
       </c>
       <c r="C64" s="81" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="D64" s="151" t="s">
         <v>202</v>
@@ -13141,7 +13133,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="65" spans="1:15" s="102" customFormat="1" ht="29.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:15" s="102" customFormat="1" ht="29.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="98" t="s">
         <v>369</v>
       </c>
@@ -13174,7 +13166,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="66" spans="1:15" s="54" customFormat="1" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:15" s="54" customFormat="1" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="79" t="s">
         <v>371</v>
       </c>
@@ -13182,7 +13174,7 @@
         <v>208</v>
       </c>
       <c r="C66" s="81" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="D66" s="151" t="s">
         <v>202</v>
@@ -13202,7 +13194,7 @@
         <v>372</v>
       </c>
       <c r="M66" s="123" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="N66" s="124" t="s">
         <v>328</v>
@@ -13211,7 +13203,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="67" spans="1:15" s="54" customFormat="1" ht="84" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:15" s="54" customFormat="1" ht="84" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="79" t="s">
         <v>374</v>
       </c>
@@ -13219,7 +13211,7 @@
         <v>208</v>
       </c>
       <c r="C67" s="81" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="D67" s="151" t="s">
         <v>202</v>
@@ -13239,16 +13231,16 @@
         <v>375</v>
       </c>
       <c r="M67" s="110" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="N67" s="124" t="s">
         <v>328</v>
       </c>
       <c r="O67" s="125" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="68" spans="1:15" s="54" customFormat="1" ht="102" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15" s="54" customFormat="1" ht="102" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="79" t="s">
         <v>376</v>
       </c>
@@ -13256,7 +13248,7 @@
         <v>212</v>
       </c>
       <c r="C68" s="81" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="D68" s="151" t="s">
         <v>202</v>
@@ -13274,16 +13266,16 @@
         <v>377</v>
       </c>
       <c r="M68" s="123" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="N68" s="124" t="s">
         <v>328</v>
       </c>
       <c r="O68" s="125" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="69" spans="1:15" s="54" customFormat="1" ht="87" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" s="54" customFormat="1" ht="87" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="79" t="s">
         <v>378</v>
       </c>
@@ -13291,7 +13283,7 @@
         <v>212</v>
       </c>
       <c r="C69" s="81" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="D69" s="151" t="s">
         <v>202</v>
@@ -13306,7 +13298,7 @@
       <c r="J69" s="123"/>
       <c r="K69" s="123"/>
       <c r="L69" s="110" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="M69" s="110" t="s">
         <v>379</v>
@@ -13318,7 +13310,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="70" spans="1:15" s="54" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:15" s="54" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="251" t="s">
         <v>382</v>
       </c>
@@ -13337,7 +13329,7 @@
       <c r="N70" s="133"/>
       <c r="O70" s="134"/>
     </row>
-    <row r="71" spans="1:15" s="54" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:15" s="54" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="79" t="s">
         <v>383</v>
       </c>
@@ -13345,7 +13337,7 @@
         <v>208</v>
       </c>
       <c r="C71" s="81" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="D71" s="151" t="s">
         <v>202</v>
@@ -13372,7 +13364,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="72" spans="1:15" s="54" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:15" s="54" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="79" t="s">
         <v>386</v>
       </c>
@@ -13380,7 +13372,7 @@
         <v>208</v>
       </c>
       <c r="C72" s="81" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="D72" s="151" t="s">
         <v>202</v>
@@ -13407,7 +13399,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="73" spans="1:15" s="102" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:15" s="102" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="98" t="s">
         <v>389</v>
       </c>
@@ -13440,7 +13432,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="74" spans="1:15" s="102" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:15" s="102" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="98" t="s">
         <v>392</v>
       </c>
@@ -13473,7 +13465,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="75" spans="1:15" s="54" customFormat="1" ht="178.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:15" s="54" customFormat="1" ht="178.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="79" t="s">
         <v>394</v>
       </c>
@@ -13481,7 +13473,7 @@
         <v>208</v>
       </c>
       <c r="C75" s="81" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="D75" s="151" t="s">
         <v>202</v>
@@ -13496,10 +13488,10 @@
       <c r="J75" s="123"/>
       <c r="K75" s="123"/>
       <c r="L75" s="110" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="M75" s="123" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="N75" s="124" t="s">
         <v>51</v>
@@ -13508,7 +13500,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="76" spans="1:15" s="54" customFormat="1" ht="71.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:15" s="54" customFormat="1" ht="71.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="79" t="s">
         <v>396</v>
       </c>
@@ -13516,7 +13508,7 @@
         <v>212</v>
       </c>
       <c r="C76" s="81" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="D76" s="151" t="s">
         <v>202</v>
@@ -13533,10 +13525,10 @@
       <c r="J76" s="123"/>
       <c r="K76" s="123"/>
       <c r="L76" s="110" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="M76" s="123" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="N76" s="124" t="s">
         <v>51</v>
@@ -13545,7 +13537,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="77" spans="1:15" s="54" customFormat="1" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:15" s="54" customFormat="1" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="79" t="s">
         <v>397</v>
       </c>
@@ -13553,7 +13545,7 @@
         <v>264</v>
       </c>
       <c r="C77" s="81" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="D77" s="151" t="s">
         <v>202</v>
@@ -13577,10 +13569,10 @@
         <v>380</v>
       </c>
       <c r="O77" s="148" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="78" spans="1:15" s="54" customFormat="1" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="78" spans="1:15" s="54" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="79" t="s">
         <v>399</v>
       </c>
@@ -13588,7 +13580,7 @@
         <v>250</v>
       </c>
       <c r="C78" s="81" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D78" s="151" t="s">
         <v>202</v>
@@ -13603,7 +13595,7 @@
       <c r="J78" s="123"/>
       <c r="K78" s="123"/>
       <c r="L78" s="169" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="M78" s="76" t="s">
         <v>76</v>
@@ -13615,7 +13607,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="79" spans="1:15" s="54" customFormat="1" ht="195" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:15" s="54" customFormat="1" ht="195" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="79" t="s">
         <v>401</v>
       </c>
@@ -13623,7 +13615,7 @@
         <v>208</v>
       </c>
       <c r="C79" s="81" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="D79" s="151" t="s">
         <v>202</v>
@@ -13638,7 +13630,7 @@
       <c r="J79" s="123"/>
       <c r="K79" s="123"/>
       <c r="L79" s="110" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="M79" s="76" t="s">
         <v>76</v>
@@ -13650,7 +13642,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="80" spans="1:15" s="54" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:15" s="54" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="79" t="s">
         <v>403</v>
       </c>
@@ -13658,7 +13650,7 @@
         <v>208</v>
       </c>
       <c r="C80" s="81" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="D80" s="146" t="s">
         <v>202</v>
@@ -13685,7 +13677,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="81" spans="1:15" s="54" customFormat="1" ht="192.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:15" s="54" customFormat="1" ht="192.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="79" t="s">
         <v>405</v>
       </c>
@@ -13693,7 +13685,7 @@
         <v>208</v>
       </c>
       <c r="C81" s="81" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="D81" s="151" t="s">
         <v>202</v>
@@ -13708,7 +13700,7 @@
       <c r="J81" s="123"/>
       <c r="K81" s="123"/>
       <c r="L81" s="128" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="M81" s="76" t="s">
         <v>76</v>
@@ -13720,7 +13712,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="82" spans="1:15" s="54" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:15" s="54" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="251" t="s">
         <v>150</v>
       </c>
@@ -13739,7 +13731,7 @@
       <c r="N82" s="133"/>
       <c r="O82" s="134"/>
     </row>
-    <row r="83" spans="1:15" s="54" customFormat="1" ht="132" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:15" s="54" customFormat="1" ht="132" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="81" t="s">
         <v>407</v>
       </c>
@@ -13747,7 +13739,7 @@
         <v>208</v>
       </c>
       <c r="C83" s="81" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="D83" s="151" t="s">
         <v>202</v>
@@ -13767,7 +13759,7 @@
         <v>408</v>
       </c>
       <c r="M83" s="123" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="N83" s="124" t="s">
         <v>328</v>
@@ -13776,7 +13768,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="84" spans="1:15" s="54" customFormat="1" ht="71.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:15" s="54" customFormat="1" ht="71.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="79" t="s">
         <v>410</v>
       </c>
@@ -13784,7 +13776,7 @@
         <v>208</v>
       </c>
       <c r="C84" s="81" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="D84" s="151" t="s">
         <v>202</v>
@@ -13811,7 +13803,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="85" spans="1:15" s="54" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:15" s="54" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="79" t="s">
         <v>413</v>
       </c>
@@ -13819,7 +13811,7 @@
         <v>264</v>
       </c>
       <c r="C85" s="81" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="D85" s="151" t="s">
         <v>202</v>
@@ -13846,7 +13838,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="86" spans="1:15" s="54" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:15" s="54" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="79" t="s">
         <v>415</v>
       </c>
@@ -13854,7 +13846,7 @@
         <v>208</v>
       </c>
       <c r="C86" s="81" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="D86" s="151" t="s">
         <v>202</v>
@@ -13881,7 +13873,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="87" spans="1:15" s="54" customFormat="1" ht="70.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:15" s="54" customFormat="1" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="79" t="s">
         <v>417</v>
       </c>
@@ -13889,7 +13881,7 @@
         <v>351</v>
       </c>
       <c r="C87" s="81" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="D87" s="151" t="s">
         <v>202</v>
@@ -13918,7 +13910,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="88" spans="1:15" s="54" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:15" s="54" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="251" t="s">
         <v>419</v>
       </c>
@@ -13937,7 +13929,7 @@
       <c r="N88" s="133"/>
       <c r="O88" s="134"/>
     </row>
-    <row r="89" spans="1:15" s="54" customFormat="1" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="89" spans="1:15" s="54" customFormat="1" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="117" t="s">
         <v>420</v>
       </c>
@@ -13945,7 +13937,7 @@
         <v>212</v>
       </c>
       <c r="C89" s="81" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="D89" s="151" t="s">
         <v>202</v>
@@ -13972,7 +13964,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="90" spans="1:15" s="54" customFormat="1" ht="57.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="90" spans="1:15" s="54" customFormat="1" ht="57.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="117" t="s">
         <v>423</v>
       </c>
@@ -13980,7 +13972,7 @@
         <v>212</v>
       </c>
       <c r="C90" s="81" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="D90" s="151" t="s">
         <v>202</v>
@@ -14007,7 +13999,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="91" spans="1:15" s="54" customFormat="1" ht="116" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:15" s="54" customFormat="1" ht="128.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="117" t="s">
         <v>425</v>
       </c>
@@ -14015,7 +14007,7 @@
         <v>208</v>
       </c>
       <c r="C91" s="81" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="D91" s="151" t="s">
         <v>202</v>
@@ -14030,7 +14022,7 @@
       <c r="J91" s="123"/>
       <c r="K91" s="123"/>
       <c r="L91" s="110" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="M91" s="110" t="s">
         <v>426</v>
@@ -14039,18 +14031,18 @@
         <v>76</v>
       </c>
       <c r="O91" s="125" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="92" spans="1:15" s="54" customFormat="1" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="117" t="s">
         <v>427</v>
-      </c>
-    </row>
-    <row r="92" spans="1:15" s="54" customFormat="1" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A92" s="117" t="s">
-        <v>428</v>
       </c>
       <c r="B92" s="80" t="s">
         <v>208</v>
       </c>
       <c r="C92" s="81" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="D92" s="151" t="s">
         <v>202</v>
@@ -14068,24 +14060,24 @@
         <v>76</v>
       </c>
       <c r="M92" s="123" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="N92" s="76" t="s">
         <v>76</v>
       </c>
       <c r="O92" s="125" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="93" spans="1:15" s="54" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A93" s="79" t="s">
         <v>429</v>
-      </c>
-    </row>
-    <row r="93" spans="1:15" s="54" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A93" s="79" t="s">
-        <v>430</v>
       </c>
       <c r="B93" s="137" t="s">
         <v>208</v>
       </c>
       <c r="C93" s="81" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="D93" s="151"/>
       <c r="E93" s="126"/>
@@ -14098,7 +14090,7 @@
       <c r="J93" s="123"/>
       <c r="K93" s="123"/>
       <c r="L93" s="110" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="M93" s="76" t="s">
         <v>76</v>
@@ -14110,9 +14102,9 @@
         <v>76</v>
       </c>
     </row>
-    <row r="94" spans="1:15" s="54" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="94" spans="1:15" s="54" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="251" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B94" s="251"/>
       <c r="C94" s="251"/>
@@ -14129,15 +14121,15 @@
       <c r="N94" s="133"/>
       <c r="O94" s="134"/>
     </row>
-    <row r="95" spans="1:15" s="54" customFormat="1" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:15" s="54" customFormat="1" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="117" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B95" s="80" t="s">
         <v>208</v>
       </c>
       <c r="C95" s="81" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="D95" s="126" t="s">
         <v>202</v>
@@ -14152,27 +14144,27 @@
       <c r="J95" s="123"/>
       <c r="K95" s="123"/>
       <c r="L95" s="123" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="M95" s="123" t="s">
         <v>244</v>
       </c>
       <c r="N95" s="124" t="s">
+        <v>433</v>
+      </c>
+      <c r="O95" s="125" t="s">
         <v>434</v>
       </c>
-      <c r="O95" s="125" t="s">
+    </row>
+    <row r="96" spans="1:15" s="54" customFormat="1" ht="87" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="79" t="s">
         <v>435</v>
-      </c>
-    </row>
-    <row r="96" spans="1:15" s="54" customFormat="1" ht="87" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A96" s="79" t="s">
-        <v>436</v>
       </c>
       <c r="B96" s="137" t="s">
         <v>212</v>
       </c>
       <c r="C96" s="81" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="D96" s="126" t="s">
         <v>202</v>
@@ -14189,21 +14181,21 @@
       <c r="J96" s="123"/>
       <c r="K96" s="123"/>
       <c r="L96" s="110" t="s">
+        <v>436</v>
+      </c>
+      <c r="M96" s="110" t="s">
         <v>437</v>
       </c>
-      <c r="M96" s="110" t="s">
+      <c r="N96" s="124" t="s">
+        <v>433</v>
+      </c>
+      <c r="O96" s="125" t="s">
         <v>438</v>
       </c>
-      <c r="N96" s="124" t="s">
-        <v>434</v>
-      </c>
-      <c r="O96" s="125" t="s">
+    </row>
+    <row r="97" spans="1:15" s="54" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="251" t="s">
         <v>439</v>
-      </c>
-    </row>
-    <row r="97" spans="1:15" s="54" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A97" s="251" t="s">
-        <v>440</v>
       </c>
       <c r="B97" s="251"/>
       <c r="C97" s="251"/>
@@ -14220,15 +14212,15 @@
       <c r="N97" s="133"/>
       <c r="O97" s="134"/>
     </row>
-    <row r="98" spans="1:15" s="54" customFormat="1" ht="123" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:15" s="54" customFormat="1" ht="123" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="79" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B98" s="137" t="s">
         <v>208</v>
       </c>
       <c r="C98" s="172" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="D98" s="126" t="s">
         <v>202</v>
@@ -14243,21 +14235,21 @@
       <c r="J98" s="123"/>
       <c r="K98" s="123"/>
       <c r="L98" s="168" t="s">
+        <v>441</v>
+      </c>
+      <c r="M98" s="110" t="s">
         <v>442</v>
       </c>
-      <c r="M98" s="110" t="s">
+      <c r="N98" s="124" t="s">
+        <v>433</v>
+      </c>
+      <c r="O98" s="125" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="99" spans="1:15" s="54" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="251" t="s">
         <v>443</v>
-      </c>
-      <c r="N98" s="124" t="s">
-        <v>434</v>
-      </c>
-      <c r="O98" s="125" t="s">
-        <v>654</v>
-      </c>
-    </row>
-    <row r="99" spans="1:15" s="54" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A99" s="251" t="s">
-        <v>444</v>
       </c>
       <c r="B99" s="251"/>
       <c r="C99" s="251"/>
@@ -14274,15 +14266,15 @@
       <c r="N99" s="133"/>
       <c r="O99" s="134"/>
     </row>
-    <row r="100" spans="1:15" s="54" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:15" s="54" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="117" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B100" s="80" t="s">
         <v>212</v>
       </c>
       <c r="C100" s="81" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="D100" s="159" t="s">
         <v>202</v>
@@ -14297,7 +14289,7 @@
       <c r="J100" s="123"/>
       <c r="K100" s="123"/>
       <c r="L100" s="110" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="M100" s="169" t="s">
         <v>76</v>
@@ -14306,18 +14298,18 @@
         <v>328</v>
       </c>
       <c r="O100" s="125" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="101" spans="1:15" s="54" customFormat="1" ht="171" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="117" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="101" spans="1:15" s="54" customFormat="1" ht="171" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A101" s="117" t="s">
+      <c r="B101" s="80" t="s">
         <v>447</v>
       </c>
-      <c r="B101" s="80" t="s">
-        <v>448</v>
-      </c>
       <c r="C101" s="81" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="D101" s="151" t="s">
         <v>202</v>
@@ -14332,27 +14324,27 @@
       <c r="J101" s="86"/>
       <c r="K101" s="86"/>
       <c r="L101" s="110" t="s">
+        <v>448</v>
+      </c>
+      <c r="M101" s="169" t="s">
+        <v>76</v>
+      </c>
+      <c r="N101" s="124" t="s">
+        <v>433</v>
+      </c>
+      <c r="O101" s="116" t="s">
         <v>449</v>
       </c>
-      <c r="M101" s="169" t="s">
-        <v>76</v>
-      </c>
-      <c r="N101" s="124" t="s">
-        <v>434</v>
-      </c>
-      <c r="O101" s="116" t="s">
+    </row>
+    <row r="102" spans="1:15" s="54" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="117" t="s">
         <v>450</v>
-      </c>
-    </row>
-    <row r="102" spans="1:15" s="54" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A102" s="117" t="s">
-        <v>451</v>
       </c>
       <c r="B102" s="80" t="s">
         <v>264</v>
       </c>
       <c r="C102" s="81" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="D102" s="151" t="s">
         <v>202</v>
@@ -14367,19 +14359,19 @@
       <c r="J102" s="123"/>
       <c r="K102" s="123"/>
       <c r="L102" s="110" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="M102" s="169" t="s">
         <v>76</v>
       </c>
       <c r="N102" s="124" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="O102" s="125" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="103" spans="1:15" s="54" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="103" spans="1:15" s="54" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="252" t="s">
         <v>174</v>
       </c>
@@ -14398,15 +14390,15 @@
       <c r="N103" s="133"/>
       <c r="O103" s="134"/>
     </row>
-    <row r="104" spans="1:15" s="102" customFormat="1" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="104" spans="1:15" s="102" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="120" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B104" s="99" t="s">
         <v>208</v>
       </c>
       <c r="C104" s="100" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D104" s="158"/>
       <c r="E104" s="129" t="s">
@@ -14419,27 +14411,27 @@
       <c r="J104" s="111"/>
       <c r="K104" s="111"/>
       <c r="L104" s="112" t="s">
+        <v>454</v>
+      </c>
+      <c r="M104" s="104" t="s">
+        <v>76</v>
+      </c>
+      <c r="N104" s="104" t="s">
+        <v>76</v>
+      </c>
+      <c r="O104" s="104" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="105" spans="1:15" s="102" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A105" s="120" t="s">
         <v>455</v>
-      </c>
-      <c r="M104" s="104" t="s">
-        <v>76</v>
-      </c>
-      <c r="N104" s="104" t="s">
-        <v>76</v>
-      </c>
-      <c r="O104" s="104" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="105" spans="1:15" s="102" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A105" s="120" t="s">
-        <v>456</v>
       </c>
       <c r="B105" s="99" t="s">
         <v>208</v>
       </c>
       <c r="C105" s="100" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="D105" s="158"/>
       <c r="E105" s="129" t="s">
@@ -14464,9 +14456,9 @@
         <v>76</v>
       </c>
     </row>
-    <row r="106" spans="1:15" s="102" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="106" spans="1:15" s="102" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A106" s="120" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B106" s="99" t="s">
         <v>264</v>
@@ -14497,15 +14489,15 @@
         <v>76</v>
       </c>
     </row>
-    <row r="107" spans="1:15" s="102" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="107" spans="1:15" s="102" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="174" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B107" s="99" t="s">
         <v>208</v>
       </c>
       <c r="C107" s="175" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="D107" s="176"/>
       <c r="E107" s="99" t="s">
@@ -14530,7 +14522,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="108" spans="1:15" s="54" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="108" spans="1:15" s="54" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A108" s="251" t="s">
         <v>182</v>
       </c>
@@ -14549,15 +14541,15 @@
       <c r="N108" s="133"/>
       <c r="O108" s="134"/>
     </row>
-    <row r="109" spans="1:15" s="102" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="109" spans="1:15" s="102" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A109" s="120" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B109" s="99" t="s">
         <v>212</v>
       </c>
       <c r="C109" s="100" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="D109" s="158"/>
       <c r="E109" s="129" t="s">
@@ -14570,7 +14562,7 @@
       <c r="J109" s="111"/>
       <c r="K109" s="111"/>
       <c r="L109" s="112" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="M109" s="104" t="s">
         <v>76</v>
@@ -14582,15 +14574,15 @@
         <v>76</v>
       </c>
     </row>
-    <row r="110" spans="1:15" s="102" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="110" spans="1:15" s="102" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A110" s="98" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B110" s="99" t="s">
         <v>264</v>
       </c>
       <c r="C110" s="100" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="D110" s="158"/>
       <c r="E110" s="129" t="s">
@@ -14615,13 +14607,13 @@
         <v>76</v>
       </c>
     </row>
-    <row r="111" spans="1:15" s="102" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="111" spans="1:15" s="102" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="98" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B111" s="99"/>
       <c r="C111" s="100" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="D111" s="158"/>
       <c r="E111" s="129" t="s">
@@ -14646,15 +14638,15 @@
         <v>76</v>
       </c>
     </row>
-    <row r="112" spans="1:15" s="102" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="112" spans="1:15" s="102" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A112" s="98" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B112" s="99" t="s">
         <v>208</v>
       </c>
       <c r="C112" s="100" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="D112" s="158"/>
       <c r="E112" s="129" t="s">
@@ -14678,7 +14670,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="113" spans="1:15" s="54" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="113" spans="1:15" s="54" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A113" s="251" t="s">
         <v>183</v>
       </c>
@@ -14697,15 +14689,15 @@
       <c r="N113" s="133"/>
       <c r="O113" s="134"/>
     </row>
-    <row r="114" spans="1:15" s="102" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="114" spans="1:15" s="102" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A114" s="120" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B114" s="99" t="s">
         <v>212</v>
       </c>
       <c r="C114" s="100" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="D114" s="158"/>
       <c r="E114" s="129" t="s">
@@ -14718,27 +14710,27 @@
       <c r="J114" s="111"/>
       <c r="K114" s="111"/>
       <c r="L114" s="112" t="s">
+        <v>470</v>
+      </c>
+      <c r="M114" s="104" t="s">
+        <v>76</v>
+      </c>
+      <c r="N114" s="104" t="s">
+        <v>76</v>
+      </c>
+      <c r="O114" s="104" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="115" spans="1:15" s="102" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A115" s="120" t="s">
         <v>471</v>
-      </c>
-      <c r="M114" s="104" t="s">
-        <v>76</v>
-      </c>
-      <c r="N114" s="104" t="s">
-        <v>76</v>
-      </c>
-      <c r="O114" s="104" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="115" spans="1:15" s="102" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A115" s="120" t="s">
-        <v>472</v>
       </c>
       <c r="B115" s="129" t="s">
         <v>212</v>
       </c>
       <c r="C115" s="100" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="D115" s="158"/>
       <c r="E115" s="129" t="s">
@@ -14763,9 +14755,9 @@
         <v>76</v>
       </c>
     </row>
-    <row r="116" spans="1:15" s="102" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="116" spans="1:15" s="102" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A116" s="177" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B116" s="178" t="s">
         <v>264</v>
@@ -14796,16 +14788,16 @@
         <v>76</v>
       </c>
     </row>
-    <row r="118" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:15" x14ac:dyDescent="0.25">
       <c r="L118" s="209"/>
     </row>
-    <row r="119" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:15" x14ac:dyDescent="0.25">
       <c r="L119" s="209"/>
     </row>
-    <row r="120" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:15" x14ac:dyDescent="0.25">
       <c r="L120" s="209"/>
     </row>
-    <row r="121" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:15" x14ac:dyDescent="0.25">
       <c r="L121" s="209"/>
     </row>
   </sheetData>
@@ -14842,9 +14834,9 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>203</v>
       </c>
@@ -14873,7 +14865,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>204</v>
       </c>
@@ -14896,15 +14888,15 @@
         <v>24</v>
       </c>
       <c r="J2" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="K2">
         <v>164</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -14925,7 +14917,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>192</v>
       </c>
@@ -14936,48 +14928,48 @@
         <v>109</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K9" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="L9">
         <f>101-32</f>
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K10" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="L10">
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="B11">
         <v>78</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="B12">
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="B13">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>192</v>
       </c>

</xml_diff>

<commit_message>
auto commit @13.01.2021: 23:39:18,13
</commit_message>
<xml_diff>
--- a/Bachelorarbeit/Weckermann_ICS_and_Test Documentation.xlsx
+++ b/Bachelorarbeit/Weckermann_ICS_and_Test Documentation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Benutzer\Henry\Downloads\Abschlussarbeit_H-BRS\Bachelorarbeit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{938F0EEF-169A-4957-BBCF-C05DF1D19D68}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAF747F1-91CC-4D4F-86F7-B5FEB5AA3683}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Conformance Statement" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1464" uniqueCount="664">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1517" uniqueCount="678">
   <si>
     <t>Im Rahmen von [BSI TR-03148 -P] muss ein Implementation Conformance Statement ausgefüllt werden. Im folgenden finden Sie eine Vorlage für das ICS. Das Originaldokument ist auf Englisch, weswegen hier die englischen Formulierungen übernommen wurden, da keine offizielle Übersetzung des Dokuments existiert. Die Eintragungen können aber auf deutsch oder englisch gemacht werden. Die hier eingetragenen Beispieldaten sind durch Echtdaten zu ersetzen. Alternativ oder ergänzend zu dem ICS in dieser Tabelle kann auch das ICS aus [BSI TR-03148-P] als Vorlage genutzt werden.</t>
   </si>
@@ -4553,6 +4553,48 @@
   <si>
     <t>setup scripts:
 TP_A_19_1_full_setup.sh</t>
+  </si>
+  <si>
+    <t>Kondition</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Anzahl</t>
+  </si>
+  <si>
+    <t>Kondition --&gt; Status</t>
+  </si>
+  <si>
+    <t>Passed</t>
+  </si>
+  <si>
+    <t>Failed</t>
+  </si>
+  <si>
+    <t>MAY - Kriterium</t>
+  </si>
+  <si>
+    <t>MUST - Kriterium</t>
+  </si>
+  <si>
+    <t>SHOULD  - Kriterium</t>
+  </si>
+  <si>
+    <t>MUST NOT - Kriterium</t>
+  </si>
+  <si>
+    <t>MUST - Kriterium / MAY</t>
+  </si>
+  <si>
+    <t>RECOMMENDED  -  Kriterium</t>
+  </si>
+  <si>
+    <t>SHOULD NOT  -  Kriterium</t>
+  </si>
+  <si>
+    <t>MUST - Kriterium / Should</t>
   </si>
 </sst>
 </file>
@@ -7969,6 +8011,37 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5BA4A80C-FE8B-4838-A4B1-9BACCB5122E9}" name="Tabelle1" displayName="Tabelle1" ref="R1:S25" totalsRowShown="0">
+  <autoFilter ref="R1:S25" xr:uid="{E8155344-BFAA-40C6-ABC5-047844C93654}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="R2:S25">
+    <sortCondition descending="1" ref="S1:S25"/>
+  </sortState>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{FB990BF4-2BFC-4D0C-8D74-B21304FF5334}" name="Kondition --&gt; Status">
+      <calculatedColumnFormula>N2 &amp; " --&gt; " &amp;O2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="2" xr3:uid="{94E8A479-DCC0-4FB0-87A8-9790C66285FE}" name="Anzahl"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{AEBD571B-0805-4DFB-907F-507B227FD89C}" name="Tabelle2" displayName="Tabelle2" ref="N1:P25" totalsRowShown="0">
+  <autoFilter ref="N1:P25" xr:uid="{1FDE2A75-9E31-4AD5-B365-78FB8B537A53}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="N2:P25">
+    <sortCondition descending="1" ref="P1:P25"/>
+  </sortState>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{BD43E015-E362-4E0E-906A-250A3BFCED35}" name="Kondition"/>
+    <tableColumn id="2" xr3:uid="{2548C823-C45B-41A2-B2EA-D11DBA74C492}" name="Status"/>
+    <tableColumn id="3" xr3:uid="{0BEF207A-8354-47BA-8102-8001837EA8A0}" name="Anzahl"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
@@ -10883,12 +10956,12 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AMI121"/>
+  <dimension ref="A1:AMI125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A105" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="Q21" sqref="Q21"/>
+      <selection pane="bottomLeft" activeCell="J128" sqref="J128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10897,7 +10970,8 @@
     <col min="2" max="2" width="18.140625" style="181" customWidth="1"/>
     <col min="3" max="3" width="142.140625" style="182" customWidth="1"/>
     <col min="4" max="6" width="5.7109375" style="183" customWidth="1"/>
-    <col min="7" max="11" width="8.7109375" style="183" customWidth="1"/>
+    <col min="7" max="10" width="8.7109375" style="183" customWidth="1"/>
+    <col min="11" max="11" width="8.42578125" style="183" customWidth="1"/>
     <col min="12" max="12" width="78.7109375" style="183" customWidth="1"/>
     <col min="13" max="13" width="36.85546875" style="181" customWidth="1"/>
     <col min="14" max="14" width="29" style="181" customWidth="1"/>
@@ -14789,16 +14863,22 @@
       </c>
     </row>
     <row r="118" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G118" s="182"/>
       <c r="L118" s="209"/>
     </row>
     <row r="119" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G119" s="182"/>
       <c r="L119" s="209"/>
     </row>
     <row r="120" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G120" s="182"/>
       <c r="L120" s="209"/>
     </row>
     <row r="121" spans="1:15" x14ac:dyDescent="0.25">
       <c r="L121" s="209"/>
+    </row>
+    <row r="125" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D125"/>
     </row>
   </sheetData>
   <autoFilter ref="B1:B473" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
@@ -14828,15 +14908,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4508FCCF-4C5B-47D5-90D2-27C08BEB1B3C}">
-  <dimension ref="A1:L14"/>
+  <dimension ref="A1:S25"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="14" max="14" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="33" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>203</v>
       </c>
@@ -14864,8 +14948,23 @@
       <c r="K1">
         <v>101</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N1" t="s">
+        <v>664</v>
+      </c>
+      <c r="O1" t="s">
+        <v>665</v>
+      </c>
+      <c r="P1" t="s">
+        <v>666</v>
+      </c>
+      <c r="R1" t="s">
+        <v>667</v>
+      </c>
+      <c r="S1" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>204</v>
       </c>
@@ -14893,8 +14992,24 @@
       <c r="K2">
         <v>164</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N2" t="s">
+        <v>671</v>
+      </c>
+      <c r="O2" t="s">
+        <v>668</v>
+      </c>
+      <c r="P2">
+        <v>49</v>
+      </c>
+      <c r="R2" t="str">
+        <f>N2 &amp; " --&gt; " &amp;O2</f>
+        <v>MUST - Kriterium --&gt; Passed</v>
+      </c>
+      <c r="S2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>654</v>
       </c>
@@ -14916,8 +15031,24 @@
       <c r="G3">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N3" t="s">
+        <v>672</v>
+      </c>
+      <c r="O3" t="s">
+        <v>668</v>
+      </c>
+      <c r="P3">
+        <v>13</v>
+      </c>
+      <c r="R3" t="str">
+        <f>N3 &amp; " --&gt; " &amp;O3</f>
+        <v>SHOULD  - Kriterium --&gt; Passed</v>
+      </c>
+      <c r="S3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>192</v>
       </c>
@@ -14927,8 +15058,96 @@
       <c r="G4">
         <v>109</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N4" t="s">
+        <v>671</v>
+      </c>
+      <c r="O4" t="s">
+        <v>669</v>
+      </c>
+      <c r="P4">
+        <v>12</v>
+      </c>
+      <c r="R4" t="str">
+        <f>N4 &amp; " --&gt; " &amp;O4</f>
+        <v>MUST - Kriterium --&gt; Failed</v>
+      </c>
+      <c r="S4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N5" t="s">
+        <v>672</v>
+      </c>
+      <c r="O5" t="s">
+        <v>669</v>
+      </c>
+      <c r="P5">
+        <v>8</v>
+      </c>
+      <c r="R5" t="str">
+        <f>N5 &amp; " --&gt; " &amp;O5</f>
+        <v>SHOULD  - Kriterium --&gt; Failed</v>
+      </c>
+      <c r="S5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N6" t="s">
+        <v>673</v>
+      </c>
+      <c r="O6" t="s">
+        <v>668</v>
+      </c>
+      <c r="P6">
+        <v>7</v>
+      </c>
+      <c r="R6" t="str">
+        <f>N6 &amp; " --&gt; " &amp;O6</f>
+        <v>MUST NOT - Kriterium --&gt; Passed</v>
+      </c>
+      <c r="S6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N7" t="s">
+        <v>671</v>
+      </c>
+      <c r="O7" t="s">
+        <v>205</v>
+      </c>
+      <c r="P7">
+        <v>4</v>
+      </c>
+      <c r="R7" t="str">
+        <f>N7 &amp; " --&gt; " &amp;O7</f>
+        <v>MUST - Kriterium --&gt; Inc.</v>
+      </c>
+      <c r="S7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N8" t="s">
+        <v>673</v>
+      </c>
+      <c r="O8" t="s">
+        <v>669</v>
+      </c>
+      <c r="P8">
+        <v>1</v>
+      </c>
+      <c r="R8" t="str">
+        <f>N8 &amp; " --&gt; " &amp;O8</f>
+        <v>MUST NOT - Kriterium --&gt; Failed</v>
+      </c>
+      <c r="S8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K9" t="s">
         <v>659</v>
       </c>
@@ -14936,49 +15155,347 @@
         <f>101-32</f>
         <v>69</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N9" t="s">
+        <v>673</v>
+      </c>
+      <c r="O9" t="s">
+        <v>205</v>
+      </c>
+      <c r="P9">
+        <v>1</v>
+      </c>
+      <c r="R9" t="str">
+        <f>N9 &amp; " --&gt; " &amp;O9</f>
+        <v>MUST NOT - Kriterium --&gt; Inc.</v>
+      </c>
+      <c r="S9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K10" t="s">
         <v>660</v>
       </c>
       <c r="L10">
         <v>32</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N10" t="s">
+        <v>670</v>
+      </c>
+      <c r="O10" t="s">
+        <v>668</v>
+      </c>
+      <c r="P10">
+        <v>1</v>
+      </c>
+      <c r="R10" t="str">
+        <f>N10 &amp; " --&gt; " &amp;O10</f>
+        <v>MAY - Kriterium --&gt; Passed</v>
+      </c>
+      <c r="S10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>658</v>
       </c>
       <c r="B11">
         <v>78</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N11" t="s">
+        <v>670</v>
+      </c>
+      <c r="O11" t="s">
+        <v>669</v>
+      </c>
+      <c r="P11">
+        <v>1</v>
+      </c>
+      <c r="R11" t="str">
+        <f>N11 &amp; " --&gt; " &amp;O11</f>
+        <v>MAY - Kriterium --&gt; Failed</v>
+      </c>
+      <c r="S11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>657</v>
       </c>
       <c r="B12">
         <v>24</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N12" t="s">
+        <v>674</v>
+      </c>
+      <c r="O12" t="s">
+        <v>668</v>
+      </c>
+      <c r="P12">
+        <v>1</v>
+      </c>
+      <c r="R12" t="str">
+        <f>N12 &amp; " --&gt; " &amp;O12</f>
+        <v>MUST - Kriterium / MAY --&gt; Passed</v>
+      </c>
+      <c r="S12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>656</v>
       </c>
       <c r="B13">
         <v>7</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N13" t="s">
+        <v>674</v>
+      </c>
+      <c r="O13" t="s">
+        <v>205</v>
+      </c>
+      <c r="P13">
+        <v>1</v>
+      </c>
+      <c r="R13" t="str">
+        <f>N13 &amp; " --&gt; " &amp;O13</f>
+        <v>MUST - Kriterium / MAY --&gt; Inc.</v>
+      </c>
+      <c r="S13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>192</v>
       </c>
       <c r="B14">
         <v>32</v>
+      </c>
+      <c r="N14" t="s">
+        <v>675</v>
+      </c>
+      <c r="O14" t="s">
+        <v>669</v>
+      </c>
+      <c r="P14">
+        <v>1</v>
+      </c>
+      <c r="R14" t="str">
+        <f>N14 &amp; " --&gt; " &amp;O14</f>
+        <v>RECOMMENDED  -  Kriterium --&gt; Failed</v>
+      </c>
+      <c r="S14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N15" t="s">
+        <v>672</v>
+      </c>
+      <c r="O15" t="s">
+        <v>205</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="R15" t="str">
+        <f>N15 &amp; " --&gt; " &amp;O15</f>
+        <v>SHOULD  - Kriterium --&gt; Inc.</v>
+      </c>
+      <c r="S15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N16" t="s">
+        <v>676</v>
+      </c>
+      <c r="O16" t="s">
+        <v>668</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="R16" t="str">
+        <f>N16 &amp; " --&gt; " &amp;O16</f>
+        <v>SHOULD NOT  -  Kriterium --&gt; Passed</v>
+      </c>
+      <c r="S16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="14:19" x14ac:dyDescent="0.25">
+      <c r="N17" t="s">
+        <v>676</v>
+      </c>
+      <c r="O17" t="s">
+        <v>669</v>
+      </c>
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="R17" t="str">
+        <f>N17 &amp; " --&gt; " &amp;O17</f>
+        <v>SHOULD NOT  -  Kriterium --&gt; Failed</v>
+      </c>
+      <c r="S17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="14:19" x14ac:dyDescent="0.25">
+      <c r="N18" t="s">
+        <v>676</v>
+      </c>
+      <c r="O18" t="s">
+        <v>205</v>
+      </c>
+      <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="R18" t="str">
+        <f>N18 &amp; " --&gt; " &amp;O18</f>
+        <v>SHOULD NOT  -  Kriterium --&gt; Inc.</v>
+      </c>
+      <c r="S18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="14:19" x14ac:dyDescent="0.25">
+      <c r="N19" t="s">
+        <v>670</v>
+      </c>
+      <c r="O19" t="s">
+        <v>205</v>
+      </c>
+      <c r="P19">
+        <v>0</v>
+      </c>
+      <c r="R19" t="str">
+        <f>N19 &amp; " --&gt; " &amp;O19</f>
+        <v>MAY - Kriterium --&gt; Inc.</v>
+      </c>
+      <c r="S19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="14:19" x14ac:dyDescent="0.25">
+      <c r="N20" t="s">
+        <v>677</v>
+      </c>
+      <c r="O20" t="s">
+        <v>668</v>
+      </c>
+      <c r="P20">
+        <v>0</v>
+      </c>
+      <c r="R20" t="str">
+        <f>N20 &amp; " --&gt; " &amp;O20</f>
+        <v>MUST - Kriterium / Should --&gt; Passed</v>
+      </c>
+      <c r="S20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="14:19" x14ac:dyDescent="0.25">
+      <c r="N21" t="s">
+        <v>677</v>
+      </c>
+      <c r="O21" t="s">
+        <v>669</v>
+      </c>
+      <c r="P21">
+        <v>0</v>
+      </c>
+      <c r="R21" t="str">
+        <f>N21 &amp; " --&gt; " &amp;O21</f>
+        <v>MUST - Kriterium / Should --&gt; Failed</v>
+      </c>
+      <c r="S21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="14:19" x14ac:dyDescent="0.25">
+      <c r="N22" t="s">
+        <v>677</v>
+      </c>
+      <c r="O22" t="s">
+        <v>205</v>
+      </c>
+      <c r="P22">
+        <v>0</v>
+      </c>
+      <c r="R22" t="str">
+        <f>N22 &amp; " --&gt; " &amp;O22</f>
+        <v>MUST - Kriterium / Should --&gt; Inc.</v>
+      </c>
+      <c r="S22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="14:19" x14ac:dyDescent="0.25">
+      <c r="N23" t="s">
+        <v>674</v>
+      </c>
+      <c r="O23" t="s">
+        <v>669</v>
+      </c>
+      <c r="P23">
+        <v>0</v>
+      </c>
+      <c r="R23" t="str">
+        <f>N23 &amp; " --&gt; " &amp;O23</f>
+        <v>MUST - Kriterium / MAY --&gt; Failed</v>
+      </c>
+      <c r="S23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="14:19" x14ac:dyDescent="0.25">
+      <c r="N24" t="s">
+        <v>675</v>
+      </c>
+      <c r="O24" t="s">
+        <v>668</v>
+      </c>
+      <c r="P24">
+        <v>0</v>
+      </c>
+      <c r="R24" t="str">
+        <f>N24 &amp; " --&gt; " &amp;O24</f>
+        <v>RECOMMENDED  -  Kriterium --&gt; Passed</v>
+      </c>
+      <c r="S24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="14:19" x14ac:dyDescent="0.25">
+      <c r="N25" t="s">
+        <v>675</v>
+      </c>
+      <c r="O25" t="s">
+        <v>205</v>
+      </c>
+      <c r="P25">
+        <v>0</v>
+      </c>
+      <c r="R25" t="str">
+        <f>N25 &amp; " --&gt; " &amp;O25</f>
+        <v>RECOMMENDED  -  Kriterium --&gt; Inc.</v>
+      </c>
+      <c r="S25">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <tableParts count="2">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>